<commit_message>
[add] added calculated features file
</commit_message>
<xml_diff>
--- a/Experiment-Data/Answer-Data.xlsx
+++ b/Experiment-Data/Answer-Data.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC_User\iCloudDrive\Documents\01_University\02_Research\Working-Directory\eye-tracking-software\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\www\Desktop\eye-tracking-software\Experiment-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3248773E-4072-4592-86B1-CF84B09D554D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC98698-AA4D-4844-8AC7-8D4142365F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{65F65776-174E-4145-8CCF-AA6B8A50F68A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{65F65776-174E-4145-8CCF-AA6B8A50F68A}"/>
   </bookViews>
   <sheets>
     <sheet name="1st" sheetId="1" r:id="rId1"/>
+    <sheet name="1st-English" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="27">
   <si>
     <t>English</t>
   </si>
@@ -117,6 +118,39 @@
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
+  <si>
+    <t xml:space="preserve">注視時間(ms) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">平均注視x座標 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 平均注視y座標</t>
+  </si>
+  <si>
+    <t xml:space="preserve">平均サッケード振幅(px) </t>
+  </si>
+  <si>
+    <t>最大サッケード振幅(px)</t>
+  </si>
+  <si>
+    <t>サッケード数</t>
+  </si>
+  <si>
+    <t>平均速度</t>
+  </si>
+  <si>
+    <t>速度の標準偏差</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 視覚的探索距離(px)</t>
+  </si>
+  <si>
+    <t>視覚的探索の均一性</t>
+  </si>
+  <si>
+    <t>平均視線回転(rad)</t>
+  </si>
 </sst>
 </file>
 
@@ -126,7 +160,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -138,7 +172,7 @@
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Aptos Narrow"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -171,7 +205,7 @@
       <charset val="128"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -227,9 +261,6 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -242,14 +273,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -587,21 +621,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C853D4-11AD-448C-900A-323815755F36}">
   <dimension ref="A1:AM37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB9" sqref="AB9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z21" sqref="Z21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" style="3" customWidth="1"/>
-    <col min="2" max="3" width="4.125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="6.25" style="14" customWidth="1"/>
-    <col min="5" max="24" width="4.375" style="2" customWidth="1"/>
-    <col min="25" max="25" width="4.125" style="3" customWidth="1"/>
+    <col min="2" max="3" width="4.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" style="13" customWidth="1"/>
+    <col min="5" max="24" width="4.42578125" style="2" customWidth="1"/>
+    <col min="25" max="25" width="4.140625" style="3" customWidth="1"/>
     <col min="26" max="26" width="10" style="3" customWidth="1"/>
-    <col min="27" max="28" width="4.125" style="3" customWidth="1"/>
-    <col min="29" max="29" width="6.125" style="3" customWidth="1"/>
-    <col min="30" max="39" width="4.375" style="4" customWidth="1"/>
+    <col min="27" max="28" width="4.140625" style="3" customWidth="1"/>
+    <col min="29" max="29" width="6.140625" style="3" customWidth="1"/>
+    <col min="30" max="39" width="4.42578125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -617,28 +651,28 @@
       <c r="D1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
       <c r="Y1" s="5"/>
       <c r="Z1" s="5" t="s">
         <v>10</v>
@@ -649,27 +683,27 @@
       <c r="AB1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AC1" s="15" t="s">
+      <c r="AC1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="18" t="s">
+      <c r="AD1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
-      <c r="AG1" s="18"/>
-      <c r="AH1" s="18"/>
-      <c r="AI1" s="18"/>
-      <c r="AJ1" s="18"/>
-      <c r="AK1" s="18"/>
-      <c r="AL1" s="18"/>
-      <c r="AM1" s="18"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="16"/>
+      <c r="AJ1" s="16"/>
+      <c r="AK1" s="16"/>
+      <c r="AL1" s="16"/>
+      <c r="AM1" s="16"/>
     </row>
     <row r="2" spans="1:39" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="12"/>
+      <c r="D2" s="11"/>
       <c r="E2" s="6">
         <v>1</v>
       </c>
@@ -766,7 +800,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -776,7 +810,7 @@
       <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="12">
         <f>COUNTIF(E3:X3,"○")/20</f>
         <v>0.5</v>
       </c>
@@ -849,7 +883,7 @@
       <c r="AB3" s="3">
         <v>1</v>
       </c>
-      <c r="AC3" s="13">
+      <c r="AC3" s="12">
         <f>(COUNTIF(AD3:AM3,"○")/10)</f>
         <v>0.9</v>
       </c>
@@ -884,11 +918,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C4" s="3">
         <v>2</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="12">
         <f t="shared" ref="D4:D30" si="0">COUNTIF(E4:X4,"○")/20</f>
         <v>0.35</v>
       </c>
@@ -955,7 +989,7 @@
       <c r="AB4" s="3">
         <v>2</v>
       </c>
-      <c r="AC4" s="13">
+      <c r="AC4" s="12">
         <f t="shared" ref="AC4:AC36" si="1">(COUNTIF(AD4:AM4,"○")/10)</f>
         <v>0.7</v>
       </c>
@@ -990,89 +1024,89 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.4">
-      <c r="D5" s="13"/>
-      <c r="E5" s="11">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="D5" s="12"/>
+      <c r="E5" s="18">
         <f>(COUNTIF(E3:E4,"○"))/2</f>
         <v>0</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="18">
         <f t="shared" ref="F5:X5" si="2">(COUNTIF(F3:F4,"○"))/2</f>
         <v>0.5</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="18">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="18">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="18">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="18">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="18">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="18">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="M5" s="11">
+      <c r="M5" s="18">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="N5" s="11">
+      <c r="N5" s="18">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="O5" s="11">
+      <c r="O5" s="18">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="P5" s="11">
+      <c r="P5" s="18">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q5" s="11">
+      <c r="Q5" s="18">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="R5" s="11">
+      <c r="R5" s="18">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S5" s="11">
+      <c r="S5" s="18">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="T5" s="11">
+      <c r="T5" s="18">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="U5" s="11">
+      <c r="U5" s="18">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="V5" s="11">
+      <c r="V5" s="18">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="W5" s="11">
+      <c r="W5" s="18">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X5" s="11">
+      <c r="X5" s="18">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="AC5" s="13"/>
+      <c r="AC5" s="12"/>
       <c r="AD5" s="10"/>
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
@@ -1084,14 +1118,14 @@
       <c r="AL5" s="1"/>
       <c r="AM5" s="1"/>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1161,7 +1195,7 @@
       <c r="AB6" s="3">
         <v>1</v>
       </c>
-      <c r="AC6" s="13">
+      <c r="AC6" s="12">
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
@@ -1196,11 +1230,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C7" s="3">
         <v>2</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="12">
         <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
@@ -1267,7 +1301,7 @@
       <c r="AB7" s="3">
         <v>2</v>
       </c>
-      <c r="AC7" s="13">
+      <c r="AC7" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
@@ -1302,11 +1336,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C8" s="3">
         <v>3</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="12">
         <f t="shared" si="0"/>
         <v>0.95</v>
       </c>
@@ -1373,7 +1407,7 @@
       <c r="AB8" s="3">
         <v>3</v>
       </c>
-      <c r="AC8" s="13">
+      <c r="AC8" s="12">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
@@ -1408,11 +1442,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C9" s="3">
         <v>4</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="12">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
@@ -1479,7 +1513,7 @@
       <c r="AB9" s="3">
         <v>4</v>
       </c>
-      <c r="AC9" s="13">
+      <c r="AC9" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
@@ -1514,11 +1548,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C10" s="3">
         <v>5</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="12">
         <f t="shared" si="0"/>
         <v>0.55000000000000004</v>
       </c>
@@ -1585,7 +1619,7 @@
       <c r="AB10" s="3">
         <v>5</v>
       </c>
-      <c r="AC10" s="13">
+      <c r="AC10" s="12">
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
@@ -1620,11 +1654,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C11" s="3">
         <v>6</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="12">
         <f t="shared" si="0"/>
         <v>0.85</v>
       </c>
@@ -1691,7 +1725,7 @@
       <c r="AB11" s="3">
         <v>6</v>
       </c>
-      <c r="AC11" s="13">
+      <c r="AC11" s="12">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
@@ -1726,11 +1760,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C12" s="3">
         <v>7</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="12">
         <f t="shared" si="0"/>
         <v>0.55000000000000004</v>
       </c>
@@ -1797,7 +1831,7 @@
       <c r="AB12" s="3">
         <v>7</v>
       </c>
-      <c r="AC12" s="13">
+      <c r="AC12" s="12">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
@@ -1832,11 +1866,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C13" s="3">
         <v>8</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="12">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
@@ -1903,7 +1937,7 @@
       <c r="AB13" s="3">
         <v>8</v>
       </c>
-      <c r="AC13" s="13">
+      <c r="AC13" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
@@ -1938,11 +1972,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C14" s="3">
         <v>9</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="12">
         <f t="shared" si="0"/>
         <v>0.65</v>
       </c>
@@ -2009,7 +2043,7 @@
       <c r="AB14" s="3">
         <v>9</v>
       </c>
-      <c r="AC14" s="13">
+      <c r="AC14" s="12">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
@@ -2044,11 +2078,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C15" s="3">
         <v>10</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="12">
         <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
@@ -2115,7 +2149,7 @@
       <c r="AB15" s="3">
         <v>10</v>
       </c>
-      <c r="AC15" s="13">
+      <c r="AC15" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
@@ -2150,89 +2184,89 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.4">
-      <c r="D16" s="13"/>
-      <c r="E16" s="11">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="D16" s="12"/>
+      <c r="E16" s="18">
         <f>(COUNTIF(E6:E15,"○"))/10</f>
         <v>0.6</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="18">
         <f t="shared" ref="F16:X16" si="3">(COUNTIF(F6:F15,"○"))/10</f>
         <v>0.4</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="18">
         <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="18">
         <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="18">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="J16" s="11">
+      <c r="J16" s="18">
         <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
-      <c r="K16" s="11">
+      <c r="K16" s="18">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="L16" s="11">
+      <c r="L16" s="18">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M16" s="11">
+      <c r="M16" s="18">
         <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
-      <c r="N16" s="11">
+      <c r="N16" s="18">
         <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
-      <c r="O16" s="11">
+      <c r="O16" s="18">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P16" s="11">
+      <c r="P16" s="18">
         <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
-      <c r="Q16" s="11">
+      <c r="Q16" s="18">
         <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
-      <c r="R16" s="11">
+      <c r="R16" s="18">
         <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
-      <c r="S16" s="11">
+      <c r="S16" s="18">
         <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
-      <c r="T16" s="11">
+      <c r="T16" s="18">
         <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
-      <c r="U16" s="11">
+      <c r="U16" s="18">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="V16" s="11">
+      <c r="V16" s="18">
         <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
-      <c r="W16" s="11">
+      <c r="W16" s="18">
         <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
-      <c r="X16" s="11">
+      <c r="X16" s="18">
         <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
-      <c r="AC16" s="13"/>
+      <c r="AC16" s="12"/>
       <c r="AD16" s="10"/>
       <c r="AE16" s="1"/>
       <c r="AF16" s="1"/>
@@ -2244,14 +2278,14 @@
       <c r="AL16" s="1"/>
       <c r="AM16" s="1"/>
     </row>
-    <row r="17" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="12">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
@@ -2321,7 +2355,7 @@
       <c r="AB17" s="3">
         <v>1</v>
       </c>
-      <c r="AC17" s="13">
+      <c r="AC17" s="12">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
@@ -2356,11 +2390,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C18" s="3">
         <v>2</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="12">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
@@ -2427,7 +2461,7 @@
       <c r="AB18" s="3">
         <v>2</v>
       </c>
-      <c r="AC18" s="13">
+      <c r="AC18" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -2462,11 +2496,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C19" s="3">
         <v>3</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="12">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
@@ -2533,7 +2567,7 @@
       <c r="AB19" s="3">
         <v>3</v>
       </c>
-      <c r="AC19" s="13">
+      <c r="AC19" s="12">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
@@ -2568,11 +2602,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C20" s="3">
         <v>4</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="12">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
@@ -2639,7 +2673,7 @@
       <c r="AB20" s="3">
         <v>4</v>
       </c>
-      <c r="AC20" s="13">
+      <c r="AC20" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
@@ -2674,11 +2708,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C21" s="3">
         <v>5</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="12">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
@@ -2745,7 +2779,7 @@
       <c r="AB21" s="3">
         <v>5</v>
       </c>
-      <c r="AC21" s="13">
+      <c r="AC21" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
@@ -2780,11 +2814,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C22" s="3">
         <v>6</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="12">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
@@ -2851,7 +2885,7 @@
       <c r="AB22" s="3">
         <v>6</v>
       </c>
-      <c r="AC22" s="13">
+      <c r="AC22" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
@@ -2886,11 +2920,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C23" s="3">
         <v>7</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="12">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
@@ -2957,7 +2991,7 @@
       <c r="AB23" s="3">
         <v>7</v>
       </c>
-      <c r="AC23" s="13">
+      <c r="AC23" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -2992,11 +3026,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C24" s="3">
         <v>8</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="12">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
@@ -3063,7 +3097,7 @@
       <c r="AB24" s="3">
         <v>8</v>
       </c>
-      <c r="AC24" s="13">
+      <c r="AC24" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -3098,11 +3132,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C25" s="3">
         <v>9</v>
       </c>
-      <c r="D25" s="13">
+      <c r="D25" s="12">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
@@ -3169,7 +3203,7 @@
       <c r="AB25" s="3">
         <v>9</v>
       </c>
-      <c r="AC25" s="13">
+      <c r="AC25" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
@@ -3204,11 +3238,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C26" s="3">
         <v>10</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="12">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
@@ -3275,7 +3309,7 @@
       <c r="AB26" s="3">
         <v>10</v>
       </c>
-      <c r="AC26" s="13">
+      <c r="AC26" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
@@ -3310,11 +3344,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C27" s="3">
         <v>11</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D27" s="12">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
@@ -3381,7 +3415,7 @@
       <c r="AB27" s="3">
         <v>11</v>
       </c>
-      <c r="AC27" s="13">
+      <c r="AC27" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -3416,11 +3450,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C28" s="3">
         <v>12</v>
       </c>
-      <c r="D28" s="13">
+      <c r="D28" s="12">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
@@ -3487,7 +3521,7 @@
       <c r="AB28" s="3">
         <v>12</v>
       </c>
-      <c r="AC28" s="13">
+      <c r="AC28" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -3522,11 +3556,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C29" s="3">
         <v>13</v>
       </c>
-      <c r="D29" s="13">
+      <c r="D29" s="12">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
@@ -3593,7 +3627,7 @@
       <c r="AB29" s="3">
         <v>13</v>
       </c>
-      <c r="AC29" s="13">
+      <c r="AC29" s="12">
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
@@ -3628,11 +3662,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C30" s="3">
         <v>14</v>
       </c>
-      <c r="D30" s="13">
+      <c r="D30" s="12">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
@@ -3699,7 +3733,7 @@
       <c r="AB30" s="3">
         <v>14</v>
       </c>
-      <c r="AC30" s="13">
+      <c r="AC30" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
@@ -3734,85 +3768,85 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="D31" s="5"/>
-      <c r="E31" s="16">
+      <c r="E31" s="17">
         <f>(COUNTIF(E17:E30,"○"))/14</f>
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="F31" s="16">
+      <c r="F31" s="17">
         <f t="shared" ref="F31:X31" si="4">(COUNTIF(F17:F30,"○"))/14</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="G31" s="16">
+      <c r="G31" s="17">
         <f t="shared" si="4"/>
         <v>0.42857142857142855</v>
       </c>
-      <c r="H31" s="16">
+      <c r="H31" s="17">
         <f t="shared" si="4"/>
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="I31" s="16">
+      <c r="I31" s="17">
         <f t="shared" si="4"/>
         <v>0.35714285714285715</v>
       </c>
-      <c r="J31" s="16">
+      <c r="J31" s="17">
         <f t="shared" si="4"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="K31" s="16">
+      <c r="K31" s="17">
         <f t="shared" si="4"/>
         <v>0.35714285714285715</v>
       </c>
-      <c r="L31" s="16">
+      <c r="L31" s="17">
         <f t="shared" si="4"/>
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="M31" s="16">
+      <c r="M31" s="17">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N31" s="16">
+      <c r="N31" s="17">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O31" s="16">
+      <c r="O31" s="17">
         <f t="shared" si="4"/>
         <v>0.2857142857142857</v>
       </c>
-      <c r="P31" s="16">
+      <c r="P31" s="17">
         <f>(COUNTIF(P17:P30,"○"))/14</f>
         <v>0</v>
       </c>
-      <c r="Q31" s="16">
+      <c r="Q31" s="17">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="R31" s="16">
+      <c r="R31" s="17">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="S31" s="16">
+      <c r="S31" s="17">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T31" s="16">
+      <c r="T31" s="17">
         <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
-      <c r="U31" s="16">
+      <c r="U31" s="17">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V31" s="16">
+      <c r="V31" s="17">
         <f t="shared" si="4"/>
         <v>0.35714285714285715</v>
       </c>
-      <c r="W31" s="16">
+      <c r="W31" s="17">
         <f t="shared" si="4"/>
         <v>0.7857142857142857</v>
       </c>
-      <c r="X31" s="16">
+      <c r="X31" s="17">
         <f t="shared" si="4"/>
         <v>7.1428571428571425E-2</v>
       </c>
@@ -3822,7 +3856,7 @@
       <c r="AB31" s="3">
         <v>1</v>
       </c>
-      <c r="AC31" s="13">
+      <c r="AC31" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
@@ -3857,11 +3891,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="AB32" s="3">
         <v>2</v>
       </c>
-      <c r="AC32" s="13">
+      <c r="AC32" s="12">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
@@ -3896,14 +3930,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="27:39" x14ac:dyDescent="0.4">
+    <row r="33" spans="27:39" x14ac:dyDescent="0.25">
       <c r="AA33" s="3" t="s">
         <v>7</v>
       </c>
       <c r="AB33" s="3">
         <v>1</v>
       </c>
-      <c r="AC33" s="13">
+      <c r="AC33" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -3938,11 +3972,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="27:39" x14ac:dyDescent="0.4">
+    <row r="34" spans="27:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="AB34" s="3">
         <v>2</v>
       </c>
-      <c r="AC34" s="13">
+      <c r="AC34" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
@@ -3977,11 +4011,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="27:39" x14ac:dyDescent="0.4">
+    <row r="35" spans="27:39" ht="16.5" x14ac:dyDescent="0.3">
       <c r="AB35" s="3">
         <v>3</v>
       </c>
-      <c r="AC35" s="13">
+      <c r="AC35" s="12">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
@@ -4016,14 +4050,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="27:39" x14ac:dyDescent="0.4">
+    <row r="36" spans="27:39" x14ac:dyDescent="0.25">
       <c r="AA36" s="3" t="s">
         <v>6</v>
       </c>
       <c r="AB36" s="3">
         <v>1</v>
       </c>
-      <c r="AC36" s="13">
+      <c r="AC36" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -4058,44 +4092,44 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="27:39" x14ac:dyDescent="0.4">
-      <c r="AD37" s="16">
+    <row r="37" spans="27:39" x14ac:dyDescent="0.25">
+      <c r="AD37" s="17">
         <f>(COUNTIF(AD3:AD36,"○")/32)</f>
         <v>1</v>
       </c>
-      <c r="AE37" s="16">
+      <c r="AE37" s="17">
         <f t="shared" ref="AE37:AM37" si="5">(COUNTIF(AE3:AE36,"○")/32)</f>
         <v>0.9375</v>
       </c>
-      <c r="AF37" s="16">
+      <c r="AF37" s="17">
         <f t="shared" si="5"/>
         <v>0.9375</v>
       </c>
-      <c r="AG37" s="16">
+      <c r="AG37" s="17">
         <f t="shared" si="5"/>
         <v>0.96875</v>
       </c>
-      <c r="AH37" s="16">
+      <c r="AH37" s="17">
         <f t="shared" si="5"/>
         <v>0.59375</v>
       </c>
-      <c r="AI37" s="16">
+      <c r="AI37" s="17">
         <f t="shared" si="5"/>
         <v>0.875</v>
       </c>
-      <c r="AJ37" s="16">
+      <c r="AJ37" s="17">
         <f t="shared" si="5"/>
         <v>0.5625</v>
       </c>
-      <c r="AK37" s="16">
+      <c r="AK37" s="17">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="AL37" s="16">
+      <c r="AL37" s="17">
         <f t="shared" si="5"/>
         <v>0.875</v>
       </c>
-      <c r="AM37" s="16">
+      <c r="AM37" s="17">
         <f t="shared" si="5"/>
         <v>0.9375</v>
       </c>
@@ -4109,4 +4143,2028 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88CCFB4E-3D94-4A97-83BE-04827B31FA43}">
+  <dimension ref="A1:AH29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AI5" sqref="AI5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="5.7109375" customWidth="1"/>
+    <col min="4" max="23" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12">
+        <f>COUNTIF(D3:W3,"○")/20</f>
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="T3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="W3" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="12">
+        <f>COUNTIF(D4:W4,"○")/20</f>
+        <v>0.35</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="U4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="V4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="W4" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12">
+        <f>COUNTIF(D5:W5,"○")/20</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W5" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="12">
+        <f>COUNTIF(D6:W6,"○")/20</f>
+        <v>0.9</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="P6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="S6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W6" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3">
+        <v>3</v>
+      </c>
+      <c r="C7" s="12">
+        <f>COUNTIF(D7:W7,"○")/20</f>
+        <v>0.95</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W7" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3">
+        <v>4</v>
+      </c>
+      <c r="C8" s="12">
+        <f>COUNTIF(D8:W8,"○")/20</f>
+        <v>0.7</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="P8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="S8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="T8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="W8" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3">
+        <v>5</v>
+      </c>
+      <c r="C9" s="12">
+        <f>COUNTIF(D9:W9,"○")/20</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="P9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W9" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3">
+        <v>6</v>
+      </c>
+      <c r="C10" s="12">
+        <f>COUNTIF(D10:W10,"○")/20</f>
+        <v>0.85</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="P10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="S10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W10" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3">
+        <v>7</v>
+      </c>
+      <c r="C11" s="12">
+        <f>COUNTIF(D11:W11,"○")/20</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="V11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W11" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3">
+        <v>8</v>
+      </c>
+      <c r="C12" s="12">
+        <f>COUNTIF(D12:W12,"○")/20</f>
+        <v>0.75</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="S12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="T12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="W12" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3">
+        <v>9</v>
+      </c>
+      <c r="C13" s="12">
+        <f>COUNTIF(D13:W13,"○")/20</f>
+        <v>0.65</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="P13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="R13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="S13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="T13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="W13" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3">
+        <v>10</v>
+      </c>
+      <c r="C14" s="12">
+        <f>COUNTIF(D14:W14,"○")/20</f>
+        <v>0.9</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="P14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="S14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W14" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+      <c r="C15" s="12">
+        <f>COUNTIF(D15:W15,"○")/20</f>
+        <v>0.2</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="R15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="T15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="U15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="V15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W15" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3">
+        <v>2</v>
+      </c>
+      <c r="C16" s="12">
+        <f>COUNTIF(D16:W16,"○")/20</f>
+        <v>0.2</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="R16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="T16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="U16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W16" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3">
+        <v>3</v>
+      </c>
+      <c r="C17" s="12">
+        <f>COUNTIF(D17:W17,"○")/20</f>
+        <v>0.2</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="R17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="T17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="U17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W17" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3">
+        <v>4</v>
+      </c>
+      <c r="C18" s="12">
+        <f>COUNTIF(D18:W18,"○")/20</f>
+        <v>0.3</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="R18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="U18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="V18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W18" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3">
+        <v>5</v>
+      </c>
+      <c r="C19" s="12">
+        <f>COUNTIF(D19:W19,"○")/20</f>
+        <v>0.25</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="R19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="U19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="V19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W19" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3">
+        <v>6</v>
+      </c>
+      <c r="C20" s="12">
+        <f>COUNTIF(D20:W20,"○")/20</f>
+        <v>0.2</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="R20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="U20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W20" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3">
+        <v>7</v>
+      </c>
+      <c r="C21" s="12">
+        <f>COUNTIF(D21:W21,"○")/20</f>
+        <v>0.25</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="R21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="U21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W21" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3">
+        <v>8</v>
+      </c>
+      <c r="C22" s="12">
+        <f>COUNTIF(D22:W22,"○")/20</f>
+        <v>0.25</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="R22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="U22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="V22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W22" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3">
+        <v>9</v>
+      </c>
+      <c r="C23" s="12">
+        <f>COUNTIF(D23:W23,"○")/20</f>
+        <v>0.2</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="R23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="T23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="U23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="V23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="W23" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3">
+        <v>10</v>
+      </c>
+      <c r="C24" s="12">
+        <f>COUNTIF(D24:W24,"○")/20</f>
+        <v>0.1</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K24" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="R24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S24" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="U24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="V24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="W24" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3">
+        <v>11</v>
+      </c>
+      <c r="C25" s="12">
+        <f>COUNTIF(D25:W25,"○")/20</f>
+        <v>0.05</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="R25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="T25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="U25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="V25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="W25" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3">
+        <v>12</v>
+      </c>
+      <c r="C26" s="12">
+        <f>COUNTIF(D26:W26,"○")/20</f>
+        <v>0.15</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="R26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="T26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="U26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="V26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W26" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3">
+        <v>13</v>
+      </c>
+      <c r="C27" s="12">
+        <f>COUNTIF(D27:W27,"○")/20</f>
+        <v>0.1</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="R27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="U27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="V27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W27" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3">
+        <v>14</v>
+      </c>
+      <c r="C28" s="12">
+        <f>COUNTIF(D28:W28,"○")/20</f>
+        <v>0.1</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="R28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="T28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="U28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W28" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="17">
+        <f>(COUNTIF(D15:D28,"○"))/14</f>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="E29" s="17">
+        <f t="shared" ref="E29:W29" si="0">(COUNTIF(E15:E28,"○"))/14</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="F29" s="17">
+        <f t="shared" si="0"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="G29" s="17">
+        <f t="shared" si="0"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="H29" s="17">
+        <f t="shared" si="0"/>
+        <v>0.35714285714285715</v>
+      </c>
+      <c r="I29" s="17">
+        <f t="shared" si="0"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="J29" s="17">
+        <f t="shared" si="0"/>
+        <v>0.35714285714285715</v>
+      </c>
+      <c r="K29" s="17">
+        <f t="shared" si="0"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="L29" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="17">
+        <f t="shared" si="0"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="O29" s="17">
+        <f>(COUNTIF(O15:O28,"○"))/14</f>
+        <v>0</v>
+      </c>
+      <c r="P29" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R29" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S29" s="17">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="T29" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U29" s="17">
+        <f t="shared" si="0"/>
+        <v>0.35714285714285715</v>
+      </c>
+      <c r="V29" s="17">
+        <f t="shared" si="0"/>
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="W29" s="17">
+        <f t="shared" si="0"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:W1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[add] added updated cluster data
</commit_message>
<xml_diff>
--- a/Experiment-Data/Answer-Data.xlsx
+++ b/Experiment-Data/Answer-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\www\Desktop\eye-tracking-software\Experiment-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72AEB27-B230-4491-A721-666521AFF80A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A27A6608-FD1C-455B-85CE-6C48855A7FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{65F65776-174E-4145-8CCF-AA6B8A50F68A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="32">
   <si>
     <t>English</t>
   </si>
@@ -171,9 +171,6 @@
   <si>
     <t>クラスタ
 数</t>
-  </si>
-  <si>
-    <t>NaN</t>
   </si>
 </sst>
 </file>
@@ -650,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C853D4-11AD-448C-900A-323815755F36}">
-  <dimension ref="A1:AX39"/>
+  <dimension ref="A1:AW39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB38" sqref="AB38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,15 +661,15 @@
     <col min="7" max="26" width="4.42578125" style="2" customWidth="1"/>
     <col min="27" max="27" width="4.140625" style="3" customWidth="1"/>
     <col min="28" max="28" width="10" style="3" customWidth="1"/>
-    <col min="29" max="32" width="4.28515625" style="3" customWidth="1"/>
-    <col min="33" max="33" width="6.140625" style="3" customWidth="1"/>
-    <col min="34" max="43" width="4.42578125" style="4" customWidth="1"/>
-    <col min="45" max="45" width="10" style="3" customWidth="1"/>
-    <col min="46" max="49" width="4.28515625" style="3" customWidth="1"/>
-    <col min="50" max="50" width="6.140625" style="3" customWidth="1"/>
+    <col min="29" max="31" width="4.28515625" style="3" customWidth="1"/>
+    <col min="32" max="32" width="6.140625" style="3" customWidth="1"/>
+    <col min="33" max="42" width="4.42578125" style="4" customWidth="1"/>
+    <col min="44" max="44" width="10" style="3" customWidth="1"/>
+    <col min="45" max="48" width="4.28515625" style="3" customWidth="1"/>
+    <col min="49" max="49" width="6.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:49" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -724,17 +721,15 @@
         <v>8</v>
       </c>
       <c r="AE1" s="5">
-        <v>2</v>
-      </c>
-      <c r="AF1" s="5">
-        <v>4</v>
-      </c>
-      <c r="AG1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="AH1" s="20" t="s">
+      <c r="AG1" s="20" t="s">
         <v>15</v>
       </c>
+      <c r="AH1" s="20"/>
       <c r="AI1" s="20"/>
       <c r="AJ1" s="20"/>
       <c r="AK1" s="20"/>
@@ -743,27 +738,26 @@
       <c r="AN1" s="20"/>
       <c r="AO1" s="20"/>
       <c r="AP1" s="20"/>
-      <c r="AQ1" s="20"/>
+      <c r="AR1" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="AS1" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AT1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AU1" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="AU1" s="5">
+        <v>2</v>
+      </c>
       <c r="AV1" s="5">
-        <v>2</v>
-      </c>
-      <c r="AW1" s="5">
         <v>4</v>
       </c>
-      <c r="AX1" s="14" t="s">
+      <c r="AW1" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:50" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:49" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -836,45 +830,44 @@
       <c r="AD2" s="5"/>
       <c r="AE2" s="5"/>
       <c r="AF2" s="5"/>
-      <c r="AG2" s="5"/>
+      <c r="AG2" s="7">
+        <v>1</v>
+      </c>
       <c r="AH2" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI2" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AJ2" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AK2" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AL2" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AM2" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AN2" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AO2" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AP2" s="7">
-        <v>9</v>
-      </c>
-      <c r="AQ2" s="7">
         <v>10</v>
       </c>
+      <c r="AR2" s="5"/>
       <c r="AS2" s="5"/>
       <c r="AT2" s="5"/>
       <c r="AU2" s="5"/>
       <c r="AV2" s="5"/>
       <c r="AW2" s="5"/>
-      <c r="AX2" s="5"/>
-    </row>
-    <row r="3" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -963,16 +956,16 @@
       <c r="AD3" s="3">
         <v>1</v>
       </c>
-      <c r="AE3" s="3">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="3">
-        <v>1</v>
-      </c>
-      <c r="AG3" s="12">
-        <f>(COUNTIF(AH3:AQ3,"○")/10)</f>
+      <c r="AE3">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="12">
+        <f>(COUNTIF(AG3:AP3,"○")/10)</f>
         <v>0.9</v>
       </c>
+      <c r="AG3" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH3" s="10" t="s">
         <v>12</v>
       </c>
@@ -988,11 +981,11 @@
       <c r="AL3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN3" s="9" t="s">
-        <v>11</v>
+      <c r="AM3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN3" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AO3" s="10" t="s">
         <v>12</v>
@@ -1000,30 +993,27 @@
       <c r="AP3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ3" s="10" t="s">
-        <v>12</v>
+      <c r="AR3" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="AS3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AT3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AU3" s="3">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="AT3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AU3">
+        <v>2</v>
       </c>
       <c r="AV3">
-        <v>2</v>
-      </c>
-      <c r="AW3">
         <v>3</v>
       </c>
-      <c r="AX3" s="12">
-        <f>(F3+AG3)/2</f>
+      <c r="AW3" s="12">
+        <f>(F3+AF3)/2</f>
         <v>0.7</v>
       </c>
     </row>
-    <row r="4" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C4" s="3">
         <v>2</v>
       </c>
@@ -1100,16 +1090,16 @@
       <c r="AD4" s="3">
         <v>2</v>
       </c>
-      <c r="AE4" s="3">
-        <v>2</v>
-      </c>
-      <c r="AF4" s="3">
-        <v>2</v>
-      </c>
-      <c r="AG4" s="12">
-        <f t="shared" ref="AG4:AG36" si="1">(COUNTIF(AH4:AQ4,"○")/10)</f>
+      <c r="AE4">
+        <v>2</v>
+      </c>
+      <c r="AF4" s="12">
+        <f t="shared" ref="AF4:AF36" si="1">(COUNTIF(AG4:AP4,"○")/10)</f>
         <v>0.7</v>
       </c>
+      <c r="AG4" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH4" s="10" t="s">
         <v>12</v>
       </c>
@@ -1122,122 +1112,120 @@
       <c r="AK4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AL4" s="10" t="s">
-        <v>12</v>
+      <c r="AL4" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AM4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AN4" s="9" t="s">
-        <v>11</v>
+      <c r="AN4" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AO4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AP4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AQ4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AU4" s="3">
+      <c r="AP4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AT4" s="3">
+        <v>2</v>
+      </c>
+      <c r="AU4">
         <v>2</v>
       </c>
       <c r="AV4">
-        <v>2</v>
-      </c>
-      <c r="AW4">
         <v>4</v>
       </c>
-      <c r="AX4" s="12">
-        <f t="shared" ref="AX4:AX30" si="2">(F4+AG4)/2</f>
+      <c r="AW4" s="12">
+        <f>(F4+AF4)/2</f>
         <v>0.52499999999999991</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="F5" s="12"/>
       <c r="G5" s="16">
         <f>(COUNTIF(G3:G4,"○"))/2</f>
         <v>0</v>
       </c>
       <c r="H5" s="16">
-        <f t="shared" ref="H5:Z5" si="3">(COUNTIF(H3:H4,"○"))/2</f>
+        <f t="shared" ref="H5:Z5" si="2">(COUNTIF(H3:H4,"○"))/2</f>
         <v>0.5</v>
       </c>
       <c r="I5" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="J5" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="K5" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="L5" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="M5" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N5" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="O5" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="P5" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="Q5" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="R5" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S5" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="T5" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U5" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="V5" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="W5" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="X5" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="Y5" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z5" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="AG5" s="12"/>
-      <c r="AH5" s="10"/>
+      <c r="AF5" s="12"/>
+      <c r="AG5" s="10"/>
+      <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
@@ -1246,10 +1234,9 @@
       <c r="AN5" s="1"/>
       <c r="AO5" s="1"/>
       <c r="AP5" s="1"/>
-      <c r="AQ5" s="1"/>
-      <c r="AX5" s="12"/>
-    </row>
-    <row r="6" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="AW5" s="12"/>
+    </row>
+    <row r="6" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1332,16 +1319,16 @@
       <c r="AD6" s="3">
         <v>1</v>
       </c>
-      <c r="AE6" s="3">
-        <v>2</v>
-      </c>
-      <c r="AF6" s="3">
-        <v>2</v>
-      </c>
-      <c r="AG6" s="12">
+      <c r="AE6">
+        <v>2</v>
+      </c>
+      <c r="AF6" s="12">
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
+      <c r="AG6" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH6" s="10" t="s">
         <v>12</v>
       </c>
@@ -1354,42 +1341,39 @@
       <c r="AK6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AL6" s="10" t="s">
-        <v>12</v>
+      <c r="AL6" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AM6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AN6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AO6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AQ6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AT6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AU6" s="3">
-        <v>1</v>
+      <c r="AN6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AP6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AS6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT6" s="3">
+        <v>1</v>
+      </c>
+      <c r="AU6">
+        <v>2</v>
       </c>
       <c r="AV6">
-        <v>2</v>
-      </c>
-      <c r="AW6">
         <v>3</v>
       </c>
-      <c r="AX6" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW6" s="12">
+        <f>(F6+AF6)/2</f>
         <v>0.85</v>
       </c>
     </row>
-    <row r="7" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C7" s="3">
         <v>2</v>
       </c>
@@ -1466,16 +1450,16 @@
       <c r="AD7" s="3">
         <v>2</v>
       </c>
-      <c r="AE7" s="3">
-        <v>2</v>
-      </c>
-      <c r="AF7" s="3">
+      <c r="AE7">
         <v>3</v>
       </c>
-      <c r="AG7" s="12">
+      <c r="AF7" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AG7" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH7" s="10" t="s">
         <v>12</v>
       </c>
@@ -1485,11 +1469,11 @@
       <c r="AJ7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL7" s="9" t="s">
-        <v>11</v>
+      <c r="AK7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL7" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AM7" s="10" t="s">
         <v>12</v>
@@ -1503,24 +1487,21 @@
       <c r="AP7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU7" s="3">
+      <c r="AT7" s="3">
+        <v>2</v>
+      </c>
+      <c r="AU7">
         <v>2</v>
       </c>
       <c r="AV7">
-        <v>2</v>
-      </c>
-      <c r="AW7">
         <v>4</v>
       </c>
-      <c r="AX7" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW7" s="12">
+        <f>(F7+AF7)/2</f>
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C8" s="3">
         <v>3</v>
       </c>
@@ -1597,30 +1578,30 @@
       <c r="AD8" s="3">
         <v>3</v>
       </c>
-      <c r="AE8" s="3">
-        <v>1</v>
-      </c>
-      <c r="AF8" s="3">
-        <v>1</v>
-      </c>
-      <c r="AG8" s="12">
+      <c r="AE8">
+        <v>1</v>
+      </c>
+      <c r="AF8" s="12">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="AH8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI8" s="9" t="s">
-        <v>11</v>
+      <c r="AG8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI8" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AJ8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL8" s="9" t="s">
-        <v>11</v>
+      <c r="AK8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL8" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AM8" s="10" t="s">
         <v>12</v>
@@ -1634,24 +1615,21 @@
       <c r="AP8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU8" s="3">
+      <c r="AT8" s="3">
         <v>3</v>
       </c>
+      <c r="AU8">
+        <v>2</v>
+      </c>
       <c r="AV8">
-        <v>2</v>
-      </c>
-      <c r="AW8">
         <v>3</v>
       </c>
-      <c r="AX8" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW8" s="12">
+        <f>(F8+AF8)/2</f>
         <v>0.875</v>
       </c>
     </row>
-    <row r="9" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C9" s="3">
         <v>4</v>
       </c>
@@ -1728,16 +1706,16 @@
       <c r="AD9" s="3">
         <v>4</v>
       </c>
-      <c r="AE9" s="3">
-        <v>1</v>
-      </c>
-      <c r="AF9" s="3">
-        <v>1</v>
-      </c>
-      <c r="AG9" s="12">
+      <c r="AE9">
+        <v>1</v>
+      </c>
+      <c r="AF9" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AG9" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH9" s="10" t="s">
         <v>12</v>
       </c>
@@ -1750,11 +1728,11 @@
       <c r="AK9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AL9" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AM9" s="9" t="s">
-        <v>11</v>
+      <c r="AL9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM9" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AN9" s="10" t="s">
         <v>12</v>
@@ -1765,24 +1743,21 @@
       <c r="AP9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ9" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU9" s="3">
+      <c r="AT9" s="3">
         <v>4</v>
       </c>
+      <c r="AU9">
+        <v>2</v>
+      </c>
       <c r="AV9">
-        <v>2</v>
-      </c>
-      <c r="AW9">
         <v>3</v>
       </c>
-      <c r="AX9" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW9" s="12">
+        <f>(F9+AF9)/2</f>
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C10" s="3">
         <v>5</v>
       </c>
@@ -1859,36 +1834,36 @@
       <c r="AD10" s="3">
         <v>5</v>
       </c>
-      <c r="AE10" s="3">
-        <v>2</v>
-      </c>
-      <c r="AF10" s="3">
-        <v>2</v>
-      </c>
-      <c r="AG10" s="12">
+      <c r="AE10">
+        <v>2</v>
+      </c>
+      <c r="AF10" s="12">
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
-      <c r="AH10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ10" s="10" t="s">
-        <v>12</v>
+      <c r="AG10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ10" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AK10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AL10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AM10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN10" s="9" t="s">
-        <v>11</v>
+      <c r="AL10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN10" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AO10" s="10" t="s">
         <v>12</v>
@@ -1896,24 +1871,21 @@
       <c r="AP10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU10" s="3">
+      <c r="AT10" s="3">
         <v>5</v>
       </c>
+      <c r="AU10">
+        <v>2</v>
+      </c>
       <c r="AV10">
-        <v>2</v>
-      </c>
-      <c r="AW10">
         <v>4</v>
       </c>
-      <c r="AX10" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW10" s="12">
+        <f>(F10+AF10)/2</f>
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C11" s="3">
         <v>6</v>
       </c>
@@ -1990,16 +1962,16 @@
       <c r="AD11" s="3">
         <v>6</v>
       </c>
-      <c r="AE11" s="3">
-        <v>2</v>
-      </c>
-      <c r="AF11" s="3">
-        <v>2</v>
-      </c>
-      <c r="AG11" s="12">
+      <c r="AE11">
+        <v>2</v>
+      </c>
+      <c r="AF11" s="12">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
+      <c r="AG11" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH11" s="10" t="s">
         <v>12</v>
       </c>
@@ -2009,17 +1981,17 @@
       <c r="AJ11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AM11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN11" s="9" t="s">
-        <v>11</v>
+      <c r="AK11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN11" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AO11" s="10" t="s">
         <v>12</v>
@@ -2027,24 +1999,21 @@
       <c r="AP11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU11" s="3">
+      <c r="AT11" s="3">
         <v>6</v>
       </c>
+      <c r="AU11">
+        <v>2</v>
+      </c>
       <c r="AV11">
-        <v>2</v>
-      </c>
-      <c r="AW11">
         <v>4</v>
       </c>
-      <c r="AX11" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW11" s="12">
+        <f>(F11+AF11)/2</f>
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C12" s="3">
         <v>7</v>
       </c>
@@ -2121,16 +2090,16 @@
       <c r="AD12" s="3">
         <v>7</v>
       </c>
-      <c r="AE12" s="3">
-        <v>2</v>
-      </c>
-      <c r="AF12" s="3">
+      <c r="AE12">
         <v>3</v>
       </c>
-      <c r="AG12" s="12">
+      <c r="AF12" s="12">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
+      <c r="AG12" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH12" s="10" t="s">
         <v>12</v>
       </c>
@@ -2140,14 +2109,14 @@
       <c r="AJ12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK12" s="10" t="s">
-        <v>12</v>
+      <c r="AK12" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AL12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AM12" s="9" t="s">
-        <v>11</v>
+      <c r="AM12" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AN12" s="10" t="s">
         <v>12</v>
@@ -2158,24 +2127,21 @@
       <c r="AP12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ12" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU12" s="3">
+      <c r="AT12" s="3">
         <v>7</v>
       </c>
+      <c r="AU12">
+        <v>2</v>
+      </c>
       <c r="AV12">
-        <v>2</v>
-      </c>
-      <c r="AW12">
         <v>4</v>
       </c>
-      <c r="AX12" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW12" s="12">
+        <f>(F12+AF12)/2</f>
         <v>0.67500000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C13" s="3">
         <v>8</v>
       </c>
@@ -2252,16 +2218,16 @@
       <c r="AD13" s="3">
         <v>8</v>
       </c>
-      <c r="AE13" s="3">
-        <v>2</v>
-      </c>
-      <c r="AF13" s="3">
+      <c r="AE13">
         <v>3</v>
       </c>
-      <c r="AG13" s="12">
+      <c r="AF13" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AG13" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH13" s="10" t="s">
         <v>12</v>
       </c>
@@ -2277,11 +2243,11 @@
       <c r="AL13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM13" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN13" s="9" t="s">
-        <v>11</v>
+      <c r="AM13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN13" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AO13" s="10" t="s">
         <v>12</v>
@@ -2289,24 +2255,21 @@
       <c r="AP13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ13" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU13" s="3">
+      <c r="AT13" s="3">
         <v>8</v>
       </c>
+      <c r="AU13">
+        <v>2</v>
+      </c>
       <c r="AV13">
-        <v>2</v>
-      </c>
-      <c r="AW13">
         <v>4</v>
       </c>
-      <c r="AX13" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW13" s="12">
+        <f>(F13+AF13)/2</f>
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C14" s="3">
         <v>9</v>
       </c>
@@ -2383,16 +2346,16 @@
       <c r="AD14" s="3">
         <v>9</v>
       </c>
-      <c r="AE14" s="3">
-        <v>2</v>
-      </c>
-      <c r="AF14" s="3">
-        <v>2</v>
-      </c>
-      <c r="AG14" s="12">
+      <c r="AE14">
+        <v>2</v>
+      </c>
+      <c r="AF14" s="12">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
+      <c r="AG14" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH14" s="10" t="s">
         <v>12</v>
       </c>
@@ -2402,17 +2365,17 @@
       <c r="AJ14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK14" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL14" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AM14" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN14" s="9" t="s">
-        <v>11</v>
+      <c r="AK14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN14" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AO14" s="10" t="s">
         <v>12</v>
@@ -2420,24 +2383,21 @@
       <c r="AP14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ14" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU14" s="3">
+      <c r="AT14" s="3">
         <v>9</v>
       </c>
+      <c r="AU14">
+        <v>2</v>
+      </c>
       <c r="AV14">
-        <v>2</v>
-      </c>
-      <c r="AW14">
         <v>4</v>
       </c>
-      <c r="AX14" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW14" s="12">
+        <f>(F14+AF14)/2</f>
         <v>0.72500000000000009</v>
       </c>
     </row>
-    <row r="15" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C15" s="3">
         <v>10</v>
       </c>
@@ -2514,16 +2474,16 @@
       <c r="AD15" s="3">
         <v>10</v>
       </c>
-      <c r="AE15" s="3">
-        <v>2</v>
-      </c>
-      <c r="AF15" s="3">
+      <c r="AE15">
         <v>3</v>
       </c>
-      <c r="AG15" s="12">
+      <c r="AF15" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AG15" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH15" s="10" t="s">
         <v>12</v>
       </c>
@@ -2539,11 +2499,11 @@
       <c r="AL15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM15" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN15" s="9" t="s">
-        <v>11</v>
+      <c r="AM15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN15" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AO15" s="10" t="s">
         <v>12</v>
@@ -2551,107 +2511,105 @@
       <c r="AP15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ15" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU15" s="3">
+      <c r="AT15" s="3">
         <v>10</v>
       </c>
+      <c r="AU15">
+        <v>2</v>
+      </c>
       <c r="AV15">
-        <v>2</v>
-      </c>
-      <c r="AW15">
         <v>4</v>
       </c>
-      <c r="AX15" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW15" s="12">
+        <f>(F15+AF15)/2</f>
         <v>0.9</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="F16" s="12"/>
       <c r="G16" s="16">
         <f>(COUNTIF(G6:G15,"○"))/10</f>
         <v>0.6</v>
       </c>
       <c r="H16" s="16">
-        <f t="shared" ref="H16:Z16" si="4">(COUNTIF(H6:H15,"○"))/10</f>
+        <f t="shared" ref="H16:Z16" si="3">(COUNTIF(H6:H15,"○"))/10</f>
         <v>0.4</v>
       </c>
       <c r="I16" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
       <c r="J16" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
       <c r="K16" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L16" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
       <c r="M16" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="N16" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O16" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
       <c r="P16" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
       <c r="Q16" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="R16" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
       <c r="S16" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
       <c r="T16" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
       <c r="U16" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
       <c r="V16" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
       <c r="W16" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="X16" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
       <c r="Y16" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
       <c r="Z16" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
-      <c r="AG16" s="12"/>
-      <c r="AH16" s="10"/>
+      <c r="AF16" s="12"/>
+      <c r="AG16" s="10"/>
+      <c r="AH16" s="1"/>
       <c r="AI16" s="1"/>
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1"/>
@@ -2660,10 +2618,9 @@
       <c r="AN16" s="1"/>
       <c r="AO16" s="1"/>
       <c r="AP16" s="1"/>
-      <c r="AQ16" s="1"/>
-      <c r="AX16" s="12"/>
-    </row>
-    <row r="17" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="AW16" s="12"/>
+    </row>
+    <row r="17" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
@@ -2746,16 +2703,16 @@
       <c r="AD17" s="3">
         <v>1</v>
       </c>
-      <c r="AE17" s="3">
-        <v>2</v>
-      </c>
-      <c r="AF17" s="3">
-        <v>2</v>
-      </c>
-      <c r="AG17" s="12">
+      <c r="AE17">
+        <v>2</v>
+      </c>
+      <c r="AF17" s="12">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
+      <c r="AG17" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH17" s="10" t="s">
         <v>12</v>
       </c>
@@ -2765,17 +2722,17 @@
       <c r="AJ17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK17" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL17" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AM17" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN17" s="9" t="s">
-        <v>11</v>
+      <c r="AK17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN17" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AO17" s="10" t="s">
         <v>12</v>
@@ -2783,27 +2740,24 @@
       <c r="AP17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ17" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AT17" s="3" t="s">
+      <c r="AS17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AU17" s="3">
-        <v>1</v>
+      <c r="AT17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AU17">
+        <v>2</v>
       </c>
       <c r="AV17">
-        <v>2</v>
-      </c>
-      <c r="AW17">
         <v>4</v>
       </c>
-      <c r="AX17" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW17" s="12">
+        <f>(F17+AF17)/2</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C18" s="3">
         <v>2</v>
       </c>
@@ -2880,16 +2834,16 @@
       <c r="AD18" s="3">
         <v>2</v>
       </c>
-      <c r="AE18" s="3">
-        <v>2</v>
-      </c>
-      <c r="AF18" s="3">
+      <c r="AE18">
         <v>3</v>
       </c>
-      <c r="AG18" s="12">
+      <c r="AF18" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="AG18" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH18" s="10" t="s">
         <v>12</v>
       </c>
@@ -2917,24 +2871,21 @@
       <c r="AP18" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ18" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU18" s="3">
+      <c r="AT18" s="3">
+        <v>2</v>
+      </c>
+      <c r="AU18">
         <v>2</v>
       </c>
       <c r="AV18">
-        <v>2</v>
-      </c>
-      <c r="AW18">
         <v>4</v>
       </c>
-      <c r="AX18" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW18" s="12">
+        <f>(F18+AF18)/2</f>
         <v>0.6</v>
       </c>
     </row>
-    <row r="19" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C19" s="3">
         <v>3</v>
       </c>
@@ -3011,30 +2962,30 @@
       <c r="AD19" s="3">
         <v>3</v>
       </c>
-      <c r="AE19" s="3">
-        <v>2</v>
-      </c>
-      <c r="AF19" s="3">
+      <c r="AE19">
         <v>3</v>
       </c>
-      <c r="AG19" s="12">
+      <c r="AF19" s="12">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
+      <c r="AG19" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH19" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AI19" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ19" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AK19" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL19" s="9" t="s">
-        <v>11</v>
+      <c r="AI19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL19" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AM19" s="10" t="s">
         <v>12</v>
@@ -3048,24 +2999,21 @@
       <c r="AP19" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ19" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU19" s="3">
+      <c r="AT19" s="3">
         <v>3</v>
       </c>
+      <c r="AU19">
+        <v>2</v>
+      </c>
       <c r="AV19">
-        <v>2</v>
-      </c>
-      <c r="AW19">
         <v>3</v>
       </c>
-      <c r="AX19" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW19" s="12">
+        <f>(F19+AF19)/2</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C20" s="3">
         <v>4</v>
       </c>
@@ -3142,16 +3090,16 @@
       <c r="AD20" s="3">
         <v>4</v>
       </c>
-      <c r="AE20" s="3">
-        <v>2</v>
-      </c>
-      <c r="AF20" s="3">
+      <c r="AE20">
         <v>3</v>
       </c>
-      <c r="AG20" s="12">
+      <c r="AF20" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AG20" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH20" s="10" t="s">
         <v>12</v>
       </c>
@@ -3167,11 +3115,11 @@
       <c r="AL20" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM20" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN20" s="9" t="s">
-        <v>11</v>
+      <c r="AM20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN20" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AO20" s="10" t="s">
         <v>12</v>
@@ -3179,24 +3127,21 @@
       <c r="AP20" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ20" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU20" s="3">
+      <c r="AT20" s="3">
         <v>4</v>
       </c>
+      <c r="AU20">
+        <v>2</v>
+      </c>
       <c r="AV20">
-        <v>2</v>
-      </c>
-      <c r="AW20">
         <v>4</v>
       </c>
-      <c r="AX20" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW20" s="12">
+        <f>(F20+AF20)/2</f>
         <v>0.6</v>
       </c>
     </row>
-    <row r="21" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C21" s="3">
         <v>5</v>
       </c>
@@ -3273,16 +3218,16 @@
       <c r="AD21" s="3">
         <v>5</v>
       </c>
-      <c r="AE21" s="3">
-        <v>1</v>
-      </c>
-      <c r="AF21" s="3">
-        <v>1</v>
-      </c>
-      <c r="AG21" s="12">
+      <c r="AE21">
+        <v>1</v>
+      </c>
+      <c r="AF21" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AG21" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH21" s="10" t="s">
         <v>12</v>
       </c>
@@ -3292,11 +3237,11 @@
       <c r="AJ21" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK21" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL21" s="9" t="s">
-        <v>11</v>
+      <c r="AK21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL21" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AM21" s="10" t="s">
         <v>12</v>
@@ -3310,24 +3255,21 @@
       <c r="AP21" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ21" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU21" s="3">
+      <c r="AT21" s="3">
         <v>5</v>
       </c>
+      <c r="AU21">
+        <v>2</v>
+      </c>
       <c r="AV21">
-        <v>2</v>
-      </c>
-      <c r="AW21">
         <v>3</v>
       </c>
-      <c r="AX21" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW21" s="12">
+        <f>(F21+AF21)/2</f>
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="22" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C22" s="3">
         <v>6</v>
       </c>
@@ -3404,16 +3346,16 @@
       <c r="AD22" s="3">
         <v>6</v>
       </c>
-      <c r="AE22" s="3">
-        <v>2</v>
-      </c>
-      <c r="AF22" s="3">
-        <v>4</v>
-      </c>
-      <c r="AG22" s="12">
+      <c r="AE22">
+        <v>3</v>
+      </c>
+      <c r="AF22" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AG22" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH22" s="10" t="s">
         <v>12</v>
       </c>
@@ -3423,11 +3365,11 @@
       <c r="AJ22" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK22" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL22" s="9" t="s">
-        <v>11</v>
+      <c r="AK22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL22" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AM22" s="10" t="s">
         <v>12</v>
@@ -3441,24 +3383,21 @@
       <c r="AP22" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ22" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU22" s="3">
+      <c r="AT22" s="3">
         <v>6</v>
       </c>
+      <c r="AU22">
+        <v>2</v>
+      </c>
       <c r="AV22">
-        <v>2</v>
-      </c>
-      <c r="AW22">
         <v>4</v>
       </c>
-      <c r="AX22" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW22" s="12">
+        <f>(F22+AF22)/2</f>
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="23" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C23" s="3">
         <v>7</v>
       </c>
@@ -3535,16 +3474,16 @@
       <c r="AD23" s="3">
         <v>7</v>
       </c>
-      <c r="AE23" s="3">
-        <v>1</v>
-      </c>
-      <c r="AF23" s="3">
-        <v>1</v>
-      </c>
-      <c r="AG23" s="12">
+      <c r="AE23">
+        <v>1</v>
+      </c>
+      <c r="AF23" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="AG23" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH23" s="10" t="s">
         <v>12</v>
       </c>
@@ -3572,24 +3511,21 @@
       <c r="AP23" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ23" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU23" s="3">
+      <c r="AT23" s="3">
         <v>7</v>
       </c>
+      <c r="AU23">
+        <v>2</v>
+      </c>
       <c r="AV23">
-        <v>2</v>
-      </c>
-      <c r="AW23">
         <v>3</v>
       </c>
-      <c r="AX23" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW23" s="12">
+        <f>(F23+AF23)/2</f>
         <v>0.625</v>
       </c>
     </row>
-    <row r="24" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C24" s="3">
         <v>8</v>
       </c>
@@ -3666,16 +3602,16 @@
       <c r="AD24" s="3">
         <v>8</v>
       </c>
-      <c r="AE24" s="3">
-        <v>2</v>
-      </c>
-      <c r="AF24" s="3">
+      <c r="AE24">
         <v>3</v>
       </c>
-      <c r="AG24" s="12">
+      <c r="AF24" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="AG24" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH24" s="10" t="s">
         <v>12</v>
       </c>
@@ -3703,24 +3639,21 @@
       <c r="AP24" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ24" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU24" s="3">
+      <c r="AT24" s="3">
         <v>8</v>
       </c>
+      <c r="AU24">
+        <v>2</v>
+      </c>
       <c r="AV24">
-        <v>2</v>
-      </c>
-      <c r="AW24">
         <v>4</v>
       </c>
-      <c r="AX24" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW24" s="12">
+        <f>(F24+AF24)/2</f>
         <v>0.625</v>
       </c>
     </row>
-    <row r="25" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C25" s="3">
         <v>9</v>
       </c>
@@ -3797,16 +3730,16 @@
       <c r="AD25" s="3">
         <v>9</v>
       </c>
-      <c r="AE25" s="3">
-        <v>2</v>
-      </c>
-      <c r="AF25" s="3">
+      <c r="AE25">
         <v>3</v>
       </c>
-      <c r="AG25" s="12">
+      <c r="AF25" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AG25" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH25" s="10" t="s">
         <v>12</v>
       </c>
@@ -3822,11 +3755,11 @@
       <c r="AL25" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM25" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN25" s="9" t="s">
-        <v>11</v>
+      <c r="AM25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN25" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AO25" s="10" t="s">
         <v>12</v>
@@ -3834,24 +3767,21 @@
       <c r="AP25" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ25" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU25" s="3">
+      <c r="AT25" s="3">
         <v>9</v>
       </c>
+      <c r="AU25">
+        <v>2</v>
+      </c>
       <c r="AV25">
-        <v>2</v>
-      </c>
-      <c r="AW25">
         <v>4</v>
       </c>
-      <c r="AX25" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW25" s="12">
+        <f>(F25+AF25)/2</f>
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="26" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C26" s="3">
         <v>10</v>
       </c>
@@ -3928,24 +3858,24 @@
       <c r="AD26" s="3">
         <v>10</v>
       </c>
-      <c r="AE26" s="3">
-        <v>2</v>
-      </c>
-      <c r="AF26" s="3">
-        <v>2</v>
-      </c>
-      <c r="AG26" s="12">
+      <c r="AE26">
+        <v>2</v>
+      </c>
+      <c r="AF26" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AG26" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH26" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AI26" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ26" s="9" t="s">
-        <v>11</v>
+      <c r="AI26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ26" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AK26" s="10" t="s">
         <v>12</v>
@@ -3965,24 +3895,21 @@
       <c r="AP26" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ26" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU26" s="3">
+      <c r="AT26" s="3">
         <v>10</v>
       </c>
+      <c r="AU26">
+        <v>2</v>
+      </c>
       <c r="AV26">
-        <v>2</v>
-      </c>
-      <c r="AW26">
         <v>3</v>
       </c>
-      <c r="AX26" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW26" s="12">
+        <f>(F26+AF26)/2</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C27" s="3">
         <v>11</v>
       </c>
@@ -4059,16 +3986,16 @@
       <c r="AD27" s="3">
         <v>11</v>
       </c>
-      <c r="AE27" s="3">
-        <v>1</v>
-      </c>
-      <c r="AF27" s="3">
-        <v>1</v>
-      </c>
-      <c r="AG27" s="12">
+      <c r="AE27">
+        <v>1</v>
+      </c>
+      <c r="AF27" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="AG27" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH27" s="10" t="s">
         <v>12</v>
       </c>
@@ -4096,24 +4023,21 @@
       <c r="AP27" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ27" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU27" s="3">
-        <v>11</v>
+      <c r="AT27" s="3">
+        <v>11</v>
+      </c>
+      <c r="AU27">
+        <v>2</v>
       </c>
       <c r="AV27">
-        <v>2</v>
-      </c>
-      <c r="AW27">
         <v>4</v>
       </c>
-      <c r="AX27" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW27" s="12">
+        <f>(F27+AF27)/2</f>
         <v>0.52500000000000002</v>
       </c>
     </row>
-    <row r="28" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C28" s="3">
         <v>12</v>
       </c>
@@ -4190,16 +4114,16 @@
       <c r="AD28" s="3">
         <v>12</v>
       </c>
-      <c r="AE28" s="3">
-        <v>1</v>
-      </c>
-      <c r="AF28" s="3">
-        <v>1</v>
-      </c>
-      <c r="AG28" s="12">
+      <c r="AE28">
+        <v>1</v>
+      </c>
+      <c r="AF28" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="AG28" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH28" s="10" t="s">
         <v>12</v>
       </c>
@@ -4227,24 +4151,21 @@
       <c r="AP28" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ28" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU28" s="3">
-        <v>12</v>
+      <c r="AT28" s="3">
+        <v>12</v>
+      </c>
+      <c r="AU28">
+        <v>2</v>
       </c>
       <c r="AV28">
-        <v>2</v>
-      </c>
-      <c r="AW28">
         <v>4</v>
       </c>
-      <c r="AX28" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW28" s="12">
+        <f>(F28+AF28)/2</f>
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="29" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C29" s="3">
         <v>13</v>
       </c>
@@ -4321,16 +4242,16 @@
       <c r="AD29" s="3">
         <v>13</v>
       </c>
-      <c r="AE29" s="3">
-        <v>1</v>
-      </c>
-      <c r="AF29" s="3">
-        <v>1</v>
-      </c>
-      <c r="AG29" s="12">
+      <c r="AE29">
+        <v>1</v>
+      </c>
+      <c r="AF29" s="12">
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
+      <c r="AG29" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH29" s="10" t="s">
         <v>12</v>
       </c>
@@ -4340,42 +4261,39 @@
       <c r="AJ29" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK29" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL29" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AM29" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN29" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AO29" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP29" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AQ29" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU29" s="3">
+      <c r="AK29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AP29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AT29" s="3">
         <v>13</v>
       </c>
+      <c r="AU29">
+        <v>2</v>
+      </c>
       <c r="AV29">
-        <v>2</v>
-      </c>
-      <c r="AW29">
         <v>4</v>
       </c>
-      <c r="AX29" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW29" s="12">
+        <f>(F29+AF29)/2</f>
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="30" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C30" s="3">
         <v>14</v>
       </c>
@@ -4452,16 +4370,16 @@
       <c r="AD30" s="3">
         <v>14</v>
       </c>
-      <c r="AE30" s="3">
-        <v>1</v>
-      </c>
-      <c r="AF30" s="3">
-        <v>1</v>
-      </c>
-      <c r="AG30" s="12">
+      <c r="AE30">
+        <v>1</v>
+      </c>
+      <c r="AF30" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AG30" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH30" s="10" t="s">
         <v>12</v>
       </c>
@@ -4471,11 +4389,11 @@
       <c r="AJ30" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK30" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL30" s="9" t="s">
-        <v>11</v>
+      <c r="AK30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL30" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AM30" s="10" t="s">
         <v>12</v>
@@ -4489,67 +4407,64 @@
       <c r="AP30" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ30" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU30" s="3">
+      <c r="AT30" s="3">
         <v>14</v>
       </c>
+      <c r="AU30">
+        <v>2</v>
+      </c>
       <c r="AV30">
-        <v>2</v>
-      </c>
-      <c r="AW30">
         <v>4</v>
       </c>
-      <c r="AX30" s="12">
-        <f t="shared" si="2"/>
+      <c r="AW30" s="12">
+        <f>(F30+AF30)/2</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F31" s="5"/>
       <c r="G31" s="15">
         <f>(COUNTIF(G17:G30,"○"))/14</f>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="H31" s="15">
-        <f t="shared" ref="H31:Z31" si="5">(COUNTIF(H17:H30,"○"))/14</f>
+        <f t="shared" ref="H31:Z31" si="4">(COUNTIF(H17:H30,"○"))/14</f>
         <v>0.14285714285714285</v>
       </c>
       <c r="I31" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.42857142857142855</v>
       </c>
       <c r="J31" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="K31" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.35714285714285715</v>
       </c>
       <c r="L31" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="M31" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.35714285714285715</v>
       </c>
       <c r="N31" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="O31" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P31" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q31" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="R31" s="15">
@@ -4557,35 +4472,35 @@
         <v>0</v>
       </c>
       <c r="S31" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T31" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U31" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="V31" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="W31" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="X31" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.35714285714285715</v>
       </c>
       <c r="Y31" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.7857142857142857</v>
       </c>
       <c r="Z31" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="AC31" s="3" t="s">
@@ -4594,16 +4509,16 @@
       <c r="AD31" s="3">
         <v>1</v>
       </c>
-      <c r="AE31" s="3">
-        <v>1</v>
-      </c>
-      <c r="AF31" s="3">
-        <v>1</v>
-      </c>
-      <c r="AG31" s="12">
+      <c r="AE31">
+        <v>1</v>
+      </c>
+      <c r="AF31" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AG31" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH31" s="10" t="s">
         <v>12</v>
       </c>
@@ -4619,11 +4534,11 @@
       <c r="AL31" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM31" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN31" s="9" t="s">
-        <v>11</v>
+      <c r="AM31" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN31" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AO31" s="10" t="s">
         <v>12</v>
@@ -4631,41 +4546,38 @@
       <c r="AP31" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ31" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AT31" s="3" t="s">
+      <c r="AS31" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AU31" s="3">
+      <c r="AT31" s="3">
+        <v>1</v>
+      </c>
+      <c r="AU31">
         <v>1</v>
       </c>
       <c r="AV31">
-        <v>1</v>
-      </c>
-      <c r="AW31">
-        <v>2</v>
-      </c>
-      <c r="AX31" s="12">
-        <f>AG31</f>
+        <v>2</v>
+      </c>
+      <c r="AW31" s="12">
+        <f>AF31</f>
         <v>0.9</v>
       </c>
     </row>
-    <row r="32" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F32" s="12"/>
       <c r="AD32" s="3">
         <v>2</v>
       </c>
-      <c r="AE32" s="3">
-        <v>1</v>
-      </c>
-      <c r="AF32" s="3">
-        <v>1</v>
-      </c>
-      <c r="AG32" s="12">
+      <c r="AE32">
+        <v>1</v>
+      </c>
+      <c r="AF32" s="12">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
+      <c r="AG32" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH32" s="10" t="s">
         <v>12</v>
       </c>
@@ -4675,11 +4587,11 @@
       <c r="AJ32" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK32" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL32" s="9" t="s">
-        <v>11</v>
+      <c r="AK32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL32" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AM32" s="10" t="s">
         <v>12</v>
@@ -4687,46 +4599,43 @@
       <c r="AN32" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AO32" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP32" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AQ32" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU32" s="3">
-        <v>2</v>
+      <c r="AO32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AP32" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AT32" s="3">
+        <v>2</v>
+      </c>
+      <c r="AU32">
+        <v>1</v>
       </c>
       <c r="AV32">
-        <v>1</v>
-      </c>
-      <c r="AW32">
-        <v>2</v>
-      </c>
-      <c r="AX32" s="12">
-        <f t="shared" ref="AX32:AX36" si="6">AG32</f>
+        <v>2</v>
+      </c>
+      <c r="AW32" s="12">
+        <f t="shared" ref="AW32:AW36" si="5">AF32</f>
         <v>0.8</v>
       </c>
     </row>
-    <row r="33" spans="29:50" x14ac:dyDescent="0.25">
+    <row r="33" spans="29:49" x14ac:dyDescent="0.25">
       <c r="AC33" s="3" t="s">
         <v>7</v>
       </c>
       <c r="AD33" s="3">
         <v>1</v>
       </c>
-      <c r="AE33" s="3">
-        <v>2</v>
-      </c>
-      <c r="AF33" s="3">
+      <c r="AE33">
         <v>3</v>
       </c>
-      <c r="AG33" s="12">
+      <c r="AF33" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="AG33" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH33" s="10" t="s">
         <v>12</v>
       </c>
@@ -4754,40 +4663,37 @@
       <c r="AP33" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ33" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AT33" s="3" t="s">
+      <c r="AS33" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AU33" s="3">
+      <c r="AT33" s="3">
+        <v>1</v>
+      </c>
+      <c r="AU33">
         <v>1</v>
       </c>
       <c r="AV33">
-        <v>1</v>
-      </c>
-      <c r="AW33">
-        <v>2</v>
-      </c>
-      <c r="AX33" s="12">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="29:50" ht="16.5" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="AW33" s="12">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="29:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="AD34" s="3">
         <v>2</v>
       </c>
-      <c r="AE34" s="3">
-        <v>1</v>
-      </c>
-      <c r="AF34" s="3">
-        <v>1</v>
-      </c>
-      <c r="AG34" s="12">
+      <c r="AE34">
+        <v>1</v>
+      </c>
+      <c r="AF34" s="12">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AG34" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH34" s="10" t="s">
         <v>12</v>
       </c>
@@ -4803,11 +4709,11 @@
       <c r="AL34" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM34" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN34" s="9" t="s">
-        <v>11</v>
+      <c r="AM34" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN34" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AO34" s="10" t="s">
         <v>12</v>
@@ -4815,37 +4721,34 @@
       <c r="AP34" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ34" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU34" s="3">
-        <v>2</v>
+      <c r="AT34" s="3">
+        <v>2</v>
+      </c>
+      <c r="AU34">
+        <v>1</v>
       </c>
       <c r="AV34">
-        <v>1</v>
-      </c>
-      <c r="AW34">
-        <v>2</v>
-      </c>
-      <c r="AX34" s="12">
-        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="AW34" s="12">
+        <f t="shared" si="5"/>
         <v>0.9</v>
       </c>
     </row>
-    <row r="35" spans="29:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="29:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="AD35" s="3">
         <v>3</v>
       </c>
-      <c r="AE35" s="3">
-        <v>2</v>
-      </c>
-      <c r="AF35" s="3">
-        <v>2</v>
-      </c>
-      <c r="AG35" s="12">
+      <c r="AE35">
+        <v>2</v>
+      </c>
+      <c r="AF35" s="12">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
+      <c r="AG35" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH35" s="10" t="s">
         <v>12</v>
       </c>
@@ -4867,46 +4770,43 @@
       <c r="AN35" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AO35" s="10" t="s">
-        <v>12</v>
+      <c r="AO35" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AP35" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AQ35" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AU35" s="3">
+      <c r="AT35" s="3">
         <v>3</v>
       </c>
+      <c r="AU35">
+        <v>1</v>
+      </c>
       <c r="AV35">
         <v>1</v>
       </c>
-      <c r="AW35">
-        <v>1</v>
-      </c>
-      <c r="AX35" s="12">
-        <f t="shared" si="6"/>
+      <c r="AW35" s="12">
+        <f t="shared" si="5"/>
         <v>0.8</v>
       </c>
     </row>
-    <row r="36" spans="29:50" x14ac:dyDescent="0.25">
+    <row r="36" spans="29:49" x14ac:dyDescent="0.25">
       <c r="AC36" s="3" t="s">
         <v>6</v>
       </c>
       <c r="AD36" s="3">
         <v>1</v>
       </c>
-      <c r="AE36" s="3">
-        <v>2</v>
-      </c>
-      <c r="AF36" s="3">
+      <c r="AE36">
         <v>3</v>
       </c>
-      <c r="AG36" s="12">
+      <c r="AF36" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="AG36" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AH36" s="10" t="s">
         <v>12</v>
       </c>
@@ -4934,78 +4834,75 @@
       <c r="AP36" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AQ36" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AT36" s="3" t="s">
+      <c r="AS36" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AU36" s="3">
+      <c r="AT36" s="3">
+        <v>1</v>
+      </c>
+      <c r="AU36">
         <v>1</v>
       </c>
       <c r="AV36">
         <v>1</v>
       </c>
-      <c r="AW36">
-        <v>1</v>
-      </c>
-      <c r="AX36" s="12">
+      <c r="AW36" s="12">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="29:49" x14ac:dyDescent="0.25">
+      <c r="AG37" s="15">
+        <f>(COUNTIF(AG3:AG36,"○")/32)</f>
+        <v>1</v>
+      </c>
+      <c r="AH37" s="15">
+        <f t="shared" ref="AH37:AP37" si="6">(COUNTIF(AH3:AH36,"○")/32)</f>
+        <v>0.9375</v>
+      </c>
+      <c r="AI37" s="15">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="29:50" x14ac:dyDescent="0.25">
-      <c r="AH37" s="15">
-        <f>(COUNTIF(AH3:AH36,"○")/32)</f>
-        <v>1</v>
-      </c>
-      <c r="AI37" s="15">
-        <f t="shared" ref="AI37:AQ37" si="7">(COUNTIF(AI3:AI36,"○")/32)</f>
         <v>0.9375</v>
       </c>
       <c r="AJ37" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
+        <v>0.96875</v>
+      </c>
+      <c r="AK37" s="15">
+        <f t="shared" si="6"/>
+        <v>0.59375</v>
+      </c>
+      <c r="AL37" s="15">
+        <f t="shared" si="6"/>
+        <v>0.875</v>
+      </c>
+      <c r="AM37" s="15">
+        <f t="shared" si="6"/>
+        <v>0.5625</v>
+      </c>
+      <c r="AN37" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AO37" s="15">
+        <f t="shared" si="6"/>
+        <v>0.875</v>
+      </c>
+      <c r="AP37" s="15">
+        <f t="shared" si="6"/>
         <v>0.9375</v>
       </c>
-      <c r="AK37" s="15">
-        <f t="shared" si="7"/>
-        <v>0.96875</v>
-      </c>
-      <c r="AL37" s="15">
-        <f t="shared" si="7"/>
-        <v>0.59375</v>
-      </c>
-      <c r="AM37" s="15">
-        <f t="shared" si="7"/>
-        <v>0.875</v>
-      </c>
-      <c r="AN37" s="15">
-        <f t="shared" si="7"/>
-        <v>0.5625</v>
-      </c>
-      <c r="AO37" s="15">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AP37" s="15">
-        <f t="shared" si="7"/>
-        <v>0.875</v>
-      </c>
-      <c r="AQ37" s="15">
-        <f t="shared" si="7"/>
-        <v>0.9375</v>
-      </c>
-    </row>
-    <row r="38" spans="29:50" x14ac:dyDescent="0.25">
-      <c r="AX38" s="12"/>
-    </row>
-    <row r="39" spans="29:50" x14ac:dyDescent="0.25">
-      <c r="AG39" s="12"/>
+    </row>
+    <row r="38" spans="29:49" x14ac:dyDescent="0.25">
+      <c r="AW38" s="12"/>
+    </row>
+    <row r="39" spans="29:49" x14ac:dyDescent="0.25">
+      <c r="AF39" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="G1:Z1"/>
-    <mergeCell ref="AH1:AQ1"/>
+    <mergeCell ref="AG1:AP1"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5015,11 +4912,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88CCFB4E-3D94-4A97-83BE-04827B31FA43}">
-  <dimension ref="A1:Z29"/>
+  <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5625,7 +5520,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
@@ -5706,881 +5601,654 @@
         <v>2</v>
       </c>
       <c r="D11" s="12">
-        <v>0.86</v>
+        <v>0.76</v>
       </c>
       <c r="E11">
-        <v>2167.9</v>
+        <v>2648.125</v>
       </c>
       <c r="F11">
-        <v>250630.62105300001</v>
+        <v>55486.696429000003</v>
       </c>
       <c r="G11">
-        <v>714.95</v>
+        <v>708.5</v>
       </c>
       <c r="H11">
-        <v>5170.9973680000003</v>
+        <v>3474</v>
       </c>
       <c r="I11">
-        <v>475.85</v>
+        <v>503.375</v>
       </c>
       <c r="J11">
-        <v>17190.344736999999</v>
+        <v>33555.696429000003</v>
       </c>
       <c r="K11">
-        <v>260.65306299999997</v>
+        <v>267.79143699999997</v>
       </c>
       <c r="L11">
-        <v>1835.207633</v>
+        <v>2273.0406410000001</v>
       </c>
       <c r="M11">
-        <v>1056.411304</v>
+        <v>1209.3295149999999</v>
       </c>
       <c r="N11">
-        <v>34679.796719999998</v>
+        <v>20713.141038000002</v>
       </c>
       <c r="O11">
-        <v>319.25</v>
+        <v>374.5</v>
       </c>
       <c r="P11">
-        <v>4776.6184210000001</v>
+        <v>1853.4285709999999</v>
       </c>
       <c r="Q11">
-        <v>1060.408426</v>
+        <v>1045.4341790000001</v>
       </c>
       <c r="R11">
-        <v>23698.880735999999</v>
+        <v>21069.456459000001</v>
       </c>
       <c r="S11">
-        <v>1993.3181139999999</v>
+        <v>2077.987709</v>
       </c>
       <c r="T11">
-        <v>111216.08438499999</v>
+        <v>103616.614068</v>
       </c>
       <c r="U11">
-        <v>127671.448353</v>
+        <v>151747.92726200001</v>
       </c>
       <c r="V11" s="18">
-        <v>998679300</v>
+        <v>337635700</v>
       </c>
       <c r="W11">
-        <v>826.87913200000003</v>
+        <v>686.14610900000002</v>
       </c>
       <c r="X11">
-        <v>24907.053950000001</v>
+        <v>7382.4387580000002</v>
       </c>
       <c r="Y11">
-        <v>4.3660000000000001E-3</v>
+        <v>9.4352000000000005E-2</v>
       </c>
       <c r="Z11">
-        <v>3.2160000000000001E-2</v>
+        <v>3.3871999999999999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B12" s="3">
-        <v>4</v>
-      </c>
+      <c r="B12" s="3"/>
       <c r="C12" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D12" s="12">
-        <v>0.89</v>
+        <v>0.92</v>
       </c>
       <c r="E12">
-        <v>1830.25</v>
+        <v>1847.75</v>
       </c>
       <c r="F12">
-        <v>118833.295455</v>
+        <v>118063.11363599999</v>
       </c>
       <c r="G12">
-        <v>772.5</v>
+        <v>719.25</v>
       </c>
       <c r="H12">
-        <v>6660.0909089999996</v>
+        <v>6670.568182</v>
       </c>
       <c r="I12">
-        <v>423.08333299999998</v>
+        <v>457.5</v>
       </c>
       <c r="J12">
-        <v>4160.992424</v>
+        <v>7420.4545449999996</v>
       </c>
       <c r="K12">
-        <v>378.01879700000001</v>
+        <v>255.894147</v>
       </c>
       <c r="L12">
-        <v>4584.8516010000003</v>
+        <v>1661.658381</v>
       </c>
       <c r="M12">
-        <v>1295.7533490000001</v>
+        <v>954.46582999999998</v>
       </c>
       <c r="N12">
-        <v>23940.556202</v>
+        <v>18376.15987</v>
       </c>
       <c r="O12">
-        <v>247.5</v>
+        <v>282.41666700000002</v>
       </c>
       <c r="P12">
-        <v>2958.272727</v>
+        <v>3370.992424</v>
       </c>
       <c r="Q12">
-        <v>1392.8550399999999</v>
+        <v>1070.391257</v>
       </c>
       <c r="R12">
-        <v>20620.633055999999</v>
+        <v>27254.802844000002</v>
       </c>
       <c r="S12">
-        <v>2700.9950840000001</v>
+        <v>1936.871717</v>
       </c>
       <c r="T12">
-        <v>191521.769967</v>
+        <v>117473.039372</v>
       </c>
       <c r="U12">
-        <v>140455.03805800001</v>
+        <v>111620.462413</v>
       </c>
       <c r="V12" s="18">
-        <v>855042200</v>
+        <v>807493900</v>
       </c>
       <c r="W12">
-        <v>1071.5283179999999</v>
+        <v>920.70114699999999</v>
       </c>
       <c r="X12">
-        <v>21250.853659</v>
+        <v>14316.348910000001</v>
       </c>
       <c r="Y12">
-        <v>-4.5433000000000001E-2</v>
+        <v>-5.5625000000000001E-2</v>
       </c>
       <c r="Z12">
-        <v>1.6001999999999999E-2</v>
+        <v>2.4178999999999999E-2</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
-      <c r="C13" s="3">
-        <v>2</v>
-      </c>
-      <c r="D13" s="12">
-        <v>0.76</v>
-      </c>
-      <c r="E13">
-        <v>2648.125</v>
-      </c>
-      <c r="F13">
-        <v>55486.696429000003</v>
-      </c>
-      <c r="G13">
-        <v>708.5</v>
-      </c>
-      <c r="H13">
-        <v>3474</v>
-      </c>
-      <c r="I13">
-        <v>503.375</v>
-      </c>
-      <c r="J13">
-        <v>33555.696429000003</v>
-      </c>
-      <c r="K13">
-        <v>267.79143699999997</v>
-      </c>
-      <c r="L13">
-        <v>2273.0406410000001</v>
-      </c>
-      <c r="M13">
-        <v>1209.3295149999999</v>
-      </c>
-      <c r="N13">
-        <v>20713.141038000002</v>
-      </c>
-      <c r="O13">
-        <v>374.5</v>
-      </c>
-      <c r="P13">
-        <v>1853.4285709999999</v>
-      </c>
-      <c r="Q13">
-        <v>1045.4341790000001</v>
-      </c>
-      <c r="R13">
-        <v>21069.456459000001</v>
-      </c>
-      <c r="S13">
-        <v>2077.987709</v>
-      </c>
-      <c r="T13">
-        <v>103616.614068</v>
-      </c>
-      <c r="U13">
-        <v>151747.92726200001</v>
-      </c>
-      <c r="V13" s="18">
-        <v>337635700</v>
-      </c>
-      <c r="W13">
-        <v>686.14610900000002</v>
-      </c>
-      <c r="X13">
-        <v>7382.4387580000002</v>
-      </c>
-      <c r="Y13">
-        <v>9.4352000000000005E-2</v>
-      </c>
-      <c r="Z13">
-        <v>3.3871999999999999E-2</v>
-      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="12"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
+      <c r="A14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2</v>
+      </c>
       <c r="C14" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D14" s="12">
-        <v>0.92</v>
+        <v>0.9</v>
       </c>
       <c r="E14">
-        <v>1897.727273</v>
+        <v>1739.833333</v>
       </c>
       <c r="F14">
-        <v>96899.418181999994</v>
+        <v>178983.76666699999</v>
       </c>
       <c r="G14">
-        <v>712.09090900000001</v>
+        <v>752</v>
       </c>
       <c r="H14">
-        <v>6661.0909089999996</v>
+        <v>14627.2</v>
       </c>
       <c r="I14">
-        <v>452.454545</v>
+        <v>432.66666700000002</v>
       </c>
       <c r="J14">
-        <v>7826.4727270000003</v>
+        <v>2790.666667</v>
       </c>
       <c r="K14">
-        <v>264.54445399999997</v>
+        <v>307.72950600000001</v>
       </c>
       <c r="L14">
-        <v>840.09712400000001</v>
+        <v>4890.5534399999997</v>
       </c>
       <c r="M14">
-        <v>980.94243300000005</v>
+        <v>1112.6261919999999</v>
       </c>
       <c r="N14">
-        <v>10960.436761999999</v>
+        <v>37055.747754999997</v>
       </c>
       <c r="O14">
-        <v>288.90909099999999</v>
+        <v>249.66666699999999</v>
       </c>
       <c r="P14">
-        <v>3151.6909089999999</v>
+        <v>4420.6666670000004</v>
       </c>
       <c r="Q14">
-        <v>1101.6214869999999</v>
+        <v>1211.0714700000001</v>
       </c>
       <c r="R14">
-        <v>17105.962804999999</v>
+        <v>71898.080390999996</v>
       </c>
       <c r="S14">
-        <v>2013.9289679999999</v>
+        <v>2251.2261530000001</v>
       </c>
       <c r="T14">
-        <v>50841.120057</v>
+        <v>175012.62764200001</v>
       </c>
       <c r="U14">
-        <v>116905.84852499999</v>
+        <v>114600.766343</v>
       </c>
       <c r="V14" s="18">
-        <v>519497200</v>
+        <v>510096100</v>
       </c>
       <c r="W14">
-        <v>917.81769599999996</v>
+        <v>1025.3733279999999</v>
       </c>
       <c r="X14">
-        <v>15638.235188000001</v>
+        <v>76444.986667999998</v>
       </c>
       <c r="Y14">
-        <v>-9.3839000000000006E-2</v>
+        <v>2.0501999999999999E-2</v>
       </c>
       <c r="Z14">
-        <v>7.3210000000000003E-3</v>
+        <v>7.541E-3</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="3">
+        <v>2</v>
+      </c>
+      <c r="D15" s="12">
+        <v>0.65</v>
+      </c>
+      <c r="E15">
+        <v>3385.0576919999999</v>
+      </c>
+      <c r="F15">
+        <v>592731.926538</v>
+      </c>
+      <c r="G15">
+        <v>827.61538499999995</v>
+      </c>
+      <c r="H15">
+        <v>1930.886154</v>
+      </c>
+      <c r="I15">
+        <v>410.90384599999999</v>
+      </c>
+      <c r="J15">
+        <v>2171.8803849999999</v>
+      </c>
+      <c r="K15">
+        <v>371.539221</v>
+      </c>
+      <c r="L15">
+        <v>1035.578855</v>
+      </c>
+      <c r="M15">
+        <v>1222.5497009999999</v>
+      </c>
+      <c r="N15">
+        <v>15536.642760999999</v>
+      </c>
+      <c r="O15">
+        <v>498.94230800000003</v>
+      </c>
+      <c r="P15">
+        <v>16900.946538</v>
+      </c>
+      <c r="Q15">
+        <v>1245.3258940000001</v>
+      </c>
+      <c r="R15">
+        <v>12740.419583999999</v>
+      </c>
+      <c r="S15">
+        <v>2578.3067820000001</v>
+      </c>
+      <c r="T15">
+        <v>49049.371189999998</v>
+      </c>
+      <c r="U15">
+        <v>193914.33996899999</v>
+      </c>
+      <c r="V15" s="18">
+        <v>1004123000</v>
+      </c>
+      <c r="W15">
+        <v>722.09551699999997</v>
+      </c>
+      <c r="X15">
+        <v>4047.1366130000001</v>
+      </c>
+      <c r="Y15">
+        <v>-0.116019</v>
+      </c>
+      <c r="Z15">
+        <v>5.2220000000000001E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B16" s="3">
         <v>4</v>
       </c>
-      <c r="D15" s="12">
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="12">
         <v>0.9</v>
       </c>
-      <c r="E15">
-        <v>1298</v>
-      </c>
-      <c r="F15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15">
-        <v>798</v>
-      </c>
-      <c r="H15" t="s">
-        <v>32</v>
-      </c>
-      <c r="I15">
-        <v>513</v>
-      </c>
-      <c r="J15" t="s">
-        <v>32</v>
-      </c>
-      <c r="K15">
-        <v>160.740771</v>
-      </c>
-      <c r="L15" t="s">
-        <v>32</v>
-      </c>
-      <c r="M15">
-        <v>663.22319000000005</v>
-      </c>
-      <c r="N15" t="s">
-        <v>32</v>
-      </c>
-      <c r="O15">
-        <v>211</v>
-      </c>
-      <c r="P15" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q15">
-        <v>726.85872099999995</v>
-      </c>
-      <c r="R15" t="s">
-        <v>32</v>
-      </c>
-      <c r="S15">
-        <v>1089.241955</v>
-      </c>
-      <c r="T15" t="s">
-        <v>32</v>
-      </c>
-      <c r="U15">
-        <v>53481.215179999999</v>
-      </c>
-      <c r="V15" t="s">
-        <v>32</v>
-      </c>
-      <c r="W15">
-        <v>952.41910600000006</v>
-      </c>
-      <c r="X15" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y15">
-        <v>0.364732</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="12"/>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="3">
-        <v>2</v>
-      </c>
+      <c r="E16">
+        <v>2178</v>
+      </c>
+      <c r="F16">
+        <v>302642</v>
+      </c>
+      <c r="G16">
+        <v>654</v>
+      </c>
+      <c r="H16">
+        <v>10368</v>
+      </c>
+      <c r="I16">
+        <v>395.5</v>
+      </c>
+      <c r="J16">
+        <v>1104.5</v>
+      </c>
+      <c r="K16">
+        <v>229.304495</v>
+      </c>
+      <c r="L16">
+        <v>106.140266</v>
+      </c>
+      <c r="M16">
+        <v>989.65582400000005</v>
+      </c>
+      <c r="N16">
+        <v>1239.699991</v>
+      </c>
+      <c r="O16">
+        <v>311.5</v>
+      </c>
+      <c r="P16">
+        <v>7320.5</v>
+      </c>
+      <c r="Q16">
+        <v>930.86591499999997</v>
+      </c>
+      <c r="R16">
+        <v>1374.7302589999999</v>
+      </c>
+      <c r="S16">
+        <v>1828.920476</v>
+      </c>
+      <c r="T16">
+        <v>1718.9084230000001</v>
+      </c>
+      <c r="U16">
+        <v>114951.28943</v>
+      </c>
+      <c r="V16" s="18">
+        <v>1191293000</v>
+      </c>
+      <c r="W16">
+        <v>713.24588500000004</v>
+      </c>
+      <c r="X16">
+        <v>45534.539232000003</v>
+      </c>
+      <c r="Y16">
+        <v>6.3261999999999999E-2</v>
+      </c>
+      <c r="Z16">
+        <v>6.6000000000000005E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
       <c r="C17" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="12">
         <v>0.9</v>
       </c>
       <c r="E17">
-        <v>1739.833333</v>
+        <v>1520.75</v>
       </c>
       <c r="F17">
-        <v>178983.76666699999</v>
+        <v>5435.5833329999996</v>
       </c>
       <c r="G17">
-        <v>752</v>
+        <v>801</v>
       </c>
       <c r="H17">
-        <v>14627.2</v>
+        <v>11318.666667</v>
       </c>
       <c r="I17">
-        <v>432.66666700000002</v>
+        <v>451.25</v>
       </c>
       <c r="J17">
-        <v>2790.666667</v>
+        <v>2901.583333</v>
       </c>
       <c r="K17">
-        <v>307.72950600000001</v>
+        <v>346.94201199999998</v>
       </c>
       <c r="L17">
-        <v>4890.5534399999997</v>
+        <v>1965.059966</v>
       </c>
       <c r="M17">
-        <v>1112.6261919999999</v>
+        <v>1174.1113760000001</v>
       </c>
       <c r="N17">
-        <v>37055.747754999997</v>
+        <v>46224.634835999997</v>
       </c>
       <c r="O17">
-        <v>249.66666699999999</v>
+        <v>218.75</v>
       </c>
       <c r="P17">
-        <v>4420.6666670000004</v>
+        <v>1104.25</v>
       </c>
       <c r="Q17">
-        <v>1211.0714700000001</v>
+        <v>1351.174248</v>
       </c>
       <c r="R17">
-        <v>71898.080390999996</v>
+        <v>40856.737567999997</v>
       </c>
       <c r="S17">
-        <v>2251.2261530000001</v>
+        <v>2462.378991</v>
       </c>
       <c r="T17">
-        <v>175012.62764200001</v>
+        <v>112772.65829599999</v>
       </c>
       <c r="U17">
-        <v>114600.766343</v>
+        <v>114425.5048</v>
       </c>
       <c r="V17" s="18">
-        <v>510096100</v>
+        <v>452939500</v>
       </c>
       <c r="W17">
-        <v>1025.3733279999999</v>
+        <v>1181.4370489999999</v>
       </c>
       <c r="X17">
-        <v>76444.986667999998</v>
+        <v>14806.590716000001</v>
       </c>
       <c r="Y17">
-        <v>2.0501999999999999E-2</v>
+        <v>-8.7799999999999998E-4</v>
       </c>
       <c r="Z17">
-        <v>7.541E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+        <v>1.0717000000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18" s="12">
-        <v>0.65</v>
+        <v>0.68</v>
       </c>
       <c r="E18">
-        <v>3385.0576919999999</v>
+        <v>2825.5625</v>
       </c>
       <c r="F18">
-        <v>592731.926538</v>
+        <v>206296.388393</v>
       </c>
       <c r="G18">
-        <v>827.61538499999995</v>
+        <v>824.3125</v>
       </c>
       <c r="H18">
-        <v>1930.886154</v>
+        <v>1045.8526790000001</v>
       </c>
       <c r="I18">
-        <v>410.90384599999999</v>
+        <v>434.75</v>
       </c>
       <c r="J18">
-        <v>2171.8803849999999</v>
+        <v>1249.9285709999999</v>
       </c>
       <c r="K18">
-        <v>371.539221</v>
+        <v>409.11131799999998</v>
       </c>
       <c r="L18">
-        <v>1035.578855</v>
+        <v>397.60211299999997</v>
       </c>
       <c r="M18">
-        <v>1222.5497009999999</v>
+        <v>1292.983442</v>
       </c>
       <c r="N18">
-        <v>15536.642760999999</v>
+        <v>13186.836364999999</v>
       </c>
       <c r="O18">
-        <v>498.94230800000003</v>
+        <v>390.5625</v>
       </c>
       <c r="P18">
-        <v>16900.946538</v>
+        <v>6146.2455360000004</v>
       </c>
       <c r="Q18">
-        <v>1245.3258940000001</v>
+        <v>1384.809481</v>
       </c>
       <c r="R18">
-        <v>12740.419583999999</v>
+        <v>3838.774077</v>
       </c>
       <c r="S18">
-        <v>2578.3067820000001</v>
+        <v>2837.7939270000002</v>
       </c>
       <c r="T18">
-        <v>49049.371189999998</v>
+        <v>17968.547284</v>
       </c>
       <c r="U18">
-        <v>193914.33996899999</v>
+        <v>199541.78588800001</v>
       </c>
       <c r="V18" s="18">
-        <v>1004123000</v>
+        <v>1000363000</v>
       </c>
       <c r="W18">
-        <v>722.09551699999997</v>
+        <v>779.69089099999997</v>
       </c>
       <c r="X18">
-        <v>4047.1366130000001</v>
+        <v>3312.2219260000002</v>
       </c>
       <c r="Y18">
-        <v>-0.116019</v>
+        <v>-0.16553899999999999</v>
       </c>
       <c r="Z18">
-        <v>5.2220000000000001E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B19" s="3">
+        <v>1.2329999999999999E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3">
         <v>4</v>
       </c>
-      <c r="C19" s="3">
-        <v>1</v>
-      </c>
       <c r="D19" s="12">
-        <v>0.9</v>
+        <v>0.63</v>
       </c>
       <c r="E19">
-        <v>2178</v>
+        <v>3633.7222219999999</v>
       </c>
       <c r="F19">
-        <v>302642</v>
+        <v>573937.15359500004</v>
       </c>
       <c r="G19">
-        <v>654</v>
+        <v>829.08333300000004</v>
       </c>
       <c r="H19">
-        <v>10368</v>
+        <v>2401.4779410000001</v>
       </c>
       <c r="I19">
-        <v>395.5</v>
+        <v>400.30555600000002</v>
       </c>
       <c r="J19">
-        <v>1104.5</v>
+        <v>2292.7393790000001</v>
       </c>
       <c r="K19">
-        <v>229.304495</v>
+        <v>354.84051199999999</v>
       </c>
       <c r="L19">
-        <v>106.140266</v>
+        <v>399.63016699999997</v>
       </c>
       <c r="M19">
-        <v>989.65582400000005</v>
+        <v>1191.245815</v>
       </c>
       <c r="N19">
-        <v>1239.699991</v>
+        <v>14046.007121000001</v>
       </c>
       <c r="O19">
-        <v>311.5</v>
+        <v>547.11111100000005</v>
       </c>
       <c r="P19">
-        <v>7320.5</v>
+        <v>14339.19281</v>
       </c>
       <c r="Q19">
-        <v>930.86591499999997</v>
+        <v>1183.3331889999999</v>
       </c>
       <c r="R19">
-        <v>1374.7302589999999</v>
+        <v>3930.4696720000002</v>
       </c>
       <c r="S19">
-        <v>1828.920476</v>
+        <v>2462.9791620000001</v>
       </c>
       <c r="T19">
-        <v>1718.9084230000001</v>
+        <v>18963.384773000002</v>
       </c>
       <c r="U19">
-        <v>114951.28943</v>
+        <v>191413.252894</v>
       </c>
       <c r="V19" s="18">
-        <v>1191293000</v>
+        <v>1043211000</v>
       </c>
       <c r="W19">
-        <v>713.24588500000004</v>
+        <v>696.49757299999999</v>
       </c>
       <c r="X19">
-        <v>45534.539232000003</v>
+        <v>2332.9682459999999</v>
       </c>
       <c r="Y19">
-        <v>6.3261999999999999E-2</v>
+        <v>-9.4009999999999996E-2</v>
       </c>
       <c r="Z19">
-        <v>6.6000000000000005E-5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+        <v>5.5040000000000002E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
-      <c r="C20" s="3">
-        <v>2</v>
-      </c>
-      <c r="D20" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="E20">
-        <v>1520.75</v>
-      </c>
-      <c r="F20">
-        <v>5435.5833329999996</v>
-      </c>
-      <c r="G20">
-        <v>801</v>
-      </c>
-      <c r="H20">
-        <v>11318.666667</v>
-      </c>
-      <c r="I20">
-        <v>451.25</v>
-      </c>
-      <c r="J20">
-        <v>2901.583333</v>
-      </c>
-      <c r="K20">
-        <v>346.94201199999998</v>
-      </c>
-      <c r="L20">
-        <v>1965.059966</v>
-      </c>
-      <c r="M20">
-        <v>1174.1113760000001</v>
-      </c>
-      <c r="N20">
-        <v>46224.634835999997</v>
-      </c>
-      <c r="O20">
-        <v>218.75</v>
-      </c>
-      <c r="P20">
-        <v>1104.25</v>
-      </c>
-      <c r="Q20">
-        <v>1351.174248</v>
-      </c>
-      <c r="R20">
-        <v>40856.737567999997</v>
-      </c>
-      <c r="S20">
-        <v>2462.378991</v>
-      </c>
-      <c r="T20">
-        <v>112772.65829599999</v>
-      </c>
-      <c r="U20">
-        <v>114425.5048</v>
-      </c>
-      <c r="V20" s="18">
-        <v>452939500</v>
-      </c>
-      <c r="W20">
-        <v>1181.4370489999999</v>
-      </c>
-      <c r="X20">
-        <v>14806.590716000001</v>
-      </c>
-      <c r="Y20">
-        <v>-8.7799999999999998E-4</v>
-      </c>
-      <c r="Z20">
-        <v>1.0717000000000001E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
-      <c r="C21" s="3">
-        <v>3</v>
-      </c>
-      <c r="D21" s="12">
-        <v>0.68</v>
-      </c>
-      <c r="E21">
-        <v>2825.5625</v>
-      </c>
-      <c r="F21">
-        <v>206296.388393</v>
-      </c>
-      <c r="G21">
-        <v>824.3125</v>
-      </c>
-      <c r="H21">
-        <v>1045.8526790000001</v>
-      </c>
-      <c r="I21">
-        <v>434.75</v>
-      </c>
-      <c r="J21">
-        <v>1249.9285709999999</v>
-      </c>
-      <c r="K21">
-        <v>409.11131799999998</v>
-      </c>
-      <c r="L21">
-        <v>397.60211299999997</v>
-      </c>
-      <c r="M21">
-        <v>1292.983442</v>
-      </c>
-      <c r="N21">
-        <v>13186.836364999999</v>
-      </c>
-      <c r="O21">
-        <v>390.5625</v>
-      </c>
-      <c r="P21">
-        <v>6146.2455360000004</v>
-      </c>
-      <c r="Q21">
-        <v>1384.809481</v>
-      </c>
-      <c r="R21">
-        <v>3838.774077</v>
-      </c>
-      <c r="S21">
-        <v>2837.7939270000002</v>
-      </c>
-      <c r="T21">
-        <v>17968.547284</v>
-      </c>
-      <c r="U21">
-        <v>199541.78588800001</v>
-      </c>
-      <c r="V21" s="18">
-        <v>1000363000</v>
-      </c>
-      <c r="W21">
-        <v>779.69089099999997</v>
-      </c>
-      <c r="X21">
-        <v>3312.2219260000002</v>
-      </c>
-      <c r="Y21">
-        <v>-0.16553899999999999</v>
-      </c>
-      <c r="Z21">
-        <v>1.2329999999999999E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
-      <c r="C22" s="3">
-        <v>4</v>
-      </c>
-      <c r="D22" s="12">
-        <v>0.63</v>
-      </c>
-      <c r="E22">
-        <v>3633.7222219999999</v>
-      </c>
-      <c r="F22">
-        <v>573937.15359500004</v>
-      </c>
-      <c r="G22">
-        <v>829.08333300000004</v>
-      </c>
-      <c r="H22">
-        <v>2401.4779410000001</v>
-      </c>
-      <c r="I22">
-        <v>400.30555600000002</v>
-      </c>
-      <c r="J22">
-        <v>2292.7393790000001</v>
-      </c>
-      <c r="K22">
-        <v>354.84051199999999</v>
-      </c>
-      <c r="L22">
-        <v>399.63016699999997</v>
-      </c>
-      <c r="M22">
-        <v>1191.245815</v>
-      </c>
-      <c r="N22">
-        <v>14046.007121000001</v>
-      </c>
-      <c r="O22">
-        <v>547.11111100000005</v>
-      </c>
-      <c r="P22">
-        <v>14339.19281</v>
-      </c>
-      <c r="Q22">
-        <v>1183.3331889999999</v>
-      </c>
-      <c r="R22">
-        <v>3930.4696720000002</v>
-      </c>
-      <c r="S22">
-        <v>2462.9791620000001</v>
-      </c>
-      <c r="T22">
-        <v>18963.384773000002</v>
-      </c>
-      <c r="U22">
-        <v>191413.252894</v>
-      </c>
-      <c r="V22" s="18">
-        <v>1043211000</v>
-      </c>
-      <c r="W22">
-        <v>696.49757299999999</v>
-      </c>
-      <c r="X22">
-        <v>2332.9682459999999</v>
-      </c>
-      <c r="Y22">
-        <v>-9.4009999999999996E-2</v>
-      </c>
-      <c r="Z22">
-        <v>5.5040000000000002E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="5"/>
+      <c r="D26" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
     <mergeCell ref="Y1:Z1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="W1:X1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[add] added updated result files
</commit_message>
<xml_diff>
--- a/Experiment-Data/Answer-Data.xlsx
+++ b/Experiment-Data/Answer-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\www\Desktop\eye-tracking-software\Experiment-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A27A6608-FD1C-455B-85CE-6C48855A7FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E956E7-4010-409F-A437-DDBF143504AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{65F65776-174E-4145-8CCF-AA6B8A50F68A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="30">
   <si>
     <t>English</t>
   </si>
@@ -122,19 +122,10 @@
     <t xml:space="preserve">注視時間(ms) </t>
   </si>
   <si>
-    <t xml:space="preserve">平均注視x座標 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 平均注視y座標</t>
-  </si>
-  <si>
     <t>サッケード数</t>
   </si>
   <si>
     <t>平均速度</t>
-  </si>
-  <si>
-    <t>速度の標準偏差</t>
   </si>
   <si>
     <t>平均視線回転(rad)</t>
@@ -171,6 +162,9 @@
   <si>
     <t>クラスタ
 数</t>
+  </si>
+  <si>
+    <t>正答率</t>
   </si>
 </sst>
 </file>
@@ -310,7 +304,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -649,9 +643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C853D4-11AD-448C-900A-323815755F36}">
   <dimension ref="A1:AW39"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB38" sqref="AB38"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -683,7 +675,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>14</v>
@@ -956,8 +948,8 @@
       <c r="AD3" s="3">
         <v>1</v>
       </c>
-      <c r="AE3">
-        <v>1</v>
+      <c r="AE3" s="3">
+        <v>2</v>
       </c>
       <c r="AF3" s="12">
         <f>(COUNTIF(AG3:AP3,"○")/10)</f>
@@ -994,7 +986,7 @@
         <v>12</v>
       </c>
       <c r="AR3" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AS3" s="3" t="s">
         <v>1</v>
@@ -1021,7 +1013,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4" s="12">
         <f t="shared" ref="F4:F30" si="0">COUNTIF(G4:Z4,"○")/20</f>
@@ -1090,8 +1082,8 @@
       <c r="AD4" s="3">
         <v>2</v>
       </c>
-      <c r="AE4">
-        <v>2</v>
+      <c r="AE4" s="3">
+        <v>1</v>
       </c>
       <c r="AF4" s="12">
         <f t="shared" ref="AF4:AF36" si="1">(COUNTIF(AG4:AP4,"○")/10)</f>
@@ -1247,7 +1239,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" s="12">
         <f t="shared" si="0"/>
@@ -1319,8 +1311,8 @@
       <c r="AD6" s="3">
         <v>1</v>
       </c>
-      <c r="AE6">
-        <v>2</v>
+      <c r="AE6" s="3">
+        <v>1</v>
       </c>
       <c r="AF6" s="12">
         <f t="shared" si="1"/>
@@ -1369,7 +1361,7 @@
         <v>3</v>
       </c>
       <c r="AW6" s="12">
-        <f>(F6+AF6)/2</f>
+        <f t="shared" ref="AW6:AW15" si="3">(F6+AF6)/2</f>
         <v>0.85</v>
       </c>
     </row>
@@ -1381,7 +1373,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F7" s="12">
         <f t="shared" si="0"/>
@@ -1450,8 +1442,8 @@
       <c r="AD7" s="3">
         <v>2</v>
       </c>
-      <c r="AE7">
-        <v>3</v>
+      <c r="AE7" s="3">
+        <v>1</v>
       </c>
       <c r="AF7" s="12">
         <f t="shared" si="1"/>
@@ -1497,7 +1489,7 @@
         <v>4</v>
       </c>
       <c r="AW7" s="12">
-        <f>(F7+AF7)/2</f>
+        <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
     </row>
@@ -1509,7 +1501,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F8" s="12">
         <f t="shared" si="0"/>
@@ -1578,8 +1570,8 @@
       <c r="AD8" s="3">
         <v>3</v>
       </c>
-      <c r="AE8">
-        <v>1</v>
+      <c r="AE8" s="3">
+        <v>2</v>
       </c>
       <c r="AF8" s="12">
         <f t="shared" si="1"/>
@@ -1625,7 +1617,7 @@
         <v>3</v>
       </c>
       <c r="AW8" s="12">
-        <f>(F8+AF8)/2</f>
+        <f t="shared" si="3"/>
         <v>0.875</v>
       </c>
     </row>
@@ -1637,7 +1629,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F9" s="12">
         <f t="shared" si="0"/>
@@ -1706,8 +1698,8 @@
       <c r="AD9" s="3">
         <v>4</v>
       </c>
-      <c r="AE9">
-        <v>1</v>
+      <c r="AE9" s="3">
+        <v>2</v>
       </c>
       <c r="AF9" s="12">
         <f t="shared" si="1"/>
@@ -1753,7 +1745,7 @@
         <v>3</v>
       </c>
       <c r="AW9" s="12">
-        <f>(F9+AF9)/2</f>
+        <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
     </row>
@@ -1765,7 +1757,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F10" s="12">
         <f t="shared" si="0"/>
@@ -1834,8 +1826,8 @@
       <c r="AD10" s="3">
         <v>5</v>
       </c>
-      <c r="AE10">
-        <v>2</v>
+      <c r="AE10" s="3">
+        <v>1</v>
       </c>
       <c r="AF10" s="12">
         <f t="shared" si="1"/>
@@ -1881,7 +1873,7 @@
         <v>4</v>
       </c>
       <c r="AW10" s="12">
-        <f>(F10+AF10)/2</f>
+        <f t="shared" si="3"/>
         <v>0.57499999999999996</v>
       </c>
     </row>
@@ -1893,7 +1885,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F11" s="12">
         <f t="shared" si="0"/>
@@ -1962,8 +1954,8 @@
       <c r="AD11" s="3">
         <v>6</v>
       </c>
-      <c r="AE11">
-        <v>2</v>
+      <c r="AE11" s="3">
+        <v>1</v>
       </c>
       <c r="AF11" s="12">
         <f t="shared" si="1"/>
@@ -2009,7 +2001,7 @@
         <v>4</v>
       </c>
       <c r="AW11" s="12">
-        <f>(F11+AF11)/2</f>
+        <f t="shared" si="3"/>
         <v>0.82499999999999996</v>
       </c>
     </row>
@@ -2018,10 +2010,10 @@
         <v>7</v>
       </c>
       <c r="D12" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F12" s="12">
         <f t="shared" si="0"/>
@@ -2090,8 +2082,8 @@
       <c r="AD12" s="3">
         <v>7</v>
       </c>
-      <c r="AE12">
-        <v>3</v>
+      <c r="AE12" s="3">
+        <v>1</v>
       </c>
       <c r="AF12" s="12">
         <f t="shared" si="1"/>
@@ -2134,10 +2126,10 @@
         <v>2</v>
       </c>
       <c r="AV12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AW12" s="12">
-        <f>(F12+AF12)/2</f>
+        <f t="shared" si="3"/>
         <v>0.67500000000000004</v>
       </c>
     </row>
@@ -2146,10 +2138,10 @@
         <v>8</v>
       </c>
       <c r="D13" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" s="12">
         <f t="shared" si="0"/>
@@ -2218,7 +2210,7 @@
       <c r="AD13" s="3">
         <v>8</v>
       </c>
-      <c r="AE13">
+      <c r="AE13" s="3">
         <v>3</v>
       </c>
       <c r="AF13" s="12">
@@ -2262,10 +2254,10 @@
         <v>2</v>
       </c>
       <c r="AV13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AW13" s="12">
-        <f>(F13+AF13)/2</f>
+        <f t="shared" si="3"/>
         <v>0.82499999999999996</v>
       </c>
     </row>
@@ -2274,10 +2266,10 @@
         <v>9</v>
       </c>
       <c r="D14" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F14" s="12">
         <f t="shared" si="0"/>
@@ -2346,8 +2338,8 @@
       <c r="AD14" s="3">
         <v>9</v>
       </c>
-      <c r="AE14">
-        <v>2</v>
+      <c r="AE14" s="3">
+        <v>1</v>
       </c>
       <c r="AF14" s="12">
         <f t="shared" si="1"/>
@@ -2390,10 +2382,10 @@
         <v>2</v>
       </c>
       <c r="AV14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AW14" s="12">
-        <f>(F14+AF14)/2</f>
+        <f t="shared" si="3"/>
         <v>0.72500000000000009</v>
       </c>
     </row>
@@ -2402,10 +2394,10 @@
         <v>10</v>
       </c>
       <c r="D15" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F15" s="12">
         <f t="shared" si="0"/>
@@ -2474,8 +2466,8 @@
       <c r="AD15" s="3">
         <v>10</v>
       </c>
-      <c r="AE15">
-        <v>3</v>
+      <c r="AE15" s="3">
+        <v>1</v>
       </c>
       <c r="AF15" s="12">
         <f t="shared" si="1"/>
@@ -2518,10 +2510,10 @@
         <v>2</v>
       </c>
       <c r="AV15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AW15" s="12">
-        <f>(F15+AF15)/2</f>
+        <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
     </row>
@@ -2532,79 +2524,79 @@
         <v>0.6</v>
       </c>
       <c r="H16" s="16">
-        <f t="shared" ref="H16:Z16" si="3">(COUNTIF(H6:H15,"○"))/10</f>
+        <f t="shared" ref="H16:Z16" si="4">(COUNTIF(H6:H15,"○"))/10</f>
         <v>0.4</v>
       </c>
       <c r="I16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
       <c r="J16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
       <c r="K16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
       <c r="M16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="N16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="O16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
       <c r="P16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
       <c r="Q16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="R16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.9</v>
       </c>
       <c r="S16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
       <c r="T16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.9</v>
       </c>
       <c r="U16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
       <c r="V16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
       <c r="W16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="X16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.9</v>
       </c>
       <c r="Y16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
       <c r="Z16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.9</v>
       </c>
       <c r="AF16" s="12"/>
@@ -2631,7 +2623,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F17" s="12">
         <f t="shared" si="0"/>
@@ -2703,8 +2695,8 @@
       <c r="AD17" s="3">
         <v>1</v>
       </c>
-      <c r="AE17">
-        <v>2</v>
+      <c r="AE17" s="3">
+        <v>1</v>
       </c>
       <c r="AF17" s="12">
         <f t="shared" si="1"/>
@@ -2753,7 +2745,7 @@
         <v>4</v>
       </c>
       <c r="AW17" s="12">
-        <f>(F17+AF17)/2</f>
+        <f t="shared" ref="AW17:AW30" si="5">(F17+AF17)/2</f>
         <v>0.5</v>
       </c>
     </row>
@@ -2765,7 +2757,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F18" s="12">
         <f t="shared" si="0"/>
@@ -2834,7 +2826,7 @@
       <c r="AD18" s="3">
         <v>2</v>
       </c>
-      <c r="AE18">
+      <c r="AE18" s="3">
         <v>3</v>
       </c>
       <c r="AF18" s="12">
@@ -2881,7 +2873,7 @@
         <v>4</v>
       </c>
       <c r="AW18" s="12">
-        <f>(F18+AF18)/2</f>
+        <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
     </row>
@@ -2962,7 +2954,7 @@
       <c r="AD19" s="3">
         <v>3</v>
       </c>
-      <c r="AE19">
+      <c r="AE19" s="3">
         <v>3</v>
       </c>
       <c r="AF19" s="12">
@@ -3009,7 +3001,7 @@
         <v>3</v>
       </c>
       <c r="AW19" s="12">
-        <f>(F19+AF19)/2</f>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3018,10 +3010,10 @@
         <v>4</v>
       </c>
       <c r="D20" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F20" s="12">
         <f t="shared" si="0"/>
@@ -3090,7 +3082,7 @@
       <c r="AD20" s="3">
         <v>4</v>
       </c>
-      <c r="AE20">
+      <c r="AE20" s="3">
         <v>3</v>
       </c>
       <c r="AF20" s="12">
@@ -3137,7 +3129,7 @@
         <v>4</v>
       </c>
       <c r="AW20" s="12">
-        <f>(F20+AF20)/2</f>
+        <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
     </row>
@@ -3218,8 +3210,8 @@
       <c r="AD21" s="3">
         <v>5</v>
       </c>
-      <c r="AE21">
-        <v>1</v>
+      <c r="AE21" s="3">
+        <v>2</v>
       </c>
       <c r="AF21" s="12">
         <f t="shared" si="1"/>
@@ -3265,7 +3257,7 @@
         <v>3</v>
       </c>
       <c r="AW21" s="12">
-        <f>(F21+AF21)/2</f>
+        <f t="shared" si="5"/>
         <v>0.57499999999999996</v>
       </c>
     </row>
@@ -3277,7 +3269,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F22" s="12">
         <f t="shared" si="0"/>
@@ -3346,7 +3338,7 @@
       <c r="AD22" s="3">
         <v>6</v>
       </c>
-      <c r="AE22">
+      <c r="AE22" s="3">
         <v>3</v>
       </c>
       <c r="AF22" s="12">
@@ -3393,7 +3385,7 @@
         <v>4</v>
       </c>
       <c r="AW22" s="12">
-        <f>(F22+AF22)/2</f>
+        <f t="shared" si="5"/>
         <v>0.55000000000000004</v>
       </c>
     </row>
@@ -3474,8 +3466,8 @@
       <c r="AD23" s="3">
         <v>7</v>
       </c>
-      <c r="AE23">
-        <v>1</v>
+      <c r="AE23" s="3">
+        <v>3</v>
       </c>
       <c r="AF23" s="12">
         <f t="shared" si="1"/>
@@ -3521,7 +3513,7 @@
         <v>3</v>
       </c>
       <c r="AW23" s="12">
-        <f>(F23+AF23)/2</f>
+        <f t="shared" si="5"/>
         <v>0.625</v>
       </c>
     </row>
@@ -3533,7 +3525,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F24" s="12">
         <f t="shared" si="0"/>
@@ -3602,7 +3594,7 @@
       <c r="AD24" s="3">
         <v>8</v>
       </c>
-      <c r="AE24">
+      <c r="AE24" s="3">
         <v>3</v>
       </c>
       <c r="AF24" s="12">
@@ -3646,10 +3638,10 @@
         <v>2</v>
       </c>
       <c r="AV24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AW24" s="12">
-        <f>(F24+AF24)/2</f>
+        <f t="shared" si="5"/>
         <v>0.625</v>
       </c>
     </row>
@@ -3658,10 +3650,10 @@
         <v>9</v>
       </c>
       <c r="D25" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F25" s="12">
         <f t="shared" si="0"/>
@@ -3730,7 +3722,7 @@
       <c r="AD25" s="3">
         <v>9</v>
       </c>
-      <c r="AE25">
+      <c r="AE25" s="3">
         <v>3</v>
       </c>
       <c r="AF25" s="12">
@@ -3774,10 +3766,10 @@
         <v>2</v>
       </c>
       <c r="AV25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AW25" s="12">
-        <f>(F25+AF25)/2</f>
+        <f t="shared" si="5"/>
         <v>0.55000000000000004</v>
       </c>
     </row>
@@ -3858,8 +3850,8 @@
       <c r="AD26" s="3">
         <v>10</v>
       </c>
-      <c r="AE26">
-        <v>2</v>
+      <c r="AE26" s="3">
+        <v>1</v>
       </c>
       <c r="AF26" s="12">
         <f t="shared" si="1"/>
@@ -3905,7 +3897,7 @@
         <v>3</v>
       </c>
       <c r="AW26" s="12">
-        <f>(F26+AF26)/2</f>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3917,7 +3909,7 @@
         <v>2</v>
       </c>
       <c r="E27" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F27" s="12">
         <f t="shared" si="0"/>
@@ -3986,8 +3978,8 @@
       <c r="AD27" s="3">
         <v>11</v>
       </c>
-      <c r="AE27">
-        <v>1</v>
+      <c r="AE27" s="3">
+        <v>3</v>
       </c>
       <c r="AF27" s="12">
         <f t="shared" si="1"/>
@@ -4033,7 +4025,7 @@
         <v>4</v>
       </c>
       <c r="AW27" s="12">
-        <f>(F27+AF27)/2</f>
+        <f t="shared" si="5"/>
         <v>0.52500000000000002</v>
       </c>
     </row>
@@ -4114,8 +4106,8 @@
       <c r="AD28" s="3">
         <v>12</v>
       </c>
-      <c r="AE28">
-        <v>1</v>
+      <c r="AE28" s="3">
+        <v>3</v>
       </c>
       <c r="AF28" s="12">
         <f t="shared" si="1"/>
@@ -4161,7 +4153,7 @@
         <v>4</v>
       </c>
       <c r="AW28" s="12">
-        <f>(F28+AF28)/2</f>
+        <f t="shared" si="5"/>
         <v>0.57499999999999996</v>
       </c>
     </row>
@@ -4173,7 +4165,7 @@
         <v>2</v>
       </c>
       <c r="E29" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F29" s="12">
         <f t="shared" si="0"/>
@@ -4242,8 +4234,8 @@
       <c r="AD29" s="3">
         <v>13</v>
       </c>
-      <c r="AE29">
-        <v>1</v>
+      <c r="AE29" s="3">
+        <v>2</v>
       </c>
       <c r="AF29" s="12">
         <f t="shared" si="1"/>
@@ -4289,7 +4281,7 @@
         <v>4</v>
       </c>
       <c r="AW29" s="12">
-        <f>(F29+AF29)/2</f>
+        <f t="shared" si="5"/>
         <v>0.39999999999999997</v>
       </c>
     </row>
@@ -4301,7 +4293,7 @@
         <v>2</v>
       </c>
       <c r="E30" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F30" s="12">
         <f t="shared" si="0"/>
@@ -4370,8 +4362,8 @@
       <c r="AD30" s="3">
         <v>14</v>
       </c>
-      <c r="AE30">
-        <v>1</v>
+      <c r="AE30" s="3">
+        <v>2</v>
       </c>
       <c r="AF30" s="12">
         <f t="shared" si="1"/>
@@ -4417,7 +4409,7 @@
         <v>4</v>
       </c>
       <c r="AW30" s="12">
-        <f>(F30+AF30)/2</f>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
     </row>
@@ -4428,43 +4420,43 @@
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="H31" s="15">
-        <f t="shared" ref="H31:Z31" si="4">(COUNTIF(H17:H30,"○"))/14</f>
+        <f t="shared" ref="H31:Z31" si="6">(COUNTIF(H17:H30,"○"))/14</f>
         <v>0.14285714285714285</v>
       </c>
       <c r="I31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.42857142857142855</v>
       </c>
       <c r="J31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="K31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.35714285714285715</v>
       </c>
       <c r="L31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="M31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.35714285714285715</v>
       </c>
       <c r="N31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="O31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="R31" s="15">
@@ -4472,35 +4464,35 @@
         <v>0</v>
       </c>
       <c r="S31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="W31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="X31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.35714285714285715</v>
       </c>
       <c r="Y31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.7857142857142857</v>
       </c>
       <c r="Z31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="AC31" s="3" t="s">
@@ -4509,8 +4501,8 @@
       <c r="AD31" s="3">
         <v>1</v>
       </c>
-      <c r="AE31">
-        <v>1</v>
+      <c r="AE31" s="3">
+        <v>2</v>
       </c>
       <c r="AF31" s="12">
         <f t="shared" si="1"/>
@@ -4556,7 +4548,7 @@
         <v>1</v>
       </c>
       <c r="AV31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW31" s="12">
         <f>AF31</f>
@@ -4568,8 +4560,8 @@
       <c r="AD32" s="3">
         <v>2</v>
       </c>
-      <c r="AE32">
-        <v>1</v>
+      <c r="AE32" s="3">
+        <v>3</v>
       </c>
       <c r="AF32" s="12">
         <f t="shared" si="1"/>
@@ -4615,7 +4607,7 @@
         <v>2</v>
       </c>
       <c r="AW32" s="12">
-        <f t="shared" ref="AW32:AW36" si="5">AF32</f>
+        <f t="shared" ref="AW32:AW36" si="7">AF32</f>
         <v>0.8</v>
       </c>
     </row>
@@ -4626,7 +4618,7 @@
       <c r="AD33" s="3">
         <v>1</v>
       </c>
-      <c r="AE33">
+      <c r="AE33" s="3">
         <v>3</v>
       </c>
       <c r="AF33" s="12">
@@ -4676,7 +4668,7 @@
         <v>2</v>
       </c>
       <c r="AW33" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -4684,8 +4676,8 @@
       <c r="AD34" s="3">
         <v>2</v>
       </c>
-      <c r="AE34">
-        <v>1</v>
+      <c r="AE34" s="3">
+        <v>2</v>
       </c>
       <c r="AF34" s="12">
         <f t="shared" si="1"/>
@@ -4728,10 +4720,10 @@
         <v>1</v>
       </c>
       <c r="AV34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW34" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.9</v>
       </c>
     </row>
@@ -4739,8 +4731,8 @@
       <c r="AD35" s="3">
         <v>3</v>
       </c>
-      <c r="AE35">
-        <v>2</v>
+      <c r="AE35" s="3">
+        <v>1</v>
       </c>
       <c r="AF35" s="12">
         <f t="shared" si="1"/>
@@ -4783,10 +4775,10 @@
         <v>1</v>
       </c>
       <c r="AV35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AW35" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.8</v>
       </c>
     </row>
@@ -4797,7 +4789,7 @@
       <c r="AD36" s="3">
         <v>1</v>
       </c>
-      <c r="AE36">
+      <c r="AE36" s="3">
         <v>3</v>
       </c>
       <c r="AF36" s="12">
@@ -4844,10 +4836,10 @@
         <v>1</v>
       </c>
       <c r="AV36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AW36" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -4857,43 +4849,47 @@
         <v>1</v>
       </c>
       <c r="AH37" s="15">
-        <f t="shared" ref="AH37:AP37" si="6">(COUNTIF(AH3:AH36,"○")/32)</f>
+        <f t="shared" ref="AH37:AP37" si="8">(COUNTIF(AH3:AH36,"○")/32)</f>
         <v>0.9375</v>
       </c>
       <c r="AI37" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.9375</v>
       </c>
       <c r="AJ37" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.96875</v>
       </c>
       <c r="AK37" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.59375</v>
       </c>
       <c r="AL37" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.875</v>
       </c>
       <c r="AM37" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.5625</v>
       </c>
       <c r="AN37" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AO37" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.875</v>
       </c>
       <c r="AP37" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.9375</v>
       </c>
+      <c r="AU37"/>
+      <c r="AV37"/>
     </row>
     <row r="38" spans="29:49" x14ac:dyDescent="0.25">
+      <c r="AU38"/>
+      <c r="AV38"/>
       <c r="AW38" s="12"/>
     </row>
     <row r="39" spans="29:49" x14ac:dyDescent="0.25">
@@ -4912,148 +4908,121 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88CCFB4E-3D94-4A97-83BE-04827B31FA43}">
-  <dimension ref="A1:Z26"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" style="3" customWidth="1"/>
     <col min="2" max="3" width="8.5703125" customWidth="1"/>
     <col min="4" max="4" width="5.7109375" style="3" customWidth="1"/>
-    <col min="5" max="27" width="10" customWidth="1"/>
+    <col min="5" max="21" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="21"/>
       <c r="G1" s="21" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H1" s="21"/>
       <c r="I1" s="21" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="21" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="L1" s="21"/>
       <c r="M1" s="21" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="N1" s="21"/>
       <c r="O1" s="21" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="P1" s="21"/>
       <c r="Q1" s="21" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="R1" s="21"/>
       <c r="S1" s="21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="T1" s="21"/>
-      <c r="U1" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z1" s="21"/>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>23</v>
-      </c>
-      <c r="R2" t="s">
-        <v>24</v>
-      </c>
-      <c r="S2" t="s">
-        <v>23</v>
-      </c>
-      <c r="T2" t="s">
-        <v>24</v>
-      </c>
-      <c r="U2" t="s">
-        <v>23</v>
-      </c>
-      <c r="V2" t="s">
-        <v>24</v>
-      </c>
-      <c r="W2" t="s">
-        <v>23</v>
-      </c>
-      <c r="X2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -5064,1191 +5033,975 @@
         <v>1</v>
       </c>
       <c r="D3" s="12">
-        <v>0.45</v>
+        <v>0.52</v>
       </c>
       <c r="E3">
-        <v>3965.9</v>
+        <v>4115.8571430000002</v>
       </c>
       <c r="F3" s="18">
-        <v>1252931</v>
+        <v>936546.9</v>
       </c>
       <c r="G3">
-        <v>851.8</v>
+        <v>242.50248099999999</v>
       </c>
       <c r="H3">
-        <v>3703.9555559999999</v>
+        <v>3546.0511310000002</v>
       </c>
       <c r="I3">
-        <v>508.2</v>
+        <v>1140.055169</v>
       </c>
       <c r="J3">
-        <v>5359.2888890000004</v>
+        <v>44413.767576999999</v>
       </c>
       <c r="K3">
-        <v>270.64907799999997</v>
+        <v>637.14285700000005</v>
       </c>
       <c r="L3">
-        <v>1909.3490609999999</v>
+        <v>31479.516484</v>
       </c>
       <c r="M3">
-        <v>1155.758601</v>
+        <v>983.46531900000002</v>
       </c>
       <c r="N3">
-        <v>52776.063038</v>
+        <v>44613.387073999998</v>
       </c>
       <c r="O3">
-        <v>602.29999999999995</v>
-      </c>
-      <c r="P3">
-        <v>30431.122222000002</v>
+        <v>218988.75994300001</v>
+      </c>
+      <c r="P3" s="18">
+        <v>3097454000</v>
       </c>
       <c r="Q3">
-        <v>1098.5083360000001</v>
+        <v>474.34010899999998</v>
       </c>
       <c r="R3">
-        <v>19029.524135</v>
+        <v>13002.227987</v>
       </c>
       <c r="S3">
-        <v>2009.786785</v>
+        <v>-8.9724999999999999E-2</v>
       </c>
       <c r="T3">
-        <v>113430.540313</v>
-      </c>
-      <c r="U3">
-        <v>239607.33085</v>
-      </c>
-      <c r="V3" s="18">
-        <v>5305183000</v>
-      </c>
-      <c r="W3">
-        <v>504.957266</v>
-      </c>
-      <c r="X3">
-        <v>14337.141594999999</v>
-      </c>
-      <c r="Y3">
-        <v>-6.7067000000000002E-2</v>
-      </c>
-      <c r="Z3">
-        <v>8.8509999999999995E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+        <v>7.7279999999999996E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3">
         <v>2</v>
       </c>
       <c r="D4" s="12">
-        <v>0.42</v>
+        <v>0.33</v>
       </c>
       <c r="E4">
-        <v>5542.5</v>
+        <v>5893.0833329999996</v>
       </c>
       <c r="F4" s="18">
-        <v>2180026</v>
+        <v>2426282</v>
       </c>
       <c r="G4">
-        <v>870.375</v>
+        <v>162.79395500000001</v>
       </c>
       <c r="H4">
-        <v>10508.65</v>
+        <v>1491.469531</v>
       </c>
       <c r="I4">
-        <v>455.5625</v>
+        <v>971.40089599999999</v>
       </c>
       <c r="J4">
-        <v>10126.929167</v>
+        <v>72044.690277999995</v>
       </c>
       <c r="K4">
-        <v>165.12946299999999</v>
+        <v>978.91666699999996</v>
       </c>
       <c r="L4">
-        <v>1190.295079</v>
+        <v>47826.628788000002</v>
       </c>
       <c r="M4">
-        <v>1003.749819</v>
+        <v>703.63727300000005</v>
       </c>
       <c r="N4">
-        <v>62432.321122000001</v>
+        <v>17100.484279</v>
       </c>
       <c r="O4">
-        <v>915.25</v>
-      </c>
-      <c r="P4">
-        <v>54234.733332999996</v>
+        <v>234286.59085800001</v>
+      </c>
+      <c r="P4" s="18">
+        <v>5330295000</v>
       </c>
       <c r="Q4">
-        <v>701.69239800000003</v>
+        <v>318.52510999999998</v>
       </c>
       <c r="R4">
-        <v>8918.2566079999997</v>
+        <v>7164.4943400000002</v>
       </c>
       <c r="S4">
-        <v>1319.6715690000001</v>
+        <v>0.10261199999999999</v>
       </c>
       <c r="T4">
-        <v>63549.171466</v>
-      </c>
-      <c r="U4">
-        <v>217575.52631300001</v>
-      </c>
-      <c r="V4" s="18">
-        <v>3311904000</v>
-      </c>
-      <c r="W4">
-        <v>338.34313700000001</v>
-      </c>
-      <c r="X4">
-        <v>6989.7978839999996</v>
-      </c>
-      <c r="Y4">
-        <v>4.0367E-2</v>
-      </c>
-      <c r="Z4">
-        <v>2.4764999999999999E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+        <v>1.6605000000000002E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
       </c>
       <c r="D5" s="12">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
       <c r="E5">
-        <v>4848.3999999999996</v>
+        <v>4540.5</v>
       </c>
       <c r="F5" s="18">
-        <v>648161.30000000005</v>
+        <v>232199</v>
       </c>
       <c r="G5">
-        <v>814</v>
+        <v>304.34769</v>
       </c>
       <c r="H5">
-        <v>1980.5</v>
+        <v>1301.720761</v>
       </c>
       <c r="I5">
-        <v>490.6</v>
+        <v>1284.720399</v>
       </c>
       <c r="J5">
-        <v>2990.3</v>
+        <v>7237.9947759999995</v>
       </c>
       <c r="K5">
-        <v>295.57636200000002</v>
+        <v>670</v>
       </c>
       <c r="L5">
-        <v>1360.9715779999999</v>
+        <v>17562</v>
       </c>
       <c r="M5">
-        <v>1239.0536729999999</v>
+        <v>1184.946228</v>
       </c>
       <c r="N5">
-        <v>15855.745697</v>
+        <v>16789.575968000001</v>
       </c>
       <c r="O5">
-        <v>715.4</v>
-      </c>
-      <c r="P5">
-        <v>23477.3</v>
+        <v>292023.93030000001</v>
+      </c>
+      <c r="P5" s="18">
+        <v>352503200</v>
       </c>
       <c r="Q5">
-        <v>1157.398512</v>
+        <v>428.31832700000001</v>
       </c>
       <c r="R5">
-        <v>16386.565287000001</v>
+        <v>2947.9414470000002</v>
       </c>
       <c r="S5">
-        <v>2180.8117929999999</v>
+        <v>-0.13603100000000001</v>
       </c>
       <c r="T5">
-        <v>38054.472474000002</v>
-      </c>
-      <c r="U5">
-        <v>303143.85025999998</v>
-      </c>
-      <c r="V5" s="18">
-        <v>882640500</v>
-      </c>
-      <c r="W5">
-        <v>409.072227</v>
-      </c>
-      <c r="X5">
-        <v>4063.017824</v>
-      </c>
-      <c r="Y5">
-        <v>-0.101822</v>
-      </c>
-      <c r="Z5">
-        <v>1.1126E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+        <v>7.0330000000000002E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="3">
         <v>2</v>
       </c>
       <c r="D6" s="12">
-        <v>0.63</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E6">
-        <v>3083.4</v>
+        <v>4658</v>
       </c>
       <c r="F6" s="18">
-        <v>223918.3</v>
+        <v>562532.4</v>
       </c>
       <c r="G6">
-        <v>889.6</v>
+        <v>197.15180699999999</v>
       </c>
       <c r="H6">
-        <v>2781.3</v>
+        <v>1810.023921</v>
       </c>
       <c r="I6">
-        <v>525.79999999999995</v>
+        <v>1075.9517760000001</v>
       </c>
       <c r="J6">
-        <v>8293.7000000000007</v>
+        <v>20597.129810999999</v>
       </c>
       <c r="K6">
-        <v>245.72179499999999</v>
+        <v>741.33333300000004</v>
       </c>
       <c r="L6">
-        <v>1381.640138</v>
+        <v>25177.866666999998</v>
       </c>
       <c r="M6">
-        <v>1072.4635290000001</v>
+        <v>809.86246200000005</v>
       </c>
       <c r="N6">
-        <v>85545.223685999998</v>
+        <v>20325.219766999999</v>
       </c>
       <c r="O6">
-        <v>489.2</v>
-      </c>
-      <c r="P6">
-        <v>13013.7</v>
+        <v>207619.90669999999</v>
+      </c>
+      <c r="P6" s="18">
+        <v>825517800</v>
       </c>
       <c r="Q6">
-        <v>1039.6181590000001</v>
+        <v>407.97479700000002</v>
       </c>
       <c r="R6">
-        <v>17759.731789000001</v>
+        <v>5390.6843959999997</v>
       </c>
       <c r="S6">
-        <v>1838.7617769999999</v>
+        <v>-0.10356</v>
       </c>
       <c r="T6">
-        <v>144040.35956899999</v>
-      </c>
-      <c r="U6">
-        <v>176070.81143999999</v>
-      </c>
-      <c r="V6" s="18">
-        <v>961799000</v>
-      </c>
-      <c r="W6">
-        <v>600.84230400000001</v>
-      </c>
-      <c r="X6">
-        <v>5210.6991820000003</v>
-      </c>
-      <c r="Y6">
-        <v>-3.2313000000000001E-2</v>
-      </c>
-      <c r="Z6">
-        <v>5.7679999999999997E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+        <v>6.0879999999999997E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="3">
         <v>3</v>
       </c>
       <c r="D7" s="12">
-        <v>0.38</v>
+        <v>0.73</v>
       </c>
       <c r="E7">
-        <v>4675.8571430000002</v>
+        <v>2878</v>
       </c>
       <c r="F7" s="18">
-        <v>671024.1</v>
+        <v>17296.669999999998</v>
       </c>
       <c r="G7">
-        <v>813.71428600000002</v>
+        <v>248.68328299999999</v>
       </c>
       <c r="H7">
-        <v>10202.571429</v>
+        <v>1783.7174399999999</v>
       </c>
       <c r="I7">
-        <v>522.42857100000003</v>
+        <v>1091.545026</v>
       </c>
       <c r="J7">
-        <v>9318.2857139999996</v>
+        <v>111632.94137299999</v>
       </c>
       <c r="K7">
-        <v>149.75370799999999</v>
+        <v>448</v>
       </c>
       <c r="L7">
-        <v>283.15125499999999</v>
+        <v>6035.3333329999996</v>
       </c>
       <c r="M7">
-        <v>942.283005</v>
+        <v>1042.3886930000001</v>
       </c>
       <c r="N7">
-        <v>49961.361427999997</v>
+        <v>23628.470001000002</v>
       </c>
       <c r="O7">
-        <v>821.42857100000003</v>
-      </c>
-      <c r="P7">
-        <v>25950.619048</v>
+        <v>163006.86945</v>
+      </c>
+      <c r="P7" s="18">
+        <v>144621400</v>
       </c>
       <c r="Q7">
-        <v>680.85039800000004</v>
+        <v>619.90985899999998</v>
       </c>
       <c r="R7">
-        <v>5559.8107650000002</v>
+        <v>4523.7880590000004</v>
       </c>
       <c r="S7">
-        <v>1190.6082919999999</v>
+        <v>-2.2665000000000001E-2</v>
       </c>
       <c r="T7">
-        <v>17959.077970999999</v>
-      </c>
-      <c r="U7">
-        <v>180272.13355699999</v>
-      </c>
-      <c r="V7" s="18">
-        <v>1158697000</v>
-      </c>
-      <c r="W7">
-        <v>390.27466399999997</v>
-      </c>
-      <c r="X7">
-        <v>6449.8400970000002</v>
-      </c>
-      <c r="Y7">
-        <v>0.147725</v>
-      </c>
-      <c r="Z7">
-        <v>1.5845999999999999E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+        <v>7.071E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="3">
         <v>4</v>
       </c>
       <c r="D8" s="12">
-        <v>0.45</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="E8">
-        <v>6216.5555560000003</v>
+        <v>4866.7142860000004</v>
       </c>
       <c r="F8" s="18">
-        <v>2415951</v>
+        <v>733688.9</v>
       </c>
       <c r="G8">
-        <v>914.44444399999998</v>
+        <v>145.52927700000001</v>
       </c>
       <c r="H8">
-        <v>7057.7777779999997</v>
+        <v>420.443713</v>
       </c>
       <c r="I8">
-        <v>403.55555600000002</v>
+        <v>870.55149100000006</v>
       </c>
       <c r="J8">
-        <v>5044.2777779999997</v>
+        <v>32476.618552</v>
       </c>
       <c r="K8">
-        <v>177.08838399999999</v>
+        <v>862.14285700000005</v>
       </c>
       <c r="L8">
-        <v>1651.6849400000001</v>
+        <v>31243.476190000001</v>
       </c>
       <c r="M8">
-        <v>1051.557341</v>
+        <v>666.38609099999996</v>
       </c>
       <c r="N8">
-        <v>73712.428924000007</v>
+        <v>7118.7096579999998</v>
       </c>
       <c r="O8">
-        <v>988.22222199999999</v>
-      </c>
-      <c r="P8">
-        <v>68534.444443999993</v>
+        <v>183805.85800000001</v>
+      </c>
+      <c r="P8" s="18">
+        <v>1103119000</v>
       </c>
       <c r="Q8">
-        <v>717.90284299999996</v>
+        <v>358.820696</v>
       </c>
       <c r="R8">
-        <v>11876.156901</v>
+        <v>7524.05584</v>
       </c>
       <c r="S8">
-        <v>1420.0541169999999</v>
+        <v>0.19308700000000001</v>
       </c>
       <c r="T8">
-        <v>79773.986787999995</v>
-      </c>
-      <c r="U8">
-        <v>246589.27623300001</v>
-      </c>
-      <c r="V8" s="18">
-        <v>3176175000</v>
-      </c>
-      <c r="W8">
-        <v>297.95194900000001</v>
-      </c>
-      <c r="X8">
-        <v>4073.3387619999999</v>
-      </c>
-      <c r="Y8">
-        <v>-4.3132999999999998E-2</v>
-      </c>
-      <c r="Z8">
-        <v>1.6619999999999999E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+        <v>3.5469999999999998E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="12"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="C9" s="3">
+        <v>5</v>
+      </c>
+      <c r="D9" s="12">
+        <v>0.38</v>
+      </c>
+      <c r="E9">
+        <v>7330</v>
+      </c>
+      <c r="F9" s="18">
+        <v>1147322</v>
+      </c>
+      <c r="G9">
+        <v>186.96450300000001</v>
+      </c>
+      <c r="H9">
+        <v>2218.985463</v>
+      </c>
+      <c r="I9">
+        <v>1112.5900630000001</v>
+      </c>
+      <c r="J9">
+        <v>106691.439973</v>
+      </c>
+      <c r="K9">
+        <v>1142.4000000000001</v>
+      </c>
+      <c r="L9">
+        <v>27386.3</v>
+      </c>
+      <c r="M9">
+        <v>755.78892599999995</v>
+      </c>
+      <c r="N9">
+        <v>30520.135163999999</v>
+      </c>
+      <c r="O9">
+        <v>304959.61686000001</v>
+      </c>
+      <c r="P9" s="18">
+        <v>2300754000</v>
+      </c>
+      <c r="Q9">
+        <v>262.111289</v>
+      </c>
+      <c r="R9">
+        <v>1596.591762</v>
+      </c>
+      <c r="S9">
+        <v>-2.4052E-2</v>
+      </c>
+      <c r="T9">
+        <v>5.9639999999999997E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="12"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B11" s="3">
         <v>3</v>
       </c>
-      <c r="C10" s="3">
-        <v>1</v>
-      </c>
-      <c r="D10" s="12">
-        <v>0.89</v>
-      </c>
-      <c r="E10">
-        <v>1830.25</v>
-      </c>
-      <c r="F10">
-        <v>118833.295455</v>
-      </c>
-      <c r="G10">
-        <v>772.5</v>
-      </c>
-      <c r="H10">
-        <v>6660.0909089999996</v>
-      </c>
-      <c r="I10">
-        <v>423.08333299999998</v>
-      </c>
-      <c r="J10">
-        <v>4160.992424</v>
-      </c>
-      <c r="K10">
-        <v>378.01879700000001</v>
-      </c>
-      <c r="L10">
-        <v>4584.8516010000003</v>
-      </c>
-      <c r="M10">
-        <v>1295.7533490000001</v>
-      </c>
-      <c r="N10">
-        <v>23940.556202</v>
-      </c>
-      <c r="O10">
-        <v>247.5</v>
-      </c>
-      <c r="P10">
-        <v>2958.272727</v>
-      </c>
-      <c r="Q10">
-        <v>1392.8550399999999</v>
-      </c>
-      <c r="R10">
-        <v>20620.633055999999</v>
-      </c>
-      <c r="S10">
-        <v>2700.9950840000001</v>
-      </c>
-      <c r="T10">
-        <v>191521.769967</v>
-      </c>
-      <c r="U10">
-        <v>140455.03805800001</v>
-      </c>
-      <c r="V10" s="18">
-        <v>855042200</v>
-      </c>
-      <c r="W10">
-        <v>1071.5283179999999</v>
-      </c>
-      <c r="X10">
-        <v>21250.853659</v>
-      </c>
-      <c r="Y10">
-        <v>-4.5433000000000001E-2</v>
-      </c>
-      <c r="Z10">
-        <v>1.6001999999999999E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
       <c r="C11" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="12">
-        <v>0.76</v>
+        <v>0.79</v>
       </c>
       <c r="E11">
-        <v>2648.125</v>
+        <v>2546.818182</v>
       </c>
       <c r="F11">
-        <v>55486.696429000003</v>
+        <v>70872.363635999995</v>
       </c>
       <c r="G11">
-        <v>708.5</v>
+        <v>262.931535</v>
       </c>
       <c r="H11">
-        <v>3474</v>
+        <v>1894.8620980000001</v>
       </c>
       <c r="I11">
-        <v>503.375</v>
+        <v>1157.2266589999999</v>
       </c>
       <c r="J11">
-        <v>33555.696429000003</v>
+        <v>23833.804942999999</v>
       </c>
       <c r="K11">
-        <v>267.79143699999997</v>
+        <v>366.09090900000001</v>
       </c>
       <c r="L11">
-        <v>2273.0406410000001</v>
+        <v>1657.2909090000001</v>
       </c>
       <c r="M11">
-        <v>1209.3295149999999</v>
+        <v>1041.261037</v>
       </c>
       <c r="N11">
-        <v>20713.141038000002</v>
+        <v>16317.290198999999</v>
       </c>
       <c r="O11">
-        <v>374.5</v>
-      </c>
-      <c r="P11">
-        <v>1853.4285709999999</v>
+        <v>146219.52908199999</v>
+      </c>
+      <c r="P11" s="18">
+        <v>376688400</v>
       </c>
       <c r="Q11">
-        <v>1045.4341790000001</v>
+        <v>721.48805400000003</v>
       </c>
       <c r="R11">
-        <v>21069.456459000001</v>
+        <v>9255.9127289999997</v>
       </c>
       <c r="S11">
-        <v>2077.987709</v>
+        <v>4.9418999999999998E-2</v>
       </c>
       <c r="T11">
-        <v>103616.614068</v>
-      </c>
-      <c r="U11">
-        <v>151747.92726200001</v>
-      </c>
-      <c r="V11" s="18">
-        <v>337635700</v>
-      </c>
-      <c r="W11">
-        <v>686.14610900000002</v>
-      </c>
-      <c r="X11">
-        <v>7382.4387580000002</v>
-      </c>
-      <c r="Y11">
-        <v>9.4352000000000005E-2</v>
-      </c>
-      <c r="Z11">
-        <v>3.3871999999999999E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+        <v>2.9637E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="3">
+        <v>2</v>
+      </c>
+      <c r="D12" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="E12">
+        <v>1802.25</v>
+      </c>
+      <c r="F12">
+        <v>152468.785714</v>
+      </c>
+      <c r="G12">
+        <v>407.75812999999999</v>
+      </c>
+      <c r="H12">
+        <v>4160.325366</v>
+      </c>
+      <c r="I12">
+        <v>1367.7705920000001</v>
+      </c>
+      <c r="J12">
+        <v>14891.410141</v>
+      </c>
+      <c r="K12">
+        <v>234.125</v>
+      </c>
+      <c r="L12">
+        <v>3675.5535709999999</v>
+      </c>
+      <c r="M12">
+        <v>1441.1302860000001</v>
+      </c>
+      <c r="N12">
+        <v>17020.043723999999</v>
+      </c>
+      <c r="O12">
+        <v>142994.662125</v>
+      </c>
+      <c r="P12" s="18">
+        <v>1160857000</v>
+      </c>
+      <c r="Q12">
+        <v>1096.0547859999999</v>
+      </c>
+      <c r="R12">
+        <v>29728.744718999998</v>
+      </c>
+      <c r="S12">
+        <v>-8.8401999999999994E-2</v>
+      </c>
+      <c r="T12">
+        <v>1.8419999999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3">
         <v>3</v>
       </c>
-      <c r="D12" s="12">
-        <v>0.92</v>
-      </c>
-      <c r="E12">
-        <v>1847.75</v>
-      </c>
-      <c r="F12">
-        <v>118063.11363599999</v>
-      </c>
-      <c r="G12">
-        <v>719.25</v>
-      </c>
-      <c r="H12">
-        <v>6670.568182</v>
-      </c>
-      <c r="I12">
-        <v>457.5</v>
-      </c>
-      <c r="J12">
-        <v>7420.4545449999996</v>
-      </c>
-      <c r="K12">
-        <v>255.894147</v>
-      </c>
-      <c r="L12">
-        <v>1661.658381</v>
-      </c>
-      <c r="M12">
-        <v>954.46582999999998</v>
-      </c>
-      <c r="N12">
-        <v>18376.15987</v>
-      </c>
-      <c r="O12">
-        <v>282.41666700000002</v>
-      </c>
-      <c r="P12">
-        <v>3370.992424</v>
-      </c>
-      <c r="Q12">
-        <v>1070.391257</v>
-      </c>
-      <c r="R12">
-        <v>27254.802844000002</v>
-      </c>
-      <c r="S12">
-        <v>1936.871717</v>
-      </c>
-      <c r="T12">
-        <v>117473.039372</v>
-      </c>
-      <c r="U12">
-        <v>111620.462413</v>
-      </c>
-      <c r="V12" s="18">
-        <v>807493900</v>
-      </c>
-      <c r="W12">
-        <v>920.70114699999999</v>
-      </c>
-      <c r="X12">
-        <v>14316.348910000001</v>
-      </c>
-      <c r="Y12">
-        <v>-5.5625000000000001E-2</v>
-      </c>
-      <c r="Z12">
-        <v>2.4178999999999999E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="12"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="3">
-        <v>2</v>
-      </c>
-      <c r="C14" s="3">
-        <v>1</v>
-      </c>
-      <c r="D14" s="12">
+      <c r="D13" s="12">
+        <v>0.94</v>
+      </c>
+      <c r="E13">
+        <v>1760.6153850000001</v>
+      </c>
+      <c r="F13">
+        <v>71317.923076999999</v>
+      </c>
+      <c r="G13">
+        <v>276.53653100000002</v>
+      </c>
+      <c r="H13">
+        <v>2172.665845</v>
+      </c>
+      <c r="I13">
+        <v>1000.431406</v>
+      </c>
+      <c r="J13">
+        <v>28250.252324000001</v>
+      </c>
+      <c r="K13">
+        <v>265.76923099999999</v>
+      </c>
+      <c r="L13">
+        <v>1957.025641</v>
+      </c>
+      <c r="M13">
+        <v>1149.1934839999999</v>
+      </c>
+      <c r="N13">
+        <v>37911.612609000003</v>
+      </c>
+      <c r="O13">
+        <v>114347.485143</v>
+      </c>
+      <c r="P13" s="18">
+        <v>873159500</v>
+      </c>
+      <c r="Q13">
+        <v>976.23965899999996</v>
+      </c>
+      <c r="R13">
+        <v>11061.338453</v>
+      </c>
+      <c r="S13">
+        <v>-2.2637000000000001E-2</v>
+      </c>
+      <c r="T13">
+        <v>2.4237999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="12"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="3">
+        <v>2</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="12">
         <v>0.9</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <v>1739.833333</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <v>178983.76666699999</v>
       </c>
-      <c r="G14">
-        <v>752</v>
-      </c>
-      <c r="H14">
-        <v>14627.2</v>
-      </c>
-      <c r="I14">
-        <v>432.66666700000002</v>
-      </c>
-      <c r="J14">
-        <v>2790.666667</v>
-      </c>
-      <c r="K14">
+      <c r="G15">
         <v>307.72950600000001</v>
       </c>
-      <c r="L14">
+      <c r="H15">
         <v>4890.5534399999997</v>
       </c>
-      <c r="M14">
+      <c r="I15">
         <v>1112.6261919999999</v>
       </c>
-      <c r="N14">
+      <c r="J15">
         <v>37055.747754999997</v>
       </c>
-      <c r="O14">
+      <c r="K15">
         <v>249.66666699999999</v>
       </c>
-      <c r="P14">
+      <c r="L15">
         <v>4420.6666670000004</v>
       </c>
-      <c r="Q14">
+      <c r="M15">
         <v>1211.0714700000001</v>
       </c>
-      <c r="R14">
+      <c r="N15">
         <v>71898.080390999996</v>
       </c>
-      <c r="S14">
-        <v>2251.2261530000001</v>
-      </c>
-      <c r="T14">
-        <v>175012.62764200001</v>
-      </c>
-      <c r="U14">
+      <c r="O15">
         <v>114600.766343</v>
       </c>
-      <c r="V14" s="18">
+      <c r="P15" s="18">
         <v>510096100</v>
       </c>
-      <c r="W14">
+      <c r="Q15">
         <v>1025.3733279999999</v>
       </c>
-      <c r="X14">
+      <c r="R15">
         <v>76444.986667999998</v>
       </c>
-      <c r="Y14">
+      <c r="S15">
         <v>2.0501999999999999E-2</v>
       </c>
-      <c r="Z14">
+      <c r="T15">
         <v>7.541E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3">
-        <v>2</v>
-      </c>
-      <c r="D15" s="12">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3">
+        <v>2</v>
+      </c>
+      <c r="D16" s="12">
         <v>0.65</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>3385.0576919999999</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <v>592731.926538</v>
       </c>
-      <c r="G15">
-        <v>827.61538499999995</v>
-      </c>
-      <c r="H15">
-        <v>1930.886154</v>
-      </c>
-      <c r="I15">
-        <v>410.90384599999999</v>
-      </c>
-      <c r="J15">
-        <v>2171.8803849999999</v>
-      </c>
-      <c r="K15">
+      <c r="G16">
         <v>371.539221</v>
       </c>
-      <c r="L15">
+      <c r="H16">
         <v>1035.578855</v>
       </c>
-      <c r="M15">
+      <c r="I16">
         <v>1222.5497009999999</v>
       </c>
-      <c r="N15">
+      <c r="J16">
         <v>15536.642760999999</v>
       </c>
-      <c r="O15">
+      <c r="K16">
         <v>498.94230800000003</v>
       </c>
-      <c r="P15">
+      <c r="L16">
         <v>16900.946538</v>
       </c>
-      <c r="Q15">
+      <c r="M16">
         <v>1245.3258940000001</v>
       </c>
-      <c r="R15">
+      <c r="N16">
         <v>12740.419583999999</v>
       </c>
-      <c r="S15">
-        <v>2578.3067820000001</v>
-      </c>
-      <c r="T15">
-        <v>49049.371189999998</v>
-      </c>
-      <c r="U15">
+      <c r="O16">
         <v>193914.33996899999</v>
       </c>
-      <c r="V15" s="18">
+      <c r="P16" s="18">
         <v>1004123000</v>
       </c>
-      <c r="W15">
+      <c r="Q16">
         <v>722.09551699999997</v>
       </c>
-      <c r="X15">
+      <c r="R16">
         <v>4047.1366130000001</v>
       </c>
-      <c r="Y15">
+      <c r="S16">
         <v>-0.116019</v>
       </c>
-      <c r="Z15">
+      <c r="T16">
         <v>5.2220000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B16" s="3">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
         <v>4</v>
       </c>
-      <c r="C16" s="3">
-        <v>1</v>
-      </c>
-      <c r="D16" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="E16">
-        <v>2178</v>
-      </c>
-      <c r="F16">
-        <v>302642</v>
-      </c>
-      <c r="G16">
-        <v>654</v>
-      </c>
-      <c r="H16">
-        <v>10368</v>
-      </c>
-      <c r="I16">
-        <v>395.5</v>
-      </c>
-      <c r="J16">
-        <v>1104.5</v>
-      </c>
-      <c r="K16">
-        <v>229.304495</v>
-      </c>
-      <c r="L16">
-        <v>106.140266</v>
-      </c>
-      <c r="M16">
-        <v>989.65582400000005</v>
-      </c>
-      <c r="N16">
-        <v>1239.699991</v>
-      </c>
-      <c r="O16">
-        <v>311.5</v>
-      </c>
-      <c r="P16">
-        <v>7320.5</v>
-      </c>
-      <c r="Q16">
-        <v>930.86591499999997</v>
-      </c>
-      <c r="R16">
-        <v>1374.7302589999999</v>
-      </c>
-      <c r="S16">
-        <v>1828.920476</v>
-      </c>
-      <c r="T16">
-        <v>1718.9084230000001</v>
-      </c>
-      <c r="U16">
-        <v>114951.28943</v>
-      </c>
-      <c r="V16" s="18">
-        <v>1191293000</v>
-      </c>
-      <c r="W16">
-        <v>713.24588500000004</v>
-      </c>
-      <c r="X16">
-        <v>45534.539232000003</v>
-      </c>
-      <c r="Y16">
-        <v>6.3261999999999999E-2</v>
-      </c>
-      <c r="Z16">
-        <v>6.6000000000000005E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
       <c r="C17" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" s="12">
         <v>0.9</v>
       </c>
       <c r="E17">
-        <v>1520.75</v>
+        <v>1565</v>
       </c>
       <c r="F17">
-        <v>5435.5833329999996</v>
+        <v>6962</v>
       </c>
       <c r="G17">
-        <v>801</v>
+        <v>384.50730299999998</v>
       </c>
       <c r="H17">
-        <v>11318.666667</v>
+        <v>164.46562700000001</v>
       </c>
       <c r="I17">
-        <v>451.25</v>
+        <v>1354.8641970000001</v>
       </c>
       <c r="J17">
-        <v>2901.583333</v>
+        <v>7984.0180710000004</v>
       </c>
       <c r="K17">
-        <v>346.94201199999998</v>
+        <v>229</v>
       </c>
       <c r="L17">
-        <v>1965.059966</v>
+        <v>512</v>
       </c>
       <c r="M17">
-        <v>1174.1113760000001</v>
+        <v>1491.7993309999999</v>
       </c>
       <c r="N17">
-        <v>46224.634835999997</v>
+        <v>13548.603668</v>
       </c>
       <c r="O17">
-        <v>218.75</v>
-      </c>
-      <c r="P17">
-        <v>1104.25</v>
+        <v>130313.86195000001</v>
+      </c>
+      <c r="P17" s="18">
+        <v>17599700</v>
       </c>
       <c r="Q17">
-        <v>1351.174248</v>
+        <v>1282.490675</v>
       </c>
       <c r="R17">
-        <v>40856.737567999997</v>
+        <v>3519.1975929999999</v>
       </c>
       <c r="S17">
-        <v>2462.378991</v>
+        <v>3.9810999999999999E-2</v>
       </c>
       <c r="T17">
-        <v>112772.65829599999</v>
-      </c>
-      <c r="U17">
-        <v>114425.5048</v>
-      </c>
-      <c r="V17" s="18">
-        <v>452939500</v>
-      </c>
-      <c r="W17">
-        <v>1181.4370489999999</v>
-      </c>
-      <c r="X17">
-        <v>14806.590716000001</v>
-      </c>
-      <c r="Y17">
-        <v>-8.7799999999999998E-4</v>
-      </c>
-      <c r="Z17">
-        <v>1.0717000000000001E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.25">
+        <v>1.9769999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" s="12">
-        <v>0.68</v>
+        <v>0.9</v>
       </c>
       <c r="E18">
-        <v>2825.5625</v>
+        <v>1827.25</v>
       </c>
       <c r="F18">
-        <v>206296.388393</v>
+        <v>265418.91666699998</v>
       </c>
       <c r="G18">
-        <v>824.3125</v>
+        <v>269.34060799999997</v>
       </c>
       <c r="H18">
-        <v>1045.8526790000001</v>
+        <v>2201.2705380000002</v>
       </c>
       <c r="I18">
-        <v>434.75</v>
+        <v>991.50719000000004</v>
       </c>
       <c r="J18">
-        <v>1249.9285709999999</v>
+        <v>418.98952400000002</v>
       </c>
       <c r="K18">
-        <v>409.11131799999998</v>
+        <v>260</v>
       </c>
       <c r="L18">
-        <v>397.60211299999997</v>
+        <v>6770</v>
       </c>
       <c r="M18">
-        <v>1292.983442</v>
+        <v>1070.7075400000001</v>
       </c>
       <c r="N18">
-        <v>13186.836364999999</v>
+        <v>36505.800989000003</v>
       </c>
       <c r="O18">
-        <v>390.5625</v>
-      </c>
-      <c r="P18">
-        <v>6146.2455360000004</v>
+        <v>106744.21854</v>
+      </c>
+      <c r="P18" s="18">
+        <v>597392200</v>
       </c>
       <c r="Q18">
-        <v>1384.809481</v>
+        <v>896.81465400000002</v>
       </c>
       <c r="R18">
-        <v>3838.774077</v>
+        <v>60125.914872000001</v>
       </c>
       <c r="S18">
-        <v>2837.7939270000002</v>
+        <v>1.0847000000000001E-2</v>
       </c>
       <c r="T18">
-        <v>17968.547284</v>
-      </c>
-      <c r="U18">
-        <v>199541.78588800001</v>
-      </c>
-      <c r="V18" s="18">
-        <v>1000363000</v>
-      </c>
-      <c r="W18">
-        <v>779.69089099999997</v>
-      </c>
-      <c r="X18">
-        <v>3312.2219260000002</v>
-      </c>
-      <c r="Y18">
-        <v>-0.16553899999999999</v>
-      </c>
-      <c r="Z18">
-        <v>1.2329999999999999E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
+        <v>5.6049999999999997E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="3">
+        <v>3</v>
+      </c>
+      <c r="D19" s="12">
+        <v>0.69</v>
+      </c>
+      <c r="E19">
+        <v>2974.9285709999999</v>
+      </c>
+      <c r="F19">
+        <v>234136.725275</v>
+      </c>
+      <c r="G19">
+        <v>389.93349599999999</v>
+      </c>
+      <c r="H19">
+        <v>886.51278300000001</v>
+      </c>
+      <c r="I19">
+        <v>1261.4699169999999</v>
+      </c>
+      <c r="J19">
+        <v>11103.441892999999</v>
+      </c>
+      <c r="K19">
+        <v>420.07142900000002</v>
+      </c>
+      <c r="L19">
+        <v>7869.8791209999999</v>
+      </c>
+      <c r="M19">
+        <v>1309.901597</v>
+      </c>
+      <c r="N19">
+        <v>11153.346777000001</v>
+      </c>
+      <c r="O19">
+        <v>190384.07129299999</v>
+      </c>
+      <c r="P19" s="18">
+        <v>774363500</v>
+      </c>
+      <c r="Q19">
+        <v>758.05282499999998</v>
+      </c>
+      <c r="R19">
+        <v>3250.556998</v>
+      </c>
+      <c r="S19">
+        <v>-0.16040399999999999</v>
+      </c>
+      <c r="T19">
+        <v>1.9319999999999999E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3">
         <v>4</v>
       </c>
-      <c r="D19" s="12">
-        <v>0.63</v>
-      </c>
-      <c r="E19">
-        <v>3633.7222219999999</v>
-      </c>
-      <c r="F19">
-        <v>573937.15359500004</v>
-      </c>
-      <c r="G19">
-        <v>829.08333300000004</v>
-      </c>
-      <c r="H19">
-        <v>2401.4779410000001</v>
-      </c>
-      <c r="I19">
-        <v>400.30555600000002</v>
-      </c>
-      <c r="J19">
-        <v>2292.7393790000001</v>
-      </c>
-      <c r="K19">
-        <v>354.84051199999999</v>
-      </c>
-      <c r="L19">
-        <v>399.63016699999997</v>
-      </c>
-      <c r="M19">
-        <v>1191.245815</v>
-      </c>
-      <c r="N19">
-        <v>14046.007121000001</v>
-      </c>
-      <c r="O19">
-        <v>547.11111100000005</v>
-      </c>
-      <c r="P19">
-        <v>14339.19281</v>
-      </c>
-      <c r="Q19">
-        <v>1183.3331889999999</v>
-      </c>
-      <c r="R19">
-        <v>3930.4696720000002</v>
-      </c>
-      <c r="S19">
-        <v>2462.9791620000001</v>
-      </c>
-      <c r="T19">
-        <v>18963.384773000002</v>
-      </c>
-      <c r="U19">
-        <v>191413.252894</v>
-      </c>
-      <c r="V19" s="18">
-        <v>1043211000</v>
-      </c>
-      <c r="W19">
-        <v>696.49757299999999</v>
-      </c>
-      <c r="X19">
-        <v>2332.9682459999999</v>
-      </c>
-      <c r="Y19">
-        <v>-9.4009999999999996E-2</v>
-      </c>
-      <c r="Z19">
-        <v>5.5040000000000002E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="D20" s="12">
+        <v>0.59</v>
+      </c>
+      <c r="E20">
+        <v>3863.541667</v>
+      </c>
+      <c r="F20">
+        <v>606570.47537899995</v>
+      </c>
+      <c r="G20">
+        <v>350.07923299999999</v>
+      </c>
+      <c r="H20">
+        <v>372.86738300000002</v>
+      </c>
+      <c r="I20">
+        <v>1177.142781</v>
+      </c>
+      <c r="J20">
+        <v>18011.172585</v>
+      </c>
+      <c r="K20">
+        <v>590.95833300000004</v>
+      </c>
+      <c r="L20">
+        <v>11956.657197</v>
+      </c>
+      <c r="M20">
+        <v>1169.987574</v>
+      </c>
+      <c r="N20">
+        <v>4275.1210730000003</v>
+      </c>
+      <c r="O20">
+        <v>198032.98675800001</v>
+      </c>
+      <c r="P20" s="18">
+        <v>1332574000</v>
+      </c>
+      <c r="Q20">
+        <v>680.14532499999996</v>
+      </c>
+      <c r="R20">
+        <v>1791.1235859999999</v>
+      </c>
+      <c r="S20">
+        <v>-6.4236000000000001E-2</v>
+      </c>
+      <c r="T20">
+        <v>4.1510000000000002E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="W1:X1"/>
+  <mergeCells count="8">
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
+    <mergeCell ref="S1:T1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[update] updated answer data
</commit_message>
<xml_diff>
--- a/Experiment-Data/Answer-Data.xlsx
+++ b/Experiment-Data/Answer-Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\www\Desktop\eye-tracking-software\Experiment-Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC_User\Desktop\eye-tracking-software\Experiment-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E956E7-4010-409F-A437-DDBF143504AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB628298-4D44-4C47-BD2A-C14BF7353D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{65F65776-174E-4145-8CCF-AA6B8A50F68A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{65F65776-174E-4145-8CCF-AA6B8A50F68A}"/>
   </bookViews>
   <sheets>
     <sheet name="1st" sheetId="1" r:id="rId1"/>
@@ -175,7 +175,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -187,7 +187,7 @@
     </font>
     <font>
       <sz val="6"/>
-      <name val="Aptos Narrow"/>
+      <name val="游ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -645,20 +645,20 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10" style="3" customWidth="1"/>
-    <col min="2" max="5" width="4.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" style="13" customWidth="1"/>
-    <col min="7" max="26" width="4.42578125" style="2" customWidth="1"/>
-    <col min="27" max="27" width="4.140625" style="3" customWidth="1"/>
+    <col min="2" max="5" width="4.25" style="3" customWidth="1"/>
+    <col min="6" max="6" width="6.25" style="13" customWidth="1"/>
+    <col min="7" max="26" width="4.375" style="2" customWidth="1"/>
+    <col min="27" max="27" width="4.125" style="3" customWidth="1"/>
     <col min="28" max="28" width="10" style="3" customWidth="1"/>
-    <col min="29" max="31" width="4.28515625" style="3" customWidth="1"/>
-    <col min="32" max="32" width="6.140625" style="3" customWidth="1"/>
-    <col min="33" max="42" width="4.42578125" style="4" customWidth="1"/>
+    <col min="29" max="31" width="4.25" style="3" customWidth="1"/>
+    <col min="32" max="32" width="6.125" style="3" customWidth="1"/>
+    <col min="33" max="42" width="4.375" style="4" customWidth="1"/>
     <col min="44" max="44" width="10" style="3" customWidth="1"/>
-    <col min="45" max="48" width="4.28515625" style="3" customWidth="1"/>
-    <col min="49" max="49" width="6.140625" style="3" customWidth="1"/>
+    <col min="45" max="48" width="4.25" style="3" customWidth="1"/>
+    <col min="49" max="49" width="6.125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -859,7 +859,7 @@
       <c r="AV2" s="5"/>
       <c r="AW2" s="5"/>
     </row>
-    <row r="3" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="4" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.4">
       <c r="C4" s="3">
         <v>2</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>0.52499999999999991</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.4">
       <c r="F5" s="12"/>
       <c r="G5" s="16">
         <f>(COUNTIF(G3:G4,"○"))/2</f>
@@ -1228,7 +1228,7 @@
       <c r="AP5" s="1"/>
       <c r="AW5" s="12"/>
     </row>
-    <row r="6" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.4">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="7" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.4">
       <c r="C7" s="3">
         <v>2</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.4">
       <c r="C8" s="3">
         <v>3</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="9" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.4">
       <c r="C9" s="3">
         <v>4</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.4">
       <c r="C10" s="3">
         <v>5</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.4">
       <c r="C11" s="3">
         <v>6</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.4">
       <c r="C12" s="3">
         <v>7</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>0.67500000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.4">
       <c r="C13" s="3">
         <v>8</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.4">
       <c r="C14" s="3">
         <v>9</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>0.72500000000000009</v>
       </c>
     </row>
-    <row r="15" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.4">
       <c r="C15" s="3">
         <v>10</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.4">
       <c r="F16" s="12"/>
       <c r="G16" s="16">
         <f>(COUNTIF(G6:G15,"○"))/10</f>
@@ -2612,7 +2612,7 @@
       <c r="AP16" s="1"/>
       <c r="AW16" s="12"/>
     </row>
-    <row r="17" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:49" x14ac:dyDescent="0.4">
       <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:49" x14ac:dyDescent="0.4">
       <c r="C18" s="3">
         <v>2</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="19" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:49" x14ac:dyDescent="0.4">
       <c r="C19" s="3">
         <v>3</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:49" x14ac:dyDescent="0.4">
       <c r="C20" s="3">
         <v>4</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="21" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:49" x14ac:dyDescent="0.4">
       <c r="C21" s="3">
         <v>5</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="22" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:49" x14ac:dyDescent="0.4">
       <c r="C22" s="3">
         <v>6</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="23" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:49" x14ac:dyDescent="0.4">
       <c r="C23" s="3">
         <v>7</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="24" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:49" x14ac:dyDescent="0.4">
       <c r="C24" s="3">
         <v>8</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="25" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:49" x14ac:dyDescent="0.4">
       <c r="C25" s="3">
         <v>9</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="26" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:49" x14ac:dyDescent="0.4">
       <c r="C26" s="3">
         <v>10</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:49" x14ac:dyDescent="0.4">
       <c r="C27" s="3">
         <v>11</v>
       </c>
@@ -4029,7 +4029,7 @@
         <v>0.52500000000000002</v>
       </c>
     </row>
-    <row r="28" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:49" x14ac:dyDescent="0.4">
       <c r="C28" s="3">
         <v>12</v>
       </c>
@@ -4157,7 +4157,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="29" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:49" x14ac:dyDescent="0.4">
       <c r="C29" s="3">
         <v>13</v>
       </c>
@@ -4285,7 +4285,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="30" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:49" x14ac:dyDescent="0.4">
       <c r="C30" s="3">
         <v>14</v>
       </c>
@@ -4413,7 +4413,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:49" x14ac:dyDescent="0.4">
       <c r="F31" s="5"/>
       <c r="G31" s="15">
         <f>(COUNTIF(G17:G30,"○"))/14</f>
@@ -4555,7 +4555,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="32" spans="2:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:49" x14ac:dyDescent="0.4">
       <c r="F32" s="12"/>
       <c r="AD32" s="3">
         <v>2</v>
@@ -4611,7 +4611,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="33" spans="29:49" x14ac:dyDescent="0.25">
+    <row r="33" spans="29:49" x14ac:dyDescent="0.4">
       <c r="AC33" s="3" t="s">
         <v>7</v>
       </c>
@@ -4672,7 +4672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="29:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="34" spans="29:49" x14ac:dyDescent="0.4">
       <c r="AD34" s="3">
         <v>2</v>
       </c>
@@ -4727,7 +4727,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="35" spans="29:49" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="29:49" x14ac:dyDescent="0.4">
       <c r="AD35" s="3">
         <v>3</v>
       </c>
@@ -4782,7 +4782,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="36" spans="29:49" x14ac:dyDescent="0.25">
+    <row r="36" spans="29:49" x14ac:dyDescent="0.4">
       <c r="AC36" s="3" t="s">
         <v>6</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="29:49" x14ac:dyDescent="0.25">
+    <row r="37" spans="29:49" x14ac:dyDescent="0.4">
       <c r="AG37" s="15">
         <f>(COUNTIF(AG3:AG36,"○")/32)</f>
         <v>1</v>
@@ -4887,12 +4887,12 @@
       <c r="AU37"/>
       <c r="AV37"/>
     </row>
-    <row r="38" spans="29:49" x14ac:dyDescent="0.25">
+    <row r="38" spans="29:49" x14ac:dyDescent="0.4">
       <c r="AU38"/>
       <c r="AV38"/>
       <c r="AW38" s="12"/>
     </row>
-    <row r="39" spans="29:49" x14ac:dyDescent="0.25">
+    <row r="39" spans="29:49" x14ac:dyDescent="0.4">
       <c r="AF39" s="12"/>
     </row>
   </sheetData>
@@ -4911,18 +4911,18 @@
   <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10" style="3" customWidth="1"/>
-    <col min="2" max="3" width="8.5703125" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" style="3" customWidth="1"/>
+    <col min="2" max="3" width="8.625" customWidth="1"/>
+    <col min="4" max="4" width="5.75" style="3" customWidth="1"/>
     <col min="5" max="21" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -4968,7 +4968,7 @@
       </c>
       <c r="T1" s="21"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -5022,7 +5022,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -5084,7 +5084,7 @@
         <v>7.7279999999999996E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.4">
       <c r="B4" s="3"/>
       <c r="C4" s="3">
         <v>2</v>
@@ -5141,7 +5141,7 @@
         <v>1.6605000000000002E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.4">
       <c r="B5" s="3">
         <v>5</v>
       </c>
@@ -5200,7 +5200,7 @@
         <v>7.0330000000000002E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.4">
       <c r="B6" s="3"/>
       <c r="C6" s="3">
         <v>2</v>
@@ -5257,7 +5257,7 @@
         <v>6.0879999999999997E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.4">
       <c r="B7" s="3"/>
       <c r="C7" s="3">
         <v>3</v>
@@ -5314,7 +5314,7 @@
         <v>7.071E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.4">
       <c r="B8" s="3"/>
       <c r="C8" s="3">
         <v>4</v>
@@ -5371,7 +5371,7 @@
         <v>3.5469999999999998E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.4">
       <c r="B9" s="3"/>
       <c r="C9" s="3">
         <v>5</v>
@@ -5428,12 +5428,12 @@
         <v>5.9639999999999997E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.4">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="12"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>2.9637E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.4">
       <c r="B12" s="3"/>
       <c r="C12" s="3">
         <v>2</v>
@@ -5552,7 +5552,7 @@
         <v>1.8419999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.4">
       <c r="B13" s="3"/>
       <c r="C13" s="3">
         <v>3</v>
@@ -5609,12 +5609,12 @@
         <v>2.4237999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.4">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="12"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
@@ -5676,7 +5676,7 @@
         <v>7.541E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.4">
       <c r="B16" s="3"/>
       <c r="C16" s="3">
         <v>2</v>
@@ -5733,7 +5733,7 @@
         <v>5.2220000000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.4">
       <c r="B17" s="3">
         <v>4</v>
       </c>
@@ -5792,7 +5792,7 @@
         <v>1.9769999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.4">
       <c r="B18" s="3"/>
       <c r="C18" s="3">
         <v>2</v>
@@ -5849,7 +5849,7 @@
         <v>5.6049999999999997E-3</v>
       </c>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.4">
       <c r="B19" s="3"/>
       <c r="C19" s="3">
         <v>3</v>
@@ -5906,7 +5906,7 @@
         <v>1.9319999999999999E-3</v>
       </c>
     </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.4">
       <c r="B20" s="3"/>
       <c r="C20" s="3">
         <v>4</v>
@@ -5963,31 +5963,31 @@
         <v>4.1510000000000002E-3</v>
       </c>
     </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.4">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.4">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.4">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.4">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.4">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.4">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:20" x14ac:dyDescent="0.4">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="5"/>
@@ -6003,6 +6003,7 @@
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
   </mergeCells>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[update] updated experiment data
</commit_message>
<xml_diff>
--- a/Experiment-Data/Answer-Data.xlsx
+++ b/Experiment-Data/Answer-Data.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC_User\Desktop\eye-tracking-software\Experiment-Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\www\Desktop\eye-tracking-software\Experiment-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA19F7CB-9A2B-44D4-AFFC-D942F0E62E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA9A6C3-DE59-42C7-948E-FFC9A2829662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{65F65776-174E-4145-8CCF-AA6B8A50F68A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{65F65776-174E-4145-8CCF-AA6B8A50F68A}"/>
   </bookViews>
   <sheets>
     <sheet name="1st" sheetId="1" r:id="rId1"/>
-    <sheet name="1st-Features" sheetId="2" r:id="rId2"/>
+    <sheet name="2nd" sheetId="3" r:id="rId2"/>
+    <sheet name="1st-Features" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="30">
   <si>
     <t>English</t>
   </si>
@@ -175,7 +176,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -187,7 +188,7 @@
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Aptos Narrow"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -644,23 +645,23 @@
   <dimension ref="A1:AX39"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" style="3" customWidth="1"/>
-    <col min="2" max="6" width="4.25" style="3" customWidth="1"/>
-    <col min="7" max="7" width="6.25" style="13" customWidth="1"/>
-    <col min="8" max="27" width="4.375" style="2" customWidth="1"/>
-    <col min="28" max="28" width="4.125" style="3" customWidth="1"/>
+    <col min="2" max="6" width="4.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" style="13" customWidth="1"/>
+    <col min="8" max="27" width="4.42578125" style="2" customWidth="1"/>
+    <col min="28" max="28" width="4.140625" style="3" customWidth="1"/>
     <col min="29" max="29" width="10" style="3" customWidth="1"/>
-    <col min="30" max="32" width="4.25" style="3" customWidth="1"/>
-    <col min="33" max="33" width="6.125" style="3" customWidth="1"/>
-    <col min="34" max="43" width="4.375" style="4" customWidth="1"/>
+    <col min="30" max="32" width="4.28515625" style="3" customWidth="1"/>
+    <col min="33" max="33" width="6.140625" style="3" customWidth="1"/>
+    <col min="34" max="43" width="4.42578125" style="4" customWidth="1"/>
     <col min="45" max="45" width="10" style="3" customWidth="1"/>
-    <col min="46" max="49" width="4.25" style="3" customWidth="1"/>
-    <col min="50" max="50" width="6.125" style="3" customWidth="1"/>
+    <col min="46" max="49" width="4.28515625" style="3" customWidth="1"/>
+    <col min="50" max="50" width="6.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -865,7 +866,7 @@
       <c r="AW2" s="5"/>
       <c r="AX2" s="5"/>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1014,7 +1015,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C4" s="3">
         <v>2</v>
       </c>
@@ -1145,7 +1146,7 @@
         <v>0.52499999999999991</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="G5" s="12"/>
       <c r="H5" s="16">
         <f>(COUNTIF(H3:H4,"○"))/2</f>
@@ -1240,7 +1241,7 @@
       <c r="AQ5" s="1"/>
       <c r="AX5" s="12"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1380,7 +1381,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C7" s="3">
         <v>2</v>
       </c>
@@ -1511,7 +1512,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C8" s="3">
         <v>3</v>
       </c>
@@ -1642,7 +1643,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C9" s="3">
         <v>4</v>
       </c>
@@ -1773,7 +1774,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C10" s="3">
         <v>5</v>
       </c>
@@ -1904,7 +1905,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C11" s="3">
         <v>6</v>
       </c>
@@ -2035,7 +2036,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C12" s="3">
         <v>7</v>
       </c>
@@ -2166,7 +2167,7 @@
         <v>0.67500000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C13" s="3">
         <v>8</v>
       </c>
@@ -2297,7 +2298,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C14" s="3">
         <v>9</v>
       </c>
@@ -2428,7 +2429,7 @@
         <v>0.72500000000000009</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C15" s="3">
         <v>10</v>
       </c>
@@ -2559,7 +2560,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="G16" s="12"/>
       <c r="H16" s="16">
         <f>(COUNTIF(H6:H15,"○"))/10</f>
@@ -2654,7 +2655,7 @@
       <c r="AQ16" s="1"/>
       <c r="AX16" s="12"/>
     </row>
-    <row r="17" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
@@ -2794,7 +2795,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C18" s="3">
         <v>2</v>
       </c>
@@ -2925,7 +2926,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="19" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C19" s="3">
         <v>3</v>
       </c>
@@ -3056,7 +3057,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C20" s="3">
         <v>4</v>
       </c>
@@ -3187,7 +3188,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="21" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C21" s="3">
         <v>5</v>
       </c>
@@ -3318,7 +3319,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="22" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C22" s="3">
         <v>6</v>
       </c>
@@ -3449,7 +3450,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="23" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C23" s="3">
         <v>7</v>
       </c>
@@ -3580,7 +3581,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="24" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C24" s="3">
         <v>8</v>
       </c>
@@ -3711,7 +3712,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="25" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C25" s="3">
         <v>9</v>
       </c>
@@ -3842,7 +3843,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="26" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C26" s="3">
         <v>10</v>
       </c>
@@ -3973,7 +3974,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C27" s="3">
         <v>11</v>
       </c>
@@ -4104,7 +4105,7 @@
         <v>0.52500000000000002</v>
       </c>
     </row>
-    <row r="28" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C28" s="3">
         <v>12</v>
       </c>
@@ -4235,7 +4236,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="29" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C29" s="3">
         <v>13</v>
       </c>
@@ -4366,7 +4367,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="30" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C30" s="3">
         <v>14</v>
       </c>
@@ -4497,7 +4498,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="G31" s="5"/>
       <c r="H31" s="15">
         <f>(COUNTIF(H17:H30,"○"))/14</f>
@@ -4639,7 +4640,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="32" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="G32" s="12"/>
       <c r="AE32" s="3">
         <v>2</v>
@@ -4695,7 +4696,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="33" spans="30:50" x14ac:dyDescent="0.4">
+    <row r="33" spans="30:50" x14ac:dyDescent="0.25">
       <c r="AD33" s="3" t="s">
         <v>7</v>
       </c>
@@ -4756,7 +4757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="30:50" x14ac:dyDescent="0.4">
+    <row r="34" spans="30:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="AE34" s="3">
         <v>2</v>
       </c>
@@ -4811,7 +4812,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="35" spans="30:50" x14ac:dyDescent="0.4">
+    <row r="35" spans="30:50" ht="16.5" x14ac:dyDescent="0.3">
       <c r="AE35" s="3">
         <v>3</v>
       </c>
@@ -4866,7 +4867,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="36" spans="30:50" x14ac:dyDescent="0.4">
+    <row r="36" spans="30:50" x14ac:dyDescent="0.25">
       <c r="AD36" s="3" t="s">
         <v>6</v>
       </c>
@@ -4927,7 +4928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="30:50" x14ac:dyDescent="0.4">
+    <row r="37" spans="30:50" x14ac:dyDescent="0.25">
       <c r="AH37" s="15">
         <f>(COUNTIF(AH3:AH36,"○")/32)</f>
         <v>1</v>
@@ -4971,12 +4972,12 @@
       <c r="AV37"/>
       <c r="AW37"/>
     </row>
-    <row r="38" spans="30:50" x14ac:dyDescent="0.4">
+    <row r="38" spans="30:50" x14ac:dyDescent="0.25">
       <c r="AV38"/>
       <c r="AW38"/>
       <c r="AX38" s="12"/>
     </row>
-    <row r="39" spans="30:50" x14ac:dyDescent="0.4">
+    <row r="39" spans="30:50" x14ac:dyDescent="0.25">
       <c r="AG39" s="12"/>
     </row>
   </sheetData>
@@ -4991,22 +4992,2912 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CCB7AF-21A6-41ED-886C-DD886AE34E4A}">
+  <dimension ref="A1:AX39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" style="3" customWidth="1"/>
+    <col min="2" max="6" width="4.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" style="13" customWidth="1"/>
+    <col min="8" max="27" width="4.42578125" style="2" customWidth="1"/>
+    <col min="28" max="28" width="4.140625" style="3" customWidth="1"/>
+    <col min="29" max="29" width="10" style="3" customWidth="1"/>
+    <col min="30" max="32" width="4.28515625" style="3" customWidth="1"/>
+    <col min="33" max="33" width="6.140625" style="3" customWidth="1"/>
+    <col min="34" max="43" width="4.42578125" style="4" customWidth="1"/>
+    <col min="45" max="45" width="10" style="3" customWidth="1"/>
+    <col min="46" max="49" width="4.28515625" style="3" customWidth="1"/>
+    <col min="50" max="50" width="6.140625" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:50" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="5">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF1" s="5">
+        <v>3</v>
+      </c>
+      <c r="AG1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH1" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI1" s="20"/>
+      <c r="AJ1" s="20"/>
+      <c r="AK1" s="20"/>
+      <c r="AL1" s="20"/>
+      <c r="AM1" s="20"/>
+      <c r="AN1" s="20"/>
+      <c r="AO1" s="20"/>
+      <c r="AP1" s="20"/>
+      <c r="AQ1" s="20"/>
+      <c r="AS1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AT1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AU1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV1" s="5">
+        <v>2</v>
+      </c>
+      <c r="AW1" s="5">
+        <v>4</v>
+      </c>
+      <c r="AX1" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:50" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="6">
+        <v>1</v>
+      </c>
+      <c r="I2" s="6">
+        <v>2</v>
+      </c>
+      <c r="J2" s="6">
+        <v>3</v>
+      </c>
+      <c r="K2" s="6">
+        <v>4</v>
+      </c>
+      <c r="L2" s="6">
+        <v>5</v>
+      </c>
+      <c r="M2" s="6">
+        <v>6</v>
+      </c>
+      <c r="N2" s="6">
+        <v>7</v>
+      </c>
+      <c r="O2" s="6">
+        <v>8</v>
+      </c>
+      <c r="P2" s="6">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>10</v>
+      </c>
+      <c r="R2" s="6">
+        <v>11</v>
+      </c>
+      <c r="S2" s="6">
+        <v>12</v>
+      </c>
+      <c r="T2" s="6">
+        <v>13</v>
+      </c>
+      <c r="U2" s="6">
+        <v>14</v>
+      </c>
+      <c r="V2" s="6">
+        <v>15</v>
+      </c>
+      <c r="W2" s="6">
+        <v>16</v>
+      </c>
+      <c r="X2" s="6">
+        <v>17</v>
+      </c>
+      <c r="Y2" s="6">
+        <v>18</v>
+      </c>
+      <c r="Z2" s="6">
+        <v>19</v>
+      </c>
+      <c r="AA2" s="6">
+        <v>20</v>
+      </c>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="7">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="7">
+        <v>3</v>
+      </c>
+      <c r="AK2" s="7">
+        <v>4</v>
+      </c>
+      <c r="AL2" s="7">
+        <v>5</v>
+      </c>
+      <c r="AM2" s="7">
+        <v>6</v>
+      </c>
+      <c r="AN2" s="7">
+        <v>7</v>
+      </c>
+      <c r="AO2" s="7">
+        <v>8</v>
+      </c>
+      <c r="AP2" s="7">
+        <v>9</v>
+      </c>
+      <c r="AQ2" s="7">
+        <v>10</v>
+      </c>
+      <c r="AS2" s="5"/>
+      <c r="AT2" s="5"/>
+      <c r="AU2" s="5"/>
+      <c r="AV2" s="5"/>
+      <c r="AW2" s="5"/>
+      <c r="AX2" s="5"/>
+    </row>
+    <row r="3" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="12">
+        <f>COUNTIF(H3:AA3,"○")/20</f>
+        <v>0.5</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="T3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="U3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="W3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="X3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="12">
+        <f>(COUNTIF(AH3:AQ3,"○")/10)</f>
+        <v>0.9</v>
+      </c>
+      <c r="AH3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AS3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AT3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AV3"/>
+      <c r="AW3"/>
+      <c r="AX3" s="12">
+        <f>(G3+AG3)/2</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+      <c r="G4" s="12">
+        <f t="shared" ref="G4:G30" si="0">COUNTIF(H4:AA4,"○")/20</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="10"/>
+      <c r="AE4" s="3">
+        <v>2</v>
+      </c>
+      <c r="AG4" s="12">
+        <f t="shared" ref="AG4:AG36" si="1">(COUNTIF(AH4:AQ4,"○")/10)</f>
+        <v>0.7</v>
+      </c>
+      <c r="AH4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AU4" s="3">
+        <v>2</v>
+      </c>
+      <c r="AV4"/>
+      <c r="AW4"/>
+      <c r="AX4" s="12">
+        <f>(G4+AG4)/2</f>
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="G5" s="12"/>
+      <c r="H5" s="16">
+        <f>(COUNTIF(H3:H4,"○"))/2</f>
+        <v>0.5</v>
+      </c>
+      <c r="I5" s="16">
+        <f t="shared" ref="I5:AA5" si="2">(COUNTIF(I3:I4,"○"))/2</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="16">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="K5" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="16">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="M5" s="16">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="N5" s="16">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="O5" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P5" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R5" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S5" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T5" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U5" s="16">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="V5" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W5" s="16">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="X5" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Y5" s="16">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="Z5" s="16">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="AA5" s="16">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="AG5" s="12"/>
+      <c r="AH5" s="10"/>
+      <c r="AI5" s="1"/>
+      <c r="AJ5" s="1"/>
+      <c r="AK5" s="1"/>
+      <c r="AL5" s="1"/>
+      <c r="AM5" s="1"/>
+      <c r="AN5" s="1"/>
+      <c r="AO5" s="1"/>
+      <c r="AP5" s="1"/>
+      <c r="AQ5" s="1"/>
+      <c r="AX5" s="12"/>
+    </row>
+    <row r="6" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="10"/>
+      <c r="AD6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE6" s="3">
+        <v>1</v>
+      </c>
+      <c r="AG6" s="12">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="AH6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AQ6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AT6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU6" s="3">
+        <v>1</v>
+      </c>
+      <c r="AV6"/>
+      <c r="AW6"/>
+      <c r="AX6" s="12">
+        <f t="shared" ref="AX6:AX15" si="3">(G6+AG6)/2</f>
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+      <c r="G7" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="9"/>
+      <c r="AE7" s="3">
+        <v>2</v>
+      </c>
+      <c r="AG7" s="12">
+        <f t="shared" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="AH7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU7" s="3">
+        <v>2</v>
+      </c>
+      <c r="AV7"/>
+      <c r="AW7"/>
+      <c r="AX7" s="12">
+        <f t="shared" si="3"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+      <c r="G8" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="10"/>
+      <c r="AE8" s="3">
+        <v>3</v>
+      </c>
+      <c r="AG8" s="12">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="AH8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU8" s="3">
+        <v>3</v>
+      </c>
+      <c r="AV8"/>
+      <c r="AW8"/>
+      <c r="AX8" s="12">
+        <f t="shared" si="3"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C9" s="3">
+        <v>4</v>
+      </c>
+      <c r="G9" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="10"/>
+      <c r="AE9" s="3">
+        <v>4</v>
+      </c>
+      <c r="AG9" s="12">
+        <f t="shared" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="AH9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU9" s="3">
+        <v>4</v>
+      </c>
+      <c r="AV9"/>
+      <c r="AW9"/>
+      <c r="AX9" s="12">
+        <f t="shared" si="3"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C10" s="3">
+        <v>5</v>
+      </c>
+      <c r="G10" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
+      <c r="AA10" s="10"/>
+      <c r="AE10" s="3">
+        <v>5</v>
+      </c>
+      <c r="AG10" s="12">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="AH10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU10" s="3">
+        <v>5</v>
+      </c>
+      <c r="AV10"/>
+      <c r="AW10"/>
+      <c r="AX10" s="12">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C11" s="3">
+        <v>6</v>
+      </c>
+      <c r="G11" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="10"/>
+      <c r="AA11" s="10"/>
+      <c r="AE11" s="3">
+        <v>6</v>
+      </c>
+      <c r="AG11" s="12">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="AH11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU11" s="3">
+        <v>6</v>
+      </c>
+      <c r="AV11"/>
+      <c r="AW11"/>
+      <c r="AX11" s="12">
+        <f t="shared" si="3"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C12" s="3">
+        <v>7</v>
+      </c>
+      <c r="G12" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="10"/>
+      <c r="AA12" s="10"/>
+      <c r="AE12" s="3">
+        <v>7</v>
+      </c>
+      <c r="AG12" s="12">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="AH12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU12" s="3">
+        <v>7</v>
+      </c>
+      <c r="AV12"/>
+      <c r="AW12"/>
+      <c r="AX12" s="12">
+        <f t="shared" si="3"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C13" s="3">
+        <v>8</v>
+      </c>
+      <c r="G13" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="10"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="10"/>
+      <c r="AE13" s="3">
+        <v>8</v>
+      </c>
+      <c r="AG13" s="12">
+        <f t="shared" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="AH13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU13" s="3">
+        <v>8</v>
+      </c>
+      <c r="AV13"/>
+      <c r="AW13"/>
+      <c r="AX13" s="12">
+        <f t="shared" si="3"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C14" s="3">
+        <v>9</v>
+      </c>
+      <c r="G14" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="10"/>
+      <c r="AE14" s="3">
+        <v>9</v>
+      </c>
+      <c r="AG14" s="12">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="AH14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU14" s="3">
+        <v>9</v>
+      </c>
+      <c r="AV14"/>
+      <c r="AW14"/>
+      <c r="AX14" s="12">
+        <f t="shared" si="3"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C15" s="3">
+        <v>10</v>
+      </c>
+      <c r="G15" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="10"/>
+      <c r="AA15" s="10"/>
+      <c r="AE15" s="3">
+        <v>10</v>
+      </c>
+      <c r="AG15" s="12">
+        <f t="shared" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="AH15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU15" s="3">
+        <v>10</v>
+      </c>
+      <c r="AV15"/>
+      <c r="AW15"/>
+      <c r="AX15" s="12">
+        <f t="shared" si="3"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="G16" s="12"/>
+      <c r="H16" s="16">
+        <f>(COUNTIF(H6:H15,"○"))/10</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="16">
+        <f t="shared" ref="I16:AA16" si="4">(COUNTIF(I6:I15,"○"))/10</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P16" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R16" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="S16" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T16" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="U16" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V16" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="W16" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="X16" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Y16" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Z16" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AA16" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG16" s="12"/>
+      <c r="AH16" s="10"/>
+      <c r="AI16" s="1"/>
+      <c r="AJ16" s="1"/>
+      <c r="AK16" s="1"/>
+      <c r="AL16" s="1"/>
+      <c r="AM16" s="1"/>
+      <c r="AN16" s="1"/>
+      <c r="AO16" s="1"/>
+      <c r="AP16" s="1"/>
+      <c r="AQ16" s="1"/>
+      <c r="AX16" s="12"/>
+    </row>
+    <row r="17" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="G17" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="10"/>
+      <c r="AA17" s="9"/>
+      <c r="AD17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AG17" s="12">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="AH17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AT17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AV17"/>
+      <c r="AW17"/>
+      <c r="AX17" s="12">
+        <f t="shared" ref="AX17:AX30" si="5">(G17+AG17)/2</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C18" s="3">
+        <v>2</v>
+      </c>
+      <c r="G18" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="10"/>
+      <c r="AA18" s="9"/>
+      <c r="AE18" s="3">
+        <v>2</v>
+      </c>
+      <c r="AG18" s="12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AH18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU18" s="3">
+        <v>2</v>
+      </c>
+      <c r="AV18"/>
+      <c r="AW18"/>
+      <c r="AX18" s="12">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C19" s="3">
+        <v>3</v>
+      </c>
+      <c r="G19" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="10"/>
+      <c r="AA19" s="9"/>
+      <c r="AE19" s="3">
+        <v>3</v>
+      </c>
+      <c r="AG19" s="12">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="AH19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU19" s="3">
+        <v>3</v>
+      </c>
+      <c r="AV19"/>
+      <c r="AW19"/>
+      <c r="AX19" s="12">
+        <f t="shared" si="5"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C20" s="3">
+        <v>4</v>
+      </c>
+      <c r="G20" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="9"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="10"/>
+      <c r="AA20" s="9"/>
+      <c r="AE20" s="3">
+        <v>4</v>
+      </c>
+      <c r="AG20" s="12">
+        <f t="shared" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="AH20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU20" s="3">
+        <v>4</v>
+      </c>
+      <c r="AV20"/>
+      <c r="AW20"/>
+      <c r="AX20" s="12">
+        <f t="shared" si="5"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="21" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C21" s="3">
+        <v>5</v>
+      </c>
+      <c r="G21" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="10"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="10"/>
+      <c r="AA21" s="9"/>
+      <c r="AE21" s="3">
+        <v>5</v>
+      </c>
+      <c r="AG21" s="12">
+        <f t="shared" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="AH21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU21" s="3">
+        <v>5</v>
+      </c>
+      <c r="AV21"/>
+      <c r="AW21"/>
+      <c r="AX21" s="12">
+        <f t="shared" si="5"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="22" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C22" s="3">
+        <v>6</v>
+      </c>
+      <c r="G22" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="10"/>
+      <c r="Z22" s="10"/>
+      <c r="AA22" s="10"/>
+      <c r="AE22" s="3">
+        <v>6</v>
+      </c>
+      <c r="AG22" s="12">
+        <f t="shared" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="AH22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU22" s="3">
+        <v>6</v>
+      </c>
+      <c r="AV22"/>
+      <c r="AW22"/>
+      <c r="AX22" s="12">
+        <f t="shared" si="5"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="23" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C23" s="3">
+        <v>7</v>
+      </c>
+      <c r="G23" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="10"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="10"/>
+      <c r="Z23" s="10"/>
+      <c r="AA23" s="9"/>
+      <c r="AE23" s="3">
+        <v>7</v>
+      </c>
+      <c r="AG23" s="12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AH23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU23" s="3">
+        <v>7</v>
+      </c>
+      <c r="AV23"/>
+      <c r="AW23"/>
+      <c r="AX23" s="12">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C24" s="3">
+        <v>8</v>
+      </c>
+      <c r="G24" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="10"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="9"/>
+      <c r="Z24" s="10"/>
+      <c r="AA24" s="9"/>
+      <c r="AE24" s="3">
+        <v>8</v>
+      </c>
+      <c r="AG24" s="12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AH24" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI24" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ24" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK24" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL24" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM24" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN24" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO24" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP24" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ24" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU24" s="3">
+        <v>8</v>
+      </c>
+      <c r="AV24"/>
+      <c r="AW24"/>
+      <c r="AX24" s="12">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C25" s="3">
+        <v>9</v>
+      </c>
+      <c r="G25" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="9"/>
+      <c r="Y25" s="9"/>
+      <c r="Z25" s="9"/>
+      <c r="AA25" s="9"/>
+      <c r="AE25" s="3">
+        <v>9</v>
+      </c>
+      <c r="AG25" s="12">
+        <f t="shared" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="AH25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU25" s="3">
+        <v>9</v>
+      </c>
+      <c r="AV25"/>
+      <c r="AW25"/>
+      <c r="AX25" s="12">
+        <f t="shared" si="5"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="26" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C26" s="3">
+        <v>10</v>
+      </c>
+      <c r="G26" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
+      <c r="W26" s="10"/>
+      <c r="X26" s="9"/>
+      <c r="Y26" s="9"/>
+      <c r="Z26" s="9"/>
+      <c r="AA26" s="9"/>
+      <c r="AE26" s="3">
+        <v>10</v>
+      </c>
+      <c r="AG26" s="12">
+        <f t="shared" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="AH26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU26" s="3">
+        <v>10</v>
+      </c>
+      <c r="AV26"/>
+      <c r="AW26"/>
+      <c r="AX26" s="12">
+        <f t="shared" si="5"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="27" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C27" s="3">
+        <v>11</v>
+      </c>
+      <c r="G27" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+      <c r="U27" s="9"/>
+      <c r="V27" s="9"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="9"/>
+      <c r="Y27" s="9"/>
+      <c r="Z27" s="9"/>
+      <c r="AA27" s="9"/>
+      <c r="AE27" s="3">
+        <v>11</v>
+      </c>
+      <c r="AG27" s="12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AH27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU27" s="3">
+        <v>11</v>
+      </c>
+      <c r="AV27"/>
+      <c r="AW27"/>
+      <c r="AX27" s="12">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C28" s="3">
+        <v>12</v>
+      </c>
+      <c r="G28" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="9"/>
+      <c r="Y28" s="9"/>
+      <c r="Z28" s="10"/>
+      <c r="AA28" s="9"/>
+      <c r="AE28" s="3">
+        <v>12</v>
+      </c>
+      <c r="AG28" s="12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AH28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU28" s="3">
+        <v>12</v>
+      </c>
+      <c r="AV28"/>
+      <c r="AW28"/>
+      <c r="AX28" s="12">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C29" s="3">
+        <v>13</v>
+      </c>
+      <c r="G29" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="9"/>
+      <c r="U29" s="9"/>
+      <c r="V29" s="9"/>
+      <c r="W29" s="10"/>
+      <c r="X29" s="9"/>
+      <c r="Y29" s="9"/>
+      <c r="Z29" s="10"/>
+      <c r="AA29" s="9"/>
+      <c r="AE29" s="3">
+        <v>13</v>
+      </c>
+      <c r="AG29" s="12">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="AH29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AQ29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU29" s="3">
+        <v>13</v>
+      </c>
+      <c r="AV29"/>
+      <c r="AW29"/>
+      <c r="AX29" s="12">
+        <f t="shared" si="5"/>
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="30" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C30" s="3">
+        <v>14</v>
+      </c>
+      <c r="G30" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="9"/>
+      <c r="U30" s="9"/>
+      <c r="V30" s="9"/>
+      <c r="W30" s="9"/>
+      <c r="X30" s="9"/>
+      <c r="Y30" s="10"/>
+      <c r="Z30" s="10"/>
+      <c r="AA30" s="9"/>
+      <c r="AE30" s="3">
+        <v>14</v>
+      </c>
+      <c r="AG30" s="12">
+        <f t="shared" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="AH30" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI30" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ30" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK30" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM30" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN30" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO30" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP30" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ30" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU30" s="3">
+        <v>14</v>
+      </c>
+      <c r="AV30"/>
+      <c r="AW30"/>
+      <c r="AX30" s="12">
+        <f t="shared" si="5"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="31" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G31" s="5"/>
+      <c r="H31" s="15">
+        <f>(COUNTIF(H17:H30,"○"))/14</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="15">
+        <f t="shared" ref="I31:AA31" si="6">(COUNTIF(I17:I30,"○"))/14</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L31" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M31" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N31" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O31" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P31" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q31" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R31" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="S31" s="15">
+        <f>(COUNTIF(S17:S30,"○"))/14</f>
+        <v>0</v>
+      </c>
+      <c r="T31" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U31" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V31" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W31" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X31" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y31" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Z31" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AA31" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AD31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE31" s="3">
+        <v>1</v>
+      </c>
+      <c r="AG31" s="12">
+        <f t="shared" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="AH31" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI31" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ31" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK31" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL31" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM31" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN31" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO31" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP31" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ31" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AT31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AU31" s="3">
+        <v>1</v>
+      </c>
+      <c r="AV31"/>
+      <c r="AW31"/>
+      <c r="AX31" s="12">
+        <f>AG31</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="32" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G32" s="12"/>
+      <c r="AE32" s="3">
+        <v>2</v>
+      </c>
+      <c r="AG32" s="12">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="AH32" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI32" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ32" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK32" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM32" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN32" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO32" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AQ32" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU32" s="3">
+        <v>2</v>
+      </c>
+      <c r="AV32"/>
+      <c r="AW32"/>
+      <c r="AX32" s="12">
+        <f t="shared" ref="AX32:AX36" si="7">AG32</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="33" spans="30:50" x14ac:dyDescent="0.25">
+      <c r="AD33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE33" s="3">
+        <v>1</v>
+      </c>
+      <c r="AG33" s="12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AH33" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI33" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ33" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK33" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL33" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM33" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN33" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO33" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP33" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ33" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AT33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AU33" s="3">
+        <v>1</v>
+      </c>
+      <c r="AV33"/>
+      <c r="AW33"/>
+      <c r="AX33" s="12">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="30:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="AE34" s="3">
+        <v>2</v>
+      </c>
+      <c r="AG34" s="12">
+        <f t="shared" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="AH34" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI34" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ34" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK34" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL34" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM34" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN34" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO34" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP34" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ34" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU34" s="3">
+        <v>2</v>
+      </c>
+      <c r="AV34"/>
+      <c r="AW34"/>
+      <c r="AX34" s="12">
+        <f t="shared" si="7"/>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="35" spans="30:50" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="AE35" s="3">
+        <v>3</v>
+      </c>
+      <c r="AG35" s="12">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="AH35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP35" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AQ35" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AU35" s="3">
+        <v>3</v>
+      </c>
+      <c r="AV35"/>
+      <c r="AW35"/>
+      <c r="AX35" s="12">
+        <f t="shared" si="7"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="36" spans="30:50" x14ac:dyDescent="0.25">
+      <c r="AD36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE36" s="3">
+        <v>1</v>
+      </c>
+      <c r="AG36" s="12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AH36" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI36" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ36" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK36" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL36" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM36" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN36" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO36" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP36" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ36" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AT36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AU36" s="3">
+        <v>1</v>
+      </c>
+      <c r="AV36"/>
+      <c r="AW36"/>
+      <c r="AX36" s="12">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="30:50" x14ac:dyDescent="0.25">
+      <c r="AH37" s="15">
+        <f>(COUNTIF(AH3:AH36,"○")/32)</f>
+        <v>1</v>
+      </c>
+      <c r="AI37" s="15">
+        <f t="shared" ref="AI37:AQ37" si="8">(COUNTIF(AI3:AI36,"○")/32)</f>
+        <v>0.9375</v>
+      </c>
+      <c r="AJ37" s="15">
+        <f t="shared" si="8"/>
+        <v>0.9375</v>
+      </c>
+      <c r="AK37" s="15">
+        <f t="shared" si="8"/>
+        <v>0.96875</v>
+      </c>
+      <c r="AL37" s="15">
+        <f t="shared" si="8"/>
+        <v>0.59375</v>
+      </c>
+      <c r="AM37" s="15">
+        <f t="shared" si="8"/>
+        <v>0.875</v>
+      </c>
+      <c r="AN37" s="15">
+        <f t="shared" si="8"/>
+        <v>0.5625</v>
+      </c>
+      <c r="AO37" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="AP37" s="15">
+        <f t="shared" si="8"/>
+        <v>0.875</v>
+      </c>
+      <c r="AQ37" s="15">
+        <f t="shared" si="8"/>
+        <v>0.9375</v>
+      </c>
+      <c r="AV37"/>
+      <c r="AW37"/>
+    </row>
+    <row r="38" spans="30:50" x14ac:dyDescent="0.25">
+      <c r="AV38"/>
+      <c r="AW38"/>
+      <c r="AX38" s="12"/>
+    </row>
+    <row r="39" spans="30:50" x14ac:dyDescent="0.25">
+      <c r="AG39" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="H1:AA1"/>
+    <mergeCell ref="AH1:AQ1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88CCFB4E-3D94-4A97-83BE-04827B31FA43}">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" style="3" customWidth="1"/>
-    <col min="2" max="3" width="8.625" customWidth="1"/>
-    <col min="4" max="4" width="5.75" style="3" customWidth="1"/>
+    <col min="2" max="3" width="8.5703125" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" style="3" customWidth="1"/>
     <col min="5" max="21" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -5052,7 +7943,7 @@
       </c>
       <c r="T1" s="21"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -5106,7 +7997,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -5168,7 +8059,7 @@
         <v>7.7279999999999996E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3">
         <v>2</v>
@@ -5225,7 +8116,7 @@
         <v>1.6605000000000002E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>3</v>
       </c>
@@ -5284,7 +8175,7 @@
         <v>7.7279999999999996E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="3">
         <v>2</v>
@@ -5341,7 +8232,7 @@
         <v>3.5469999999999998E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="3">
         <v>3</v>
@@ -5398,7 +8289,7 @@
         <v>5.9639999999999997E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>5</v>
       </c>
@@ -5457,7 +8348,7 @@
         <v>7.0330000000000002E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="3">
         <v>2</v>
@@ -5514,7 +8405,7 @@
         <v>6.0879999999999997E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="3">
         <v>3</v>
@@ -5571,7 +8462,7 @@
         <v>7.071E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="3">
         <v>4</v>
@@ -5628,7 +8519,7 @@
         <v>3.5469999999999998E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="3">
         <v>5</v>
@@ -5685,12 +8576,12 @@
         <v>5.9639999999999997E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="12"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
@@ -5752,7 +8643,7 @@
         <v>2.9637E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="3">
         <v>2</v>
@@ -5809,7 +8700,7 @@
         <v>1.8419999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="3">
         <v>3</v>
@@ -5866,12 +8757,12 @@
         <v>2.4237999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="12"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>27</v>
       </c>
@@ -5933,7 +8824,7 @@
         <v>7.541E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="3">
         <v>2</v>
@@ -5990,7 +8881,7 @@
         <v>5.2220000000000001E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <v>4</v>
       </c>
@@ -6049,7 +8940,7 @@
         <v>1.9769999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="3">
         <v>2</v>
@@ -6106,7 +8997,7 @@
         <v>5.6049999999999997E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="3">
         <v>3</v>
@@ -6163,7 +9054,7 @@
         <v>1.9319999999999999E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="3">
         <v>4</v>
@@ -6220,31 +9111,31 @@
         <v>4.1510000000000002E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="5"/>

</xml_diff>

<commit_message>
[move] organized experiment data
</commit_message>
<xml_diff>
--- a/Experiment-Data/Answer-Data.xlsx
+++ b/Experiment-Data/Answer-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC_User\Desktop\eye-tracking-software\Experiment-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93E7A11-1ADB-4B52-88E1-F9928BEDEA0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D73BD0F-D6D5-4E86-AA23-FA8B29497E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{65F65776-174E-4145-8CCF-AA6B8A50F68A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{65F65776-174E-4145-8CCF-AA6B8A50F68A}"/>
   </bookViews>
   <sheets>
     <sheet name="1st" sheetId="1" r:id="rId1"/>
@@ -644,7 +644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C853D4-11AD-448C-900A-323815755F36}">
   <dimension ref="A1:AX39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -4995,7 +4995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CCB7AF-21A6-41ED-886C-DD886AE34E4A}">
   <dimension ref="A1:AX40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="AX36" sqref="AX36"/>
     </sheetView>
   </sheetViews>
@@ -8316,7 +8316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88CCFB4E-3D94-4A97-83BE-04827B31FA43}">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>

</xml_diff>

<commit_message>
[fix] fixed several data
</commit_message>
<xml_diff>
--- a/Experiment-Data/Answer-Data.xlsx
+++ b/Experiment-Data/Answer-Data.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\www\Desktop\eye-tracking-software\Experiment-Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC_User\Desktop\eye-tracking-software\Experiment-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A7508B-86C8-42C6-8A40-439979953893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0B7A31-2822-430E-AD49-FDC18F000B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{65F65776-174E-4145-8CCF-AA6B8A50F68A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{65F65776-174E-4145-8CCF-AA6B8A50F68A}"/>
   </bookViews>
   <sheets>
-    <sheet name="1st" sheetId="1" r:id="rId1"/>
-    <sheet name="1st-Features" sheetId="2" r:id="rId2"/>
-    <sheet name="2nd" sheetId="3" r:id="rId3"/>
+    <sheet name="1st-Scores" sheetId="1" r:id="rId1"/>
+    <sheet name="1st-E-Data" sheetId="2" r:id="rId2"/>
+    <sheet name="2nd-Scores" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -176,13 +176,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="176" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -194,7 +194,7 @@
     </font>
     <font>
       <sz val="6"/>
-      <name val="Aptos Narrow"/>
+      <name val="游ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -244,6 +244,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -271,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -320,36 +326,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -357,8 +350,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,30 +690,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C853D4-11AD-448C-900A-323815755F36}">
-  <dimension ref="A1:BB44"/>
+  <dimension ref="A1:BB42"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T35" sqref="T35"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10" style="3" customWidth="1"/>
-    <col min="2" max="3" width="4.28515625" style="3" customWidth="1"/>
-    <col min="4" max="7" width="5.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" style="13" customWidth="1"/>
-    <col min="9" max="28" width="4.42578125" style="2" customWidth="1"/>
-    <col min="29" max="29" width="4.140625" style="3" customWidth="1"/>
+    <col min="2" max="3" width="4.25" style="3" customWidth="1"/>
+    <col min="4" max="7" width="5.75" style="3" customWidth="1"/>
+    <col min="8" max="8" width="6.25" style="13" customWidth="1"/>
+    <col min="9" max="28" width="4.375" style="2" customWidth="1"/>
+    <col min="29" max="29" width="4.125" style="3" customWidth="1"/>
     <col min="30" max="30" width="10" style="3" customWidth="1"/>
-    <col min="31" max="32" width="4.28515625" style="3" customWidth="1"/>
-    <col min="33" max="35" width="5.7109375" style="3" customWidth="1"/>
-    <col min="36" max="36" width="6.140625" style="3" customWidth="1"/>
-    <col min="37" max="46" width="4.42578125" style="4" customWidth="1"/>
-    <col min="47" max="47" width="4.140625" customWidth="1"/>
+    <col min="31" max="32" width="4.25" style="3" customWidth="1"/>
+    <col min="33" max="35" width="5.75" style="3" customWidth="1"/>
+    <col min="36" max="36" width="6.125" style="3" customWidth="1"/>
+    <col min="37" max="46" width="4.375" style="4" customWidth="1"/>
+    <col min="47" max="47" width="4.125" customWidth="1"/>
     <col min="48" max="48" width="10" style="3" customWidth="1"/>
-    <col min="49" max="50" width="4.28515625" style="3" customWidth="1"/>
-    <col min="51" max="53" width="5.7109375" style="3" customWidth="1"/>
-    <col min="54" max="54" width="6.140625" style="3" customWidth="1"/>
+    <col min="49" max="50" width="4.25" style="3" customWidth="1"/>
+    <col min="51" max="53" width="5.75" style="3" customWidth="1"/>
+    <col min="54" max="54" width="6.125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:54" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -745,28 +741,28 @@
       <c r="H1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
       <c r="AC1" s="5"/>
       <c r="AD1" s="5" t="s">
         <v>10</v>
@@ -789,18 +785,18 @@
       <c r="AJ1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="AK1" s="19" t="s">
+      <c r="AK1" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="AL1" s="19"/>
-      <c r="AM1" s="19"/>
-      <c r="AN1" s="19"/>
-      <c r="AO1" s="19"/>
-      <c r="AP1" s="19"/>
-      <c r="AQ1" s="19"/>
-      <c r="AR1" s="19"/>
-      <c r="AS1" s="19"/>
-      <c r="AT1" s="19"/>
+      <c r="AL1" s="23"/>
+      <c r="AM1" s="23"/>
+      <c r="AN1" s="23"/>
+      <c r="AO1" s="23"/>
+      <c r="AP1" s="23"/>
+      <c r="AQ1" s="23"/>
+      <c r="AR1" s="23"/>
+      <c r="AS1" s="23"/>
+      <c r="AT1" s="23"/>
       <c r="AV1" s="5" t="s">
         <v>10</v>
       </c>
@@ -938,7 +934,7 @@
       <c r="BA2" s="5"/>
       <c r="BB2" s="5"/>
     </row>
-    <row r="3" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1099,7 +1095,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="4" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C4" s="3">
         <v>2</v>
       </c>
@@ -1242,7 +1238,7 @@
         <v>0.52499999999999991</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.4">
       <c r="H5" s="12"/>
       <c r="I5" s="16">
         <f>(COUNTIF(I3:I4,"○"))/2</f>
@@ -1337,7 +1333,7 @@
       <c r="AT5" s="1"/>
       <c r="BB5" s="12"/>
     </row>
-    <row r="6" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.4">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1485,11 +1481,11 @@
         <v>2</v>
       </c>
       <c r="BB6" s="12">
-        <f>(H6+AJ6)/2</f>
+        <f t="shared" ref="BB6:BB15" si="3">(H6+AJ6)/2</f>
         <v>0.85</v>
       </c>
     </row>
-    <row r="7" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C7" s="3">
         <v>2</v>
       </c>
@@ -1628,11 +1624,11 @@
         <v>3</v>
       </c>
       <c r="BB7" s="12">
-        <f>(H7+AJ7)/2</f>
+        <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C8" s="3">
         <v>3</v>
       </c>
@@ -1771,11 +1767,11 @@
         <v>1</v>
       </c>
       <c r="BB8" s="12">
-        <f>(H8+AJ8)/2</f>
+        <f t="shared" si="3"/>
         <v>0.875</v>
       </c>
     </row>
-    <row r="9" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C9" s="3">
         <v>4</v>
       </c>
@@ -1914,11 +1910,11 @@
         <v>2</v>
       </c>
       <c r="BB9" s="12">
-        <f>(H9+AJ9)/2</f>
+        <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C10" s="3">
         <v>5</v>
       </c>
@@ -2057,11 +2053,11 @@
         <v>4</v>
       </c>
       <c r="BB10" s="12">
-        <f>(H10+AJ10)/2</f>
+        <f t="shared" si="3"/>
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C11" s="3">
         <v>6</v>
       </c>
@@ -2200,11 +2196,11 @@
         <v>4</v>
       </c>
       <c r="BB11" s="12">
-        <f>(H11+AJ11)/2</f>
+        <f t="shared" si="3"/>
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C12" s="3">
         <v>7</v>
       </c>
@@ -2343,11 +2339,11 @@
         <v>3</v>
       </c>
       <c r="BB12" s="12">
-        <f>(H12+AJ12)/2</f>
+        <f t="shared" si="3"/>
         <v>0.67500000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C13" s="3">
         <v>8</v>
       </c>
@@ -2486,11 +2482,11 @@
         <v>3</v>
       </c>
       <c r="BB13" s="12">
-        <f>(H13+AJ13)/2</f>
+        <f t="shared" si="3"/>
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C14" s="3">
         <v>9</v>
       </c>
@@ -2629,11 +2625,11 @@
         <v>4</v>
       </c>
       <c r="BB14" s="12">
-        <f>(H14+AJ14)/2</f>
+        <f t="shared" si="3"/>
         <v>0.72500000000000009</v>
       </c>
     </row>
-    <row r="15" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C15" s="3">
         <v>10</v>
       </c>
@@ -2772,90 +2768,90 @@
         <v>3</v>
       </c>
       <c r="BB15" s="12">
-        <f>(H15+AJ15)/2</f>
+        <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
     </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" x14ac:dyDescent="0.4">
       <c r="H16" s="12"/>
       <c r="I16" s="16">
         <f>(COUNTIF(I6:I15,"○"))/10</f>
         <v>0.6</v>
       </c>
       <c r="J16" s="16">
-        <f t="shared" ref="J16:AB16" si="3">(COUNTIF(J6:J15,"○"))/10</f>
+        <f t="shared" ref="J16:AB16" si="4">(COUNTIF(J6:J15,"○"))/10</f>
         <v>0.4</v>
       </c>
       <c r="K16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
       <c r="L16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
       <c r="M16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="N16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
       <c r="O16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="P16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
       <c r="R16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
       <c r="S16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="T16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.9</v>
       </c>
       <c r="U16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
       <c r="V16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.9</v>
       </c>
       <c r="W16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
       <c r="X16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
       <c r="Y16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Z16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.9</v>
       </c>
       <c r="AA16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
       <c r="AB16" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.9</v>
       </c>
       <c r="AJ16" s="12"/>
@@ -2871,7 +2867,7 @@
       <c r="AT16" s="1"/>
       <c r="BB16" s="12"/>
     </row>
-    <row r="17" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:54" x14ac:dyDescent="0.4">
       <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
@@ -3019,11 +3015,11 @@
         <v>3</v>
       </c>
       <c r="BB17" s="12">
-        <f>(H17+AJ17)/2</f>
+        <f t="shared" ref="BB17:BB30" si="5">(H17+AJ17)/2</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C18" s="3">
         <v>2</v>
       </c>
@@ -3162,11 +3158,11 @@
         <v>3</v>
       </c>
       <c r="BB18" s="12">
-        <f>(H18+AJ18)/2</f>
+        <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
     </row>
-    <row r="19" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C19" s="3">
         <v>3</v>
       </c>
@@ -3305,11 +3301,11 @@
         <v>4</v>
       </c>
       <c r="BB19" s="12">
-        <f>(H19+AJ19)/2</f>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C20" s="3">
         <v>4</v>
       </c>
@@ -3448,11 +3444,11 @@
         <v>4</v>
       </c>
       <c r="BB20" s="12">
-        <f>(H20+AJ20)/2</f>
+        <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
     </row>
-    <row r="21" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C21" s="3">
         <v>5</v>
       </c>
@@ -3591,11 +3587,11 @@
         <v>1</v>
       </c>
       <c r="BB21" s="12">
-        <f>(H21+AJ21)/2</f>
+        <f t="shared" si="5"/>
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C22" s="3">
         <v>6</v>
       </c>
@@ -3734,11 +3730,11 @@
         <v>3</v>
       </c>
       <c r="BB22" s="12">
-        <f>(H22+AJ22)/2</f>
+        <f t="shared" si="5"/>
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C23" s="3">
         <v>7</v>
       </c>
@@ -3877,11 +3873,11 @@
         <v>2</v>
       </c>
       <c r="BB23" s="12">
-        <f>(H23+AJ23)/2</f>
+        <f t="shared" si="5"/>
         <v>0.625</v>
       </c>
     </row>
-    <row r="24" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C24" s="3">
         <v>8</v>
       </c>
@@ -4020,11 +4016,11 @@
         <v>1</v>
       </c>
       <c r="BB24" s="12">
-        <f>(H24+AJ24)/2</f>
+        <f t="shared" si="5"/>
         <v>0.625</v>
       </c>
     </row>
-    <row r="25" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C25" s="3">
         <v>9</v>
       </c>
@@ -4163,11 +4159,11 @@
         <v>4</v>
       </c>
       <c r="BB25" s="12">
-        <f>(H25+AJ25)/2</f>
+        <f t="shared" si="5"/>
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C26" s="3">
         <v>10</v>
       </c>
@@ -4306,11 +4302,11 @@
         <v>4</v>
       </c>
       <c r="BB26" s="12">
-        <f>(H26+AJ26)/2</f>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C27" s="3">
         <v>11</v>
       </c>
@@ -4449,11 +4445,11 @@
         <v>3</v>
       </c>
       <c r="BB27" s="12">
-        <f>(H27+AJ27)/2</f>
+        <f t="shared" si="5"/>
         <v>0.52500000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C28" s="3">
         <v>12</v>
       </c>
@@ -4592,11 +4588,11 @@
         <v>3</v>
       </c>
       <c r="BB28" s="12">
-        <f>(H28+AJ28)/2</f>
+        <f t="shared" si="5"/>
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="29" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C29" s="3">
         <v>13</v>
       </c>
@@ -4735,11 +4731,11 @@
         <v>4</v>
       </c>
       <c r="BB29" s="12">
-        <f>(H29+AJ29)/2</f>
+        <f t="shared" si="5"/>
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C30" s="3">
         <v>14</v>
       </c>
@@ -4878,54 +4874,54 @@
         <v>3</v>
       </c>
       <c r="BB30" s="12">
-        <f>(H30+AJ30)/2</f>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:54" x14ac:dyDescent="0.4">
       <c r="H31" s="5"/>
       <c r="I31" s="15">
         <f>(COUNTIF(I17:I30,"○"))/14</f>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="J31" s="15">
-        <f t="shared" ref="J31:AB31" si="4">(COUNTIF(J17:J30,"○"))/14</f>
+        <f t="shared" ref="J31:AB31" si="6">(COUNTIF(J17:J30,"○"))/14</f>
         <v>0.14285714285714285</v>
       </c>
       <c r="K31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.42857142857142855</v>
       </c>
       <c r="L31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="M31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.35714285714285715</v>
       </c>
       <c r="N31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="O31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.35714285714285715</v>
       </c>
       <c r="P31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="Q31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="T31" s="15">
@@ -4933,35 +4929,35 @@
         <v>0</v>
       </c>
       <c r="U31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="W31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="X31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="Y31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Z31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.35714285714285715</v>
       </c>
       <c r="AA31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.7857142857142857</v>
       </c>
       <c r="AB31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="AE31" s="3" t="s">
@@ -5033,26 +5029,26 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="32" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:54" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C32" s="3">
         <v>1</v>
       </c>
-      <c r="D32" s="21">
+      <c r="D32" s="12">
         <f>AVERAGE(H3,H6,H8,H9,H19,H21,H23,H24,H26)</f>
         <v>0.46666666666666667</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="12">
         <f>AVERAGE(H3,H6,H8,H9,H19,H21,H23,H24,H26)</f>
         <v>0.46666666666666667</v>
       </c>
-      <c r="F32" s="21">
+      <c r="F32" s="12">
         <f>AVERAGE(H8,H9,H21,H24)</f>
         <v>0.53749999999999998</v>
       </c>
-      <c r="G32" s="21">
+      <c r="G32" s="12">
         <f>AVERAGE(H8,H9,H24,H21)</f>
         <v>0.53749999999999998</v>
       </c>
@@ -5116,27 +5112,27 @@
         <v>1</v>
       </c>
       <c r="BB32" s="12">
-        <f t="shared" ref="BB32:BB36" si="5">AJ32</f>
+        <f t="shared" ref="BB32:BB36" si="7">AJ32</f>
         <v>0.8</v>
       </c>
     </row>
-    <row r="33" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C33" s="3">
         <v>2</v>
       </c>
-      <c r="D33" s="21">
+      <c r="D33" s="12">
         <f>AVERAGE(H4,H7,H10,H11,H12,H13,H14,H15,H17,H18,H20,H22,H25,H27,H28,H29,H30)</f>
         <v>0.41176470588235298</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="12">
         <f>AVERAGE(H4,H7,H12,H13,H17,H18,H22,H27,H28)</f>
         <v>0.37222222222222223</v>
       </c>
-      <c r="F33" s="21">
+      <c r="F33" s="12">
         <f>AVERAGE(H3,H6,H19,H23,H26)</f>
         <v>0.41</v>
       </c>
-      <c r="G33" s="21">
+      <c r="G33" s="12">
         <f>AVERAGE(H3,H6,H19,H23,H26)</f>
         <v>0.41</v>
       </c>
@@ -5205,24 +5201,23 @@
         <v>1</v>
       </c>
       <c r="BB33" s="12">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C34" s="3">
         <v>3</v>
       </c>
-      <c r="D34" s="22"/>
-      <c r="E34" s="21">
+      <c r="E34" s="12">
         <f>AVERAGE(H10,H11,H14,H15,H20,H25,H29,H30)</f>
         <v>0.45624999999999999</v>
       </c>
-      <c r="F34" s="21">
+      <c r="F34" s="12">
         <f>AVERAGE(H4,H7,H12,H13,H17,H18,H22,H27,H28)</f>
         <v>0.37222222222222223</v>
       </c>
-      <c r="G34" s="21">
+      <c r="G34" s="12">
         <f>AVERAGE(H4,H7,H12,H13,H17,H18,H22,H27,H28)</f>
         <v>0.37222222222222223</v>
       </c>
@@ -5285,21 +5280,19 @@
         <v>2</v>
       </c>
       <c r="BB34" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.9</v>
       </c>
     </row>
-    <row r="35" spans="1:54" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C35" s="3">
         <v>4</v>
       </c>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="21">
+      <c r="F35" s="12">
         <f>AVERAGE(H10,H11,H14,H15,H20,H25,H29,H30)</f>
         <v>0.45624999999999999</v>
       </c>
-      <c r="G35" s="21">
+      <c r="G35" s="12">
         <f>AVERAGE(H14,H15,H20,H25)</f>
         <v>0.51250000000000007</v>
       </c>
@@ -5362,18 +5355,15 @@
         <v>3</v>
       </c>
       <c r="BB35" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.8</v>
       </c>
     </row>
-    <row r="36" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:54" x14ac:dyDescent="0.4">
       <c r="C36" s="3">
         <v>5</v>
       </c>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="21">
+      <c r="G36" s="12">
         <f>AVERAGE(H10,H11,H29,H30)</f>
         <v>0.4</v>
       </c>
@@ -5442,27 +5432,27 @@
         <v>1</v>
       </c>
       <c r="BB36" s="12">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:54" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:54" x14ac:dyDescent="0.4">
       <c r="A37" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="23">
+      <c r="D37" s="18">
         <f>_xlfn.STDEV.P(D32:D33)</f>
         <v>2.7450980392156848E-2</v>
       </c>
-      <c r="E37" s="23">
+      <c r="E37" s="18">
         <f>_xlfn.STDEV.P(E32:E34)</f>
         <v>4.2280712005378474E-2</v>
       </c>
-      <c r="F37" s="23">
+      <c r="F37" s="18">
         <f>_xlfn.STDEV.P(F32:F35)</f>
         <v>6.1644873448273775E-2</v>
       </c>
-      <c r="G37" s="26">
+      <c r="G37" s="19">
         <f>_xlfn.STDEV.P(G32:G36)</f>
         <v>6.5800718597149824E-2</v>
       </c>
@@ -5471,61 +5461,61 @@
         <v>1</v>
       </c>
       <c r="AL37" s="15">
-        <f t="shared" ref="AL37:AT37" si="6">(COUNTIF(AL3:AL36,"○")/32)</f>
+        <f t="shared" ref="AL37:AT37" si="8">(COUNTIF(AL3:AL36,"○")/32)</f>
         <v>0.9375</v>
       </c>
       <c r="AM37" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.9375</v>
       </c>
       <c r="AN37" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.96875</v>
       </c>
       <c r="AO37" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.59375</v>
       </c>
       <c r="AP37" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.875</v>
       </c>
       <c r="AQ37" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.5625</v>
       </c>
       <c r="AR37" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AS37" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.875</v>
       </c>
       <c r="AT37" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.9375</v>
       </c>
       <c r="AY37"/>
       <c r="AZ37"/>
       <c r="BA37"/>
     </row>
-    <row r="38" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:54" x14ac:dyDescent="0.4">
       <c r="AD38" s="3" t="s">
         <v>23</v>
       </c>
       <c r="AF38" s="3">
         <v>1</v>
       </c>
-      <c r="AG38" s="21">
+      <c r="AG38" s="12">
         <f>AVERAGE(AJ3,AJ6:AJ7,AJ9:AJ11,AJ14,AJ17,AJ25:AJ26,AJ29,AJ35)</f>
         <v>0.80833333333333324</v>
       </c>
-      <c r="AH38" s="21">
+      <c r="AH38" s="12">
         <f>AVERAGE(AJ3,AJ6,AJ7,AJ9:AJ11,AJ14,AJ17,AJ25:AJ26,AJ29,AJ35)</f>
         <v>0.80833333333333324</v>
       </c>
-      <c r="AI38" s="21">
+      <c r="AI38" s="12">
         <f>AVERAGE(AJ29,AJ26,AJ25,AJ9,AJ11)</f>
         <v>0.84000000000000008</v>
       </c>
@@ -5535,33 +5525,33 @@
       <c r="AX38" s="3">
         <v>1</v>
       </c>
-      <c r="AY38" s="21">
+      <c r="AY38" s="12">
         <f>AVERAGE(BB36,BB31:BB34,BB24,BB23,BB21,BB9,BB8,BB6,BB3)</f>
         <v>0.8041666666666667</v>
       </c>
-      <c r="AZ38" s="21">
+      <c r="AZ38" s="12">
         <f>AVERAGE(BB36,BB31:BB34,BB23:BB24,BB21,BB8:BB9,BB6,BB3)</f>
         <v>0.8041666666666667</v>
       </c>
-      <c r="BA38" s="21">
+      <c r="BA38" s="12">
         <f>AVERAGE(BB36,BB33,BB32,BB24,BB21,BB8)</f>
         <v>0.8125</v>
       </c>
       <c r="BB38" s="12"/>
     </row>
-    <row r="39" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:54" x14ac:dyDescent="0.4">
       <c r="AF39" s="3">
         <v>2</v>
       </c>
-      <c r="AG39" s="21">
+      <c r="AG39" s="12">
         <f>AVERAGE(AJ4,AJ8,AJ12:AJ13,AJ15,AJ18:AJ24,AJ27,AJ28,AJ30,AJ31,AJ32,AJ33,AJ34,AJ36)</f>
         <v>0.90500000000000003</v>
       </c>
-      <c r="AH39" s="21">
+      <c r="AH39" s="12">
         <f>AVERAGE(AJ4,AJ8,AJ20:AJ21,AJ23:AJ24,AJ27:AJ28,AJ30:AJ32,AJ34)</f>
         <v>0.9</v>
       </c>
-      <c r="AI39" s="21">
+      <c r="AI39" s="12">
         <f>AVERAGE(AJ3,AJ6,AJ7,AJ10,AJ14,AJ17,AJ35)</f>
         <v>0.7857142857142857</v>
       </c>
@@ -5569,112 +5559,90 @@
       <c r="AX39" s="3">
         <v>2</v>
       </c>
-      <c r="AY39" s="21">
+      <c r="AY39" s="12">
         <f>AVERAGE(BB35,BB25:BB30,BB22,BB18:BB20,BB17,BB15,BB10:BB14,BB7,BB4)</f>
         <v>0.62749999999999995</v>
       </c>
-      <c r="AZ39" s="21">
+      <c r="AZ39" s="12">
         <f>AVERAGE(BB35,BB30,BB27:BB28,BB22,BB17:BB18,BB15,BB12:BB13,BB7,BB4)</f>
         <v>0.65625</v>
       </c>
-      <c r="BA39" s="21">
+      <c r="BA39" s="12">
         <f>AVERAGE(BB34,BB31,BB23,BB6,BB9,BB3)</f>
         <v>0.79583333333333339</v>
       </c>
     </row>
-    <row r="40" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:54" x14ac:dyDescent="0.4">
       <c r="AF40" s="3">
         <v>3</v>
       </c>
-      <c r="AG40" s="22"/>
-      <c r="AH40" s="21">
+      <c r="AH40" s="12">
         <f>AVERAGE(AJ36,AJ33,AJ22,AJ18:AJ19,AJ15,AJ12,AJ13)</f>
         <v>0.91250000000000009</v>
       </c>
-      <c r="AI40" s="21">
+      <c r="AI40" s="12">
         <f>AVERAGE(AJ4,AJ8,AJ20:AJ21,AJ23,AJ24,AJ27,AJ28,AJ30,AJ31,AJ32,AJ34)</f>
         <v>0.9</v>
       </c>
       <c r="AX40" s="3">
         <v>3</v>
       </c>
-      <c r="AY40" s="22"/>
-      <c r="AZ40" s="21">
+      <c r="AZ40" s="12">
         <f>AVERAGE(BB29,BB25:BB26,BB20,BB19,BB14,BB11,BB10)</f>
         <v>0.58437499999999998</v>
       </c>
-      <c r="BA40" s="21">
+      <c r="BA40" s="12">
         <f>AVERAGE(BB35,BB30,BB28,BB27,BB22,BB18,BB17,BB15,BB13,BB12,BB7,BB4)</f>
         <v>0.65625000000000011</v>
       </c>
     </row>
-    <row r="41" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:54" x14ac:dyDescent="0.4">
       <c r="AF41" s="3">
         <v>4</v>
       </c>
-      <c r="AG41" s="22"/>
-      <c r="AH41" s="22"/>
-      <c r="AI41" s="21">
+      <c r="AI41" s="12">
         <f>AVERAGE(AJ12,AJ13,AJ15,AJ18:AJ19,AJ22,AJ33,AJ36)</f>
         <v>0.91250000000000009</v>
       </c>
       <c r="AX41" s="3">
         <v>4</v>
       </c>
-      <c r="AY41" s="22"/>
-      <c r="AZ41" s="22"/>
-      <c r="BA41" s="21">
+      <c r="BA41" s="12">
         <f>AVERAGE(BB29,BB26,BB25,BB20,BB19,BB14,BB11,BB10)</f>
         <v>0.58437499999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:54" x14ac:dyDescent="0.4">
       <c r="AD42" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AG42" s="24">
+      <c r="AG42" s="18">
         <f>_xlfn.STDEV.P(AG38:AG39)</f>
         <v>4.8333333333333395E-2</v>
       </c>
-      <c r="AH42" s="24">
+      <c r="AH42" s="18">
         <f>_xlfn.STDEV.P(AH38:AH40)</f>
         <v>4.643959304805699E-2</v>
       </c>
-      <c r="AI42" s="25">
+      <c r="AI42" s="19">
         <f>_xlfn.STDEV.P(AI38:AI41)</f>
         <v>5.0679927370363392E-2</v>
       </c>
       <c r="AV42" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AY42" s="24">
+      <c r="AY42" s="18">
         <f>_xlfn.STDEV.P(AY38:AY39)</f>
         <v>8.8333333333332972E-2</v>
       </c>
-      <c r="AZ42" s="24">
+      <c r="AZ42" s="18">
         <f>_xlfn.STDEV.P(AZ38:AZ40)</f>
         <v>9.1502114510412499E-2</v>
       </c>
-      <c r="BA42" s="25">
+      <c r="BA42" s="19">
         <f>_xlfn.STDEV.P(BA38:BA41)</f>
         <v>9.5556594882409335E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="AG43" s="22"/>
-      <c r="AH43" s="22"/>
-      <c r="AI43" s="22"/>
-      <c r="AY43" s="22"/>
-      <c r="AZ43" s="22"/>
-      <c r="BA43" s="22"/>
-    </row>
-    <row r="44" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="AG44" s="22"/>
-      <c r="AH44" s="22"/>
-      <c r="AI44" s="22"/>
-      <c r="AY44" s="22"/>
-      <c r="AZ44" s="22"/>
-      <c r="BA44" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5689,137 +5657,120 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88CCFB4E-3D94-4A97-83BE-04827B31FA43}">
-  <dimension ref="A1:W40"/>
+  <dimension ref="A1:V40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.375" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="10" style="3" customWidth="1"/>
-    <col min="5" max="5" width="3.5703125" customWidth="1"/>
+    <col min="5" max="5" width="3.625" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="3.5703125" customWidth="1"/>
+    <col min="9" max="9" width="3.625" customWidth="1"/>
     <col min="10" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="3.5703125" customWidth="1"/>
+    <col min="14" max="14" width="3.625" customWidth="1"/>
     <col min="15" max="19" width="10" customWidth="1"/>
-    <col min="20" max="20" width="3.5703125" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" customWidth="1"/>
-    <col min="23" max="23" width="9.140625" customWidth="1"/>
+    <col min="20" max="20" width="3.625" customWidth="1"/>
+    <col min="21" max="21" width="9.125" customWidth="1"/>
+    <col min="23" max="23" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-    </row>
-    <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1"/>
+    </row>
+    <row r="2" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="28">
-        <v>2</v>
-      </c>
-      <c r="D2" s="28"/>
+      <c r="C2" s="26">
+        <v>2</v>
+      </c>
+      <c r="D2" s="26"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="28">
+      <c r="F2" s="26">
         <v>3</v>
       </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="28">
+      <c r="J2" s="26">
         <v>4</v>
       </c>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
       <c r="N2" s="3"/>
-      <c r="O2" s="28">
+      <c r="O2" s="26">
         <v>5</v>
       </c>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="28" t="s">
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="V2" s="28"/>
-      <c r="W2" s="20"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="V2" s="26"/>
+    </row>
+    <row r="3" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="3">
-        <v>2</v>
-      </c>
-      <c r="H3" s="3">
+      <c r="C3" s="27">
+        <v>1</v>
+      </c>
+      <c r="D3" s="27">
+        <v>2</v>
+      </c>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27">
+        <v>1</v>
+      </c>
+      <c r="G3" s="27">
+        <v>2</v>
+      </c>
+      <c r="H3" s="27">
         <v>3</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3">
-        <v>1</v>
-      </c>
-      <c r="K3" s="3">
-        <v>2</v>
-      </c>
-      <c r="L3" s="3">
+      <c r="I3" s="27"/>
+      <c r="J3" s="27">
+        <v>1</v>
+      </c>
+      <c r="K3" s="27">
+        <v>2</v>
+      </c>
+      <c r="L3" s="27">
         <v>3</v>
       </c>
-      <c r="M3" s="3">
+      <c r="M3" s="27">
         <v>4</v>
       </c>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3">
-        <v>1</v>
-      </c>
-      <c r="P3" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="3">
+      <c r="N3" s="27"/>
+      <c r="O3" s="27">
+        <v>1</v>
+      </c>
+      <c r="P3" s="27">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="27">
         <v>3</v>
       </c>
-      <c r="R3" s="3">
+      <c r="R3" s="27">
         <v>4</v>
       </c>
-      <c r="S3" s="5">
+      <c r="S3" s="27">
         <v>5</v>
       </c>
       <c r="T3" s="8"/>
@@ -5830,65 +5781,65 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="21">
+      <c r="C4" s="12">
         <v>0.47</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="12">
         <v>0.41</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21">
+      <c r="E4" s="12"/>
+      <c r="F4" s="12">
         <v>0.47000000000000003</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="12">
         <v>0.37</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="12">
         <v>0.46</v>
       </c>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21">
+      <c r="I4" s="12"/>
+      <c r="J4" s="12">
         <v>0.54</v>
       </c>
-      <c r="K4" s="21">
+      <c r="K4" s="12">
         <v>0.41000000000000003</v>
       </c>
-      <c r="L4" s="21">
+      <c r="L4" s="12">
         <v>0.37</v>
       </c>
-      <c r="M4" s="21">
+      <c r="M4" s="12">
         <v>0.46</v>
       </c>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21">
+      <c r="N4" s="12"/>
+      <c r="O4" s="12">
         <v>0.54</v>
       </c>
-      <c r="P4" s="21">
+      <c r="P4" s="12">
         <v>0.41000000000000003</v>
       </c>
-      <c r="Q4" s="21">
+      <c r="Q4" s="12">
         <v>0.37</v>
       </c>
-      <c r="R4" s="21">
+      <c r="R4" s="12">
         <v>0.51</v>
       </c>
-      <c r="S4" s="21">
+      <c r="S4" s="12">
         <v>0.4</v>
       </c>
       <c r="T4" s="8"/>
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
     </row>
-    <row r="5" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+    <row r="5" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C5">
@@ -5933,16 +5884,16 @@
       <c r="S5">
         <v>8290</v>
       </c>
-      <c r="U5" s="29">
+      <c r="U5" s="24">
         <v>0.432672</v>
       </c>
-      <c r="V5" s="29">
+      <c r="V5" s="24">
         <v>0.31031199999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="31" t="s">
+    <row r="6" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="25"/>
+      <c r="B6" s="21" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="17">
@@ -5987,12 +5938,12 @@
       <c r="S6" s="17">
         <v>1305614</v>
       </c>
-      <c r="U6" s="29"/>
-      <c r="V6" s="29"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="31" t="s">
+      <c r="U6" s="24"/>
+      <c r="V6" s="24"/>
+    </row>
+    <row r="7" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="25"/>
+      <c r="B7" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C7">
@@ -6051,14 +6002,14 @@
         <f t="shared" si="0"/>
         <v>1142.6346747758007</v>
       </c>
-      <c r="U7" s="29"/>
-      <c r="V7" s="29"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="U7" s="24"/>
+      <c r="V7" s="24"/>
+    </row>
+    <row r="8" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C8">
@@ -6103,16 +6054,16 @@
       <c r="S8">
         <v>171.08226999999999</v>
       </c>
-      <c r="U8" s="29">
+      <c r="U8" s="24">
         <v>-0.383185</v>
       </c>
-      <c r="V8" s="29">
+      <c r="V8" s="24">
         <v>0.373394</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="31" t="s">
+    <row r="9" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="25"/>
+      <c r="B9" s="21" t="s">
         <v>30</v>
       </c>
       <c r="C9">
@@ -6157,12 +6108,12 @@
       <c r="S9">
         <v>714.98308499999996</v>
       </c>
-      <c r="U9" s="29"/>
-      <c r="V9" s="29"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="31" t="s">
+      <c r="U9" s="24"/>
+      <c r="V9" s="24"/>
+    </row>
+    <row r="10" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="25"/>
+      <c r="B10" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C10">
@@ -6221,14 +6172,14 @@
         <f t="shared" si="1"/>
         <v>26.739167619804473</v>
       </c>
-      <c r="U10" s="29"/>
-      <c r="V10" s="29"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
+    </row>
+    <row r="11" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C11">
@@ -6273,16 +6224,16 @@
       <c r="S11">
         <v>1126.640887</v>
       </c>
-      <c r="U11" s="29">
+      <c r="U11" s="24">
         <v>-0.106474</v>
       </c>
-      <c r="V11" s="29">
+      <c r="V11" s="24">
         <v>0.34509499999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="31" t="s">
+    <row r="12" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="25"/>
+      <c r="B12" s="21" t="s">
         <v>30</v>
       </c>
       <c r="C12">
@@ -6327,12 +6278,12 @@
       <c r="S12">
         <v>140939.082222</v>
       </c>
-      <c r="U12" s="29"/>
-      <c r="V12" s="29"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="31" t="s">
+      <c r="U12" s="24"/>
+      <c r="V12" s="24"/>
+    </row>
+    <row r="13" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="25"/>
+      <c r="B13" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C13">
@@ -6391,14 +6342,14 @@
         <f t="shared" si="2"/>
         <v>375.41854272531612</v>
       </c>
-      <c r="U13" s="29"/>
-      <c r="V13" s="29"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
+      <c r="U13" s="24"/>
+      <c r="V13" s="24"/>
+    </row>
+    <row r="14" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C14">
@@ -6443,16 +6394,16 @@
       <c r="S14">
         <v>1297</v>
       </c>
-      <c r="U14" s="29">
+      <c r="U14" s="24">
         <v>0.47118300000000002</v>
       </c>
-      <c r="V14" s="29">
+      <c r="V14" s="24">
         <v>0.17700099999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="B15" s="31" t="s">
+    <row r="15" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="25"/>
+      <c r="B15" s="21" t="s">
         <v>30</v>
       </c>
       <c r="C15">
@@ -6497,12 +6448,12 @@
       <c r="S15">
         <v>11906</v>
       </c>
-      <c r="U15" s="29"/>
-      <c r="V15" s="29"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="31" t="s">
+      <c r="U15" s="24"/>
+      <c r="V15" s="24"/>
+    </row>
+    <row r="16" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="25"/>
+      <c r="B16" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C16">
@@ -6561,14 +6512,14 @@
         <f t="shared" si="3"/>
         <v>109.1146186356347</v>
       </c>
-      <c r="U16" s="29"/>
-      <c r="V16" s="29"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="30" t="s">
+      <c r="U16" s="24"/>
+      <c r="V16" s="24"/>
+    </row>
+    <row r="17" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C17">
@@ -6613,16 +6564,16 @@
       <c r="S17">
         <v>690.60456899999997</v>
       </c>
-      <c r="U17" s="29">
+      <c r="U17" s="24">
         <v>-0.41881600000000002</v>
       </c>
-      <c r="V17" s="29">
+      <c r="V17" s="24">
         <v>0.30126500000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="31" t="s">
+    <row r="18" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="25"/>
+      <c r="B18" s="21" t="s">
         <v>30</v>
       </c>
       <c r="C18">
@@ -6667,12 +6618,12 @@
       <c r="S18">
         <v>5539.0099110000001</v>
       </c>
-      <c r="U18" s="29"/>
-      <c r="V18" s="29"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="31" t="s">
+      <c r="U18" s="24"/>
+      <c r="V18" s="24"/>
+    </row>
+    <row r="19" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="25"/>
+      <c r="B19" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C19">
@@ -6731,14 +6682,14 @@
         <f t="shared" si="4"/>
         <v>74.424524929622493</v>
       </c>
-      <c r="U19" s="29"/>
-      <c r="V19" s="29"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
+      <c r="U19" s="24"/>
+      <c r="V19" s="24"/>
+    </row>
+    <row r="20" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C20">
@@ -6783,16 +6734,16 @@
       <c r="S20">
         <v>323105.30287499999</v>
       </c>
-      <c r="U20" s="29">
+      <c r="U20" s="24">
         <v>0.141819</v>
       </c>
-      <c r="V20" s="29">
+      <c r="V20" s="24">
         <v>0.574376</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="B21" s="31" t="s">
+    <row r="21" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="25"/>
+      <c r="B21" s="21" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="17">
@@ -6837,12 +6788,12 @@
       <c r="S21" s="17">
         <v>3904909000</v>
       </c>
-      <c r="U21" s="29"/>
-      <c r="V21" s="29"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
-      <c r="B22" s="31" t="s">
+      <c r="U21" s="24"/>
+      <c r="V21" s="24"/>
+    </row>
+    <row r="22" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="25"/>
+      <c r="B22" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C22">
@@ -6901,14 +6852,14 @@
         <f t="shared" si="5"/>
         <v>62489.271079122052</v>
       </c>
-      <c r="U22" s="29"/>
-      <c r="V22" s="29"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
+      <c r="U22" s="24"/>
+      <c r="V22" s="24"/>
+    </row>
+    <row r="23" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C23">
@@ -6953,16 +6904,16 @@
       <c r="S23">
         <v>232.03806</v>
       </c>
-      <c r="U23" s="29">
+      <c r="U23" s="24">
         <v>-0.45667099999999999</v>
       </c>
-      <c r="V23" s="29">
+      <c r="V23" s="24">
         <v>-0.16567999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="B24" s="31" t="s">
+    <row r="24" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="25"/>
+      <c r="B24" s="21" t="s">
         <v>30</v>
       </c>
       <c r="C24">
@@ -7007,12 +6958,12 @@
       <c r="S24">
         <v>143.42356799999999</v>
       </c>
-      <c r="U24" s="29"/>
-      <c r="V24" s="29"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
-      <c r="B25" s="31" t="s">
+      <c r="U24" s="24"/>
+      <c r="V24" s="24"/>
+    </row>
+    <row r="25" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="25"/>
+      <c r="B25" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C25">
@@ -7071,14 +7022,14 @@
         <f t="shared" si="6"/>
         <v>11.97595791575772</v>
       </c>
-      <c r="U25" s="29"/>
-      <c r="V25" s="29"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
+      <c r="U25" s="24"/>
+      <c r="V25" s="24"/>
+    </row>
+    <row r="26" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C26">
@@ -7123,16 +7074,16 @@
       <c r="S26">
         <v>-3.7527999999999999E-2</v>
       </c>
-      <c r="U26" s="29">
+      <c r="U26" s="24">
         <v>0.168956</v>
       </c>
-      <c r="V26" s="29">
+      <c r="V26" s="24">
         <v>-0.40711900000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
-      <c r="B27" s="31" t="s">
+    <row r="27" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="25"/>
+      <c r="B27" s="21" t="s">
         <v>30</v>
       </c>
       <c r="C27">
@@ -7177,12 +7128,12 @@
       <c r="S27">
         <v>6.3410000000000003E-3</v>
       </c>
-      <c r="U27" s="29"/>
-      <c r="V27" s="29"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
-      <c r="B28" s="31" t="s">
+      <c r="U27" s="24"/>
+      <c r="V27" s="24"/>
+    </row>
+    <row r="28" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="25"/>
+      <c r="B28" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C28">
@@ -7241,82 +7192,69 @@
         <f t="shared" si="7"/>
         <v>7.9630396206473816E-2</v>
       </c>
-      <c r="U28" s="29"/>
-      <c r="V28" s="29"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U28" s="24"/>
+      <c r="V28" s="24"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.4">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="12"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.4">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="12"/>
       <c r="P30" s="17"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.4">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="12"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.4">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="12"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="12"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="V14:V16"/>
-    <mergeCell ref="V11:V13"/>
-    <mergeCell ref="V8:V10"/>
-    <mergeCell ref="V5:V7"/>
-    <mergeCell ref="U17:U19"/>
-    <mergeCell ref="U20:U22"/>
-    <mergeCell ref="U23:U25"/>
-    <mergeCell ref="U26:U28"/>
-    <mergeCell ref="V26:V28"/>
-    <mergeCell ref="V23:V25"/>
-    <mergeCell ref="V20:V22"/>
-    <mergeCell ref="V17:V19"/>
-    <mergeCell ref="U5:U7"/>
-    <mergeCell ref="U8:U10"/>
-    <mergeCell ref="U11:U13"/>
-    <mergeCell ref="U14:U16"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="O2:S2"/>
     <mergeCell ref="J2:M2"/>
@@ -7327,31 +7265,30 @@
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="A23:A25"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="U20:U22"/>
+    <mergeCell ref="U23:U25"/>
+    <mergeCell ref="U26:U28"/>
+    <mergeCell ref="V26:V28"/>
+    <mergeCell ref="V23:V25"/>
+    <mergeCell ref="V20:V22"/>
+    <mergeCell ref="V14:V16"/>
+    <mergeCell ref="V11:V13"/>
+    <mergeCell ref="V8:V10"/>
+    <mergeCell ref="V5:V7"/>
+    <mergeCell ref="U17:U19"/>
+    <mergeCell ref="V17:V19"/>
+    <mergeCell ref="U5:U7"/>
+    <mergeCell ref="U8:U10"/>
+    <mergeCell ref="U11:U13"/>
+    <mergeCell ref="U14:U16"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="U5:U28">
-    <cfRule type="colorScale" priority="12">
+  <conditionalFormatting sqref="C4:S4">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V5:V28">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
+        <color rgb="FFFFEF9C"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
@@ -7368,16 +7305,6 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:S8">
     <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C4:S4">
-    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -7446,7 +7373,32 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="U5:U28">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V5:V28">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7458,20 +7410,20 @@
       <selection activeCell="AZ10" sqref="AZ10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10" style="3" customWidth="1"/>
-    <col min="2" max="6" width="4.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" style="13" customWidth="1"/>
-    <col min="8" max="27" width="4.42578125" style="2" customWidth="1"/>
-    <col min="28" max="28" width="4.140625" style="3" customWidth="1"/>
+    <col min="2" max="6" width="4.25" style="3" customWidth="1"/>
+    <col min="7" max="7" width="6.25" style="13" customWidth="1"/>
+    <col min="8" max="27" width="4.375" style="2" customWidth="1"/>
+    <col min="28" max="28" width="4.125" style="3" customWidth="1"/>
     <col min="29" max="29" width="10" style="3" customWidth="1"/>
-    <col min="30" max="32" width="4.28515625" style="3" customWidth="1"/>
-    <col min="33" max="33" width="6.140625" style="3" customWidth="1"/>
-    <col min="34" max="43" width="4.42578125" style="4" customWidth="1"/>
+    <col min="30" max="32" width="4.25" style="3" customWidth="1"/>
+    <col min="33" max="33" width="6.125" style="3" customWidth="1"/>
+    <col min="34" max="43" width="4.375" style="4" customWidth="1"/>
     <col min="45" max="45" width="10" style="3" customWidth="1"/>
-    <col min="46" max="49" width="4.28515625" style="3" customWidth="1"/>
-    <col min="50" max="50" width="6.140625" style="3" customWidth="1"/>
+    <col min="46" max="49" width="4.25" style="3" customWidth="1"/>
+    <col min="50" max="50" width="6.125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -7496,28 +7448,28 @@
       <c r="G1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
       <c r="AB1" s="5"/>
       <c r="AC1" s="5" t="s">
         <v>10</v>
@@ -7534,18 +7486,18 @@
       <c r="AG1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="AH1" s="19" t="s">
+      <c r="AH1" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="AI1" s="19"/>
-      <c r="AJ1" s="19"/>
-      <c r="AK1" s="19"/>
-      <c r="AL1" s="19"/>
-      <c r="AM1" s="19"/>
-      <c r="AN1" s="19"/>
-      <c r="AO1" s="19"/>
-      <c r="AP1" s="19"/>
-      <c r="AQ1" s="19"/>
+      <c r="AI1" s="23"/>
+      <c r="AJ1" s="23"/>
+      <c r="AK1" s="23"/>
+      <c r="AL1" s="23"/>
+      <c r="AM1" s="23"/>
+      <c r="AN1" s="23"/>
+      <c r="AO1" s="23"/>
+      <c r="AP1" s="23"/>
+      <c r="AQ1" s="23"/>
       <c r="AS1" s="5" t="s">
         <v>10</v>
       </c>
@@ -7676,7 +7628,7 @@
       <c r="AW2" s="5"/>
       <c r="AX2" s="5"/>
     </row>
-    <row r="3" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -7809,7 +7761,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="4" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.4">
       <c r="C4" s="3">
         <v>2</v>
       </c>
@@ -7864,7 +7816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.4">
       <c r="G5" s="12"/>
       <c r="H5" s="16">
         <f>(COUNTIF(H3:H4,"○"))/2</f>
@@ -7959,7 +7911,7 @@
       <c r="AQ5" s="1"/>
       <c r="AX5" s="12"/>
     </row>
-    <row r="6" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.4">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -8083,7 +8035,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="7" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.4">
       <c r="C7" s="3">
         <v>2</v>
       </c>
@@ -8198,7 +8150,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.4">
       <c r="C8" s="3">
         <v>3</v>
       </c>
@@ -8313,7 +8265,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.4">
       <c r="C9" s="3">
         <v>4</v>
       </c>
@@ -8368,7 +8320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.4">
       <c r="C10" s="3">
         <v>5</v>
       </c>
@@ -8423,7 +8375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.4">
       <c r="C11" s="3">
         <v>6</v>
       </c>
@@ -8478,7 +8430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.4">
       <c r="C12" s="3">
         <v>7</v>
       </c>
@@ -8533,7 +8485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.4">
       <c r="C13" s="3">
         <v>8</v>
       </c>
@@ -8648,7 +8600,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.4">
       <c r="C14" s="3">
         <v>9</v>
       </c>
@@ -8763,7 +8715,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.4">
       <c r="C15" s="3">
         <v>10</v>
       </c>
@@ -8818,7 +8770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.4">
       <c r="G16" s="12"/>
       <c r="H16" s="16">
         <f>(COUNTIF(H6:H15,"○"))/10</f>
@@ -8913,7 +8865,7 @@
       <c r="AQ16" s="1"/>
       <c r="AX16" s="12"/>
     </row>
-    <row r="17" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:50" x14ac:dyDescent="0.4">
       <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
@@ -9037,7 +8989,7 @@
         <v>0.92500000000000004</v>
       </c>
     </row>
-    <row r="18" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C18" s="3">
         <v>2</v>
       </c>
@@ -9152,7 +9104,7 @@
         <v>0.77500000000000002</v>
       </c>
     </row>
-    <row r="19" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C19" s="3">
         <v>3</v>
       </c>
@@ -9267,7 +9219,7 @@
         <v>0.85000000000000009</v>
       </c>
     </row>
-    <row r="20" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C20" s="3">
         <v>4</v>
       </c>
@@ -9322,7 +9274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C21" s="3">
         <v>5</v>
       </c>
@@ -9437,7 +9389,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="22" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C22" s="3">
         <v>6</v>
       </c>
@@ -9552,7 +9504,7 @@
         <v>0.85000000000000009</v>
       </c>
     </row>
-    <row r="23" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C23" s="3">
         <v>7</v>
       </c>
@@ -9607,7 +9559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C24" s="3">
         <v>8</v>
       </c>
@@ -9722,7 +9674,7 @@
         <v>0.92500000000000004</v>
       </c>
     </row>
-    <row r="25" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C25" s="3">
         <v>9</v>
       </c>
@@ -9837,7 +9789,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="26" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C26" s="3">
         <v>10</v>
       </c>
@@ -9952,7 +9904,7 @@
         <v>0.67500000000000004</v>
       </c>
     </row>
-    <row r="27" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C27" s="3">
         <v>11</v>
       </c>
@@ -10067,7 +10019,7 @@
         <v>0.72499999999999998</v>
       </c>
     </row>
-    <row r="28" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C28" s="3">
         <v>12</v>
       </c>
@@ -10182,7 +10134,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="29" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C29" s="3">
         <v>13</v>
       </c>
@@ -10237,7 +10189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C30" s="3">
         <v>14</v>
       </c>
@@ -10352,7 +10304,7 @@
         <v>0.85000000000000009</v>
       </c>
     </row>
-    <row r="31" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:50" x14ac:dyDescent="0.4">
       <c r="G31" s="5"/>
       <c r="H31" s="15">
         <f>(COUNTIF(H17:H30,"○"))/14</f>
@@ -10487,7 +10439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:50" x14ac:dyDescent="0.4">
       <c r="G32" s="12"/>
       <c r="AE32" s="3">
         <v>2</v>
@@ -10536,7 +10488,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="33" spans="30:50" x14ac:dyDescent="0.25">
+    <row r="33" spans="30:50" x14ac:dyDescent="0.4">
       <c r="AD33" s="3" t="s">
         <v>7</v>
       </c>
@@ -10570,7 +10522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="30:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="34" spans="30:50" x14ac:dyDescent="0.4">
       <c r="AE34" s="3">
         <v>2</v>
       </c>
@@ -10598,7 +10550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="30:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="30:50" x14ac:dyDescent="0.4">
       <c r="AE35" s="3">
         <v>3</v>
       </c>
@@ -10626,7 +10578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="30:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="30:50" x14ac:dyDescent="0.4">
       <c r="AE36" s="3">
         <v>4</v>
       </c>
@@ -10674,7 +10626,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="37" spans="30:50" x14ac:dyDescent="0.25">
+    <row r="37" spans="30:50" x14ac:dyDescent="0.4">
       <c r="AD37" s="3" t="s">
         <v>6</v>
       </c>
@@ -10708,7 +10660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="30:50" x14ac:dyDescent="0.25">
+    <row r="38" spans="30:50" x14ac:dyDescent="0.4">
       <c r="AH38" s="15">
         <f>(COUNTIF(AH3:AH37,"○")/32)</f>
         <v>0.625</v>
@@ -10752,12 +10704,12 @@
       <c r="AV38"/>
       <c r="AW38"/>
     </row>
-    <row r="39" spans="30:50" x14ac:dyDescent="0.25">
+    <row r="39" spans="30:50" x14ac:dyDescent="0.4">
       <c r="AV39"/>
       <c r="AW39"/>
       <c r="AX39" s="12"/>
     </row>
-    <row r="40" spans="30:50" x14ac:dyDescent="0.25">
+    <row r="40" spans="30:50" x14ac:dyDescent="0.4">
       <c r="AG40" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[update] added 2nd experiment data
</commit_message>
<xml_diff>
--- a/Experiment-Data/Answer-Data.xlsx
+++ b/Experiment-Data/Answer-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\www\Desktop\eye-tracking-software\Experiment-Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC_User\Desktop\eye-tracking-software\Experiment-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE671995-0E1A-42ED-85FF-2D5EB2688257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BA7D13-6796-4903-B219-77624808F407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{65F65776-174E-4145-8CCF-AA6B8A50F68A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{65F65776-174E-4145-8CCF-AA6B8A50F68A}"/>
   </bookViews>
   <sheets>
     <sheet name="1st-Scores" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1670" uniqueCount="38">
   <si>
     <t>English</t>
   </si>
@@ -208,13 +208,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="176" formatCode="0.000"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -226,7 +226,7 @@
     </font>
     <font>
       <sz val="6"/>
-      <name val="Aptos Narrow"/>
+      <name val="游ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -293,7 +293,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -452,10 +452,10 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -536,22 +536,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -561,6 +552,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1989,24 +1989,24 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10" style="3" customWidth="1"/>
-    <col min="2" max="3" width="4.28515625" style="3" customWidth="1"/>
-    <col min="4" max="5" width="5.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" style="13" customWidth="1"/>
-    <col min="7" max="26" width="4.42578125" style="2" customWidth="1"/>
-    <col min="27" max="27" width="4.140625" style="3" customWidth="1"/>
+    <col min="2" max="3" width="4.25" style="3" customWidth="1"/>
+    <col min="4" max="5" width="5.75" style="3" customWidth="1"/>
+    <col min="6" max="6" width="6.25" style="13" customWidth="1"/>
+    <col min="7" max="26" width="4.375" style="2" customWidth="1"/>
+    <col min="27" max="27" width="4.125" style="3" customWidth="1"/>
     <col min="28" max="28" width="10" style="3" customWidth="1"/>
-    <col min="29" max="30" width="4.28515625" style="3" customWidth="1"/>
-    <col min="31" max="33" width="5.7109375" style="3" customWidth="1"/>
-    <col min="34" max="34" width="6.140625" style="3" customWidth="1"/>
-    <col min="35" max="44" width="4.42578125" style="4" customWidth="1"/>
-    <col min="45" max="45" width="4.140625" customWidth="1"/>
+    <col min="29" max="30" width="4.25" style="3" customWidth="1"/>
+    <col min="31" max="33" width="5.75" style="3" customWidth="1"/>
+    <col min="34" max="34" width="6.125" style="3" customWidth="1"/>
+    <col min="35" max="44" width="4.375" style="4" customWidth="1"/>
+    <col min="45" max="45" width="4.125" customWidth="1"/>
     <col min="46" max="46" width="10" style="3" customWidth="1"/>
-    <col min="47" max="48" width="4.28515625" style="3" customWidth="1"/>
-    <col min="49" max="52" width="5.7109375" style="3" customWidth="1"/>
-    <col min="53" max="53" width="6.140625" style="3" customWidth="1"/>
+    <col min="47" max="48" width="4.25" style="3" customWidth="1"/>
+    <col min="49" max="52" width="5.75" style="3" customWidth="1"/>
+    <col min="53" max="53" width="6.125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:53" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2223,7 +2223,7 @@
       <c r="AZ2" s="5"/>
       <c r="BA2" s="5"/>
     </row>
-    <row r="3" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="4" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C4" s="3">
         <v>2</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>0.52499999999999991</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.4">
       <c r="F5" s="12"/>
       <c r="G5" s="16">
         <f>(COUNTIF(G3:G4,"○"))/2</f>
@@ -2616,7 +2616,7 @@
       <c r="AR5" s="1"/>
       <c r="BA5" s="12"/>
     </row>
-    <row r="6" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.4">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="7" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C7" s="3">
         <v>2</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C8" s="3">
         <v>3</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="9" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C9" s="3">
         <v>4</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C10" s="3">
         <v>5</v>
       </c>
@@ -3325,7 +3325,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C11" s="3">
         <v>6</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C12" s="3">
         <v>7</v>
       </c>
@@ -3605,7 +3605,7 @@
         <v>0.67500000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C13" s="3">
         <v>8</v>
       </c>
@@ -3745,7 +3745,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C14" s="3">
         <v>9</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>0.72500000000000009</v>
       </c>
     </row>
-    <row r="15" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C15" s="3">
         <v>10</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.4">
       <c r="F16" s="12"/>
       <c r="G16" s="16">
         <f>(COUNTIF(G6:G15,"○"))/10</f>
@@ -4120,7 +4120,7 @@
       <c r="AR16" s="1"/>
       <c r="BA16" s="12"/>
     </row>
-    <row r="17" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.4">
       <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C18" s="3">
         <v>2</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="19" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C19" s="3">
         <v>3</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C20" s="3">
         <v>4</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="21" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C21" s="3">
         <v>5</v>
       </c>
@@ -4829,7 +4829,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C22" s="3">
         <v>6</v>
       </c>
@@ -4969,7 +4969,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C23" s="3">
         <v>7</v>
       </c>
@@ -5109,7 +5109,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="24" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C24" s="3">
         <v>8</v>
       </c>
@@ -5249,7 +5249,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="25" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C25" s="3">
         <v>9</v>
       </c>
@@ -5389,7 +5389,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C26" s="3">
         <v>10</v>
       </c>
@@ -5529,7 +5529,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C27" s="3">
         <v>11</v>
       </c>
@@ -5669,7 +5669,7 @@
         <v>0.52500000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C28" s="3">
         <v>12</v>
       </c>
@@ -5809,7 +5809,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="29" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C29" s="3">
         <v>13</v>
       </c>
@@ -5949,7 +5949,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C30" s="3">
         <v>14</v>
       </c>
@@ -6089,7 +6089,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:53" x14ac:dyDescent="0.4">
       <c r="F31" s="5"/>
       <c r="G31" s="15">
         <f>(COUNTIF(G17:G30,"○"))/14</f>
@@ -6243,7 +6243,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="32" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
         <v>19</v>
       </c>
@@ -6325,7 +6325,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="33" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C33" s="3">
         <v>2</v>
       </c>
@@ -6409,7 +6409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:53" x14ac:dyDescent="0.4">
       <c r="C34" s="3">
         <v>3</v>
       </c>
@@ -6483,7 +6483,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="35" spans="1:53" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A35" s="3" t="s">
         <v>20</v>
       </c>
@@ -6561,7 +6561,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="36" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:53" x14ac:dyDescent="0.4">
       <c r="AC36" s="3" t="s">
         <v>6</v>
       </c>
@@ -6634,7 +6634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:53" x14ac:dyDescent="0.4">
       <c r="AI37" s="15">
         <f>(COUNTIF(AI3:AI36,"○")/32)</f>
         <v>1</v>
@@ -6680,7 +6680,7 @@
       <c r="AY37"/>
       <c r="AZ37"/>
     </row>
-    <row r="38" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:53" x14ac:dyDescent="0.4">
       <c r="AB38" s="3" t="s">
         <v>19</v>
       </c>
@@ -6723,7 +6723,7 @@
       </c>
       <c r="BA38" s="12"/>
     </row>
-    <row r="39" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:53" x14ac:dyDescent="0.4">
       <c r="AD39" s="3">
         <v>2</v>
       </c>
@@ -6760,7 +6760,7 @@
         <v>0.7142857142857143</v>
       </c>
     </row>
-    <row r="40" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:53" x14ac:dyDescent="0.4">
       <c r="AD40" s="3">
         <v>3</v>
       </c>
@@ -6788,7 +6788,7 @@
         <v>0.66249999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:53" x14ac:dyDescent="0.4">
       <c r="AD41" s="3">
         <v>4</v>
       </c>
@@ -6808,7 +6808,7 @@
         <v>0.60500000000000009</v>
       </c>
     </row>
-    <row r="42" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:53" x14ac:dyDescent="0.4">
       <c r="AB42" s="3" t="s">
         <v>20</v>
       </c>
@@ -6832,7 +6832,7 @@
         <v>0.65555555555555556</v>
       </c>
     </row>
-    <row r="43" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:53" x14ac:dyDescent="0.4">
       <c r="AT43" s="3" t="s">
         <v>20</v>
       </c>
@@ -6873,27 +6873,27 @@
       <selection pane="topRight" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.375" customWidth="1"/>
     <col min="3" max="4" width="10" style="3" customWidth="1"/>
-    <col min="5" max="5" width="3.5703125" customWidth="1"/>
+    <col min="5" max="5" width="3.625" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="3.5703125" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="3.625" customWidth="1"/>
+    <col min="10" max="10" width="9.125" customWidth="1"/>
+    <col min="12" max="12" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46">
         <v>2</v>
       </c>
-      <c r="D1" s="45"/>
+      <c r="D1" s="46"/>
       <c r="E1" s="22"/>
       <c r="F1" s="57">
         <v>3</v>
@@ -6901,16 +6901,16 @@
       <c r="G1" s="57"/>
       <c r="H1" s="57"/>
       <c r="I1" s="22"/>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="45"/>
-    </row>
-    <row r="2" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="K1" s="46"/>
+    </row>
+    <row r="2" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="46"/>
+      <c r="B2" s="47"/>
       <c r="C2" s="27">
         <v>2</v>
       </c>
@@ -6935,7 +6935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="54" t="s">
         <v>23</v>
       </c>
@@ -6959,14 +6959,14 @@
         <v>295.16666700000002</v>
       </c>
       <c r="I3" s="25"/>
-      <c r="J3" s="50">
+      <c r="J3" s="45">
         <v>-0.188448</v>
       </c>
-      <c r="K3" s="48">
+      <c r="K3" s="51">
         <v>0.54788800000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="54"/>
       <c r="B4" s="21" t="s">
         <v>32</v>
@@ -6988,10 +6988,10 @@
         <v>45.984417654244574</v>
       </c>
       <c r="I4" s="22"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="47"/>
-    </row>
-    <row r="5" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J4" s="46"/>
+      <c r="K4" s="52"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="55"/>
       <c r="B5" s="23" t="s">
         <v>35</v>
@@ -7018,10 +7018,10 @@
         <v>0.15579136398299531</v>
       </c>
       <c r="I5" s="24"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="49"/>
-    </row>
-    <row r="6" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J5" s="47"/>
+      <c r="K5" s="53"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="56" t="s">
         <v>24</v>
       </c>
@@ -7045,14 +7045,14 @@
         <v>1165.094081</v>
       </c>
       <c r="I6" s="22"/>
-      <c r="J6" s="45">
+      <c r="J6" s="46">
         <v>0.503328</v>
       </c>
-      <c r="K6" s="47">
+      <c r="K6" s="52">
         <v>-4.8842999999999998E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="54"/>
       <c r="B7" s="33" t="s">
         <v>17</v>
@@ -7074,10 +7074,10 @@
         <v>120.80618517691882</v>
       </c>
       <c r="I7" s="22"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="47"/>
-    </row>
-    <row r="8" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J7" s="46"/>
+      <c r="K7" s="52"/>
+    </row>
+    <row r="8" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="55"/>
       <c r="B8" s="23" t="s">
         <v>34</v>
@@ -7104,10 +7104,10 @@
         <v>0.10368792284416285</v>
       </c>
       <c r="I8" s="22"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="47"/>
-    </row>
-    <row r="9" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="46"/>
+      <c r="K8" s="52"/>
+    </row>
+    <row r="9" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="56" t="s">
         <v>25</v>
       </c>
@@ -7131,14 +7131,14 @@
         <v>1078.5</v>
       </c>
       <c r="I9" s="25"/>
-      <c r="J9" s="50">
+      <c r="J9" s="45">
         <v>-0.221611</v>
       </c>
-      <c r="K9" s="48">
+      <c r="K9" s="51">
         <v>0.53761899999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="54"/>
       <c r="B10" s="33" t="s">
         <v>17</v>
@@ -7160,10 +7160,10 @@
         <v>258.54109924729568</v>
       </c>
       <c r="I10" s="22"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="47"/>
-    </row>
-    <row r="11" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J10" s="46"/>
+      <c r="K10" s="52"/>
+    </row>
+    <row r="11" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="55"/>
       <c r="B11" s="35" t="s">
         <v>34</v>
@@ -7190,10 +7190,10 @@
         <v>0.23972285512034833</v>
       </c>
       <c r="I11" s="24"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="49"/>
-    </row>
-    <row r="12" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="47"/>
+      <c r="K11" s="53"/>
+    </row>
+    <row r="12" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="56" t="s">
         <v>26</v>
       </c>
@@ -7217,14 +7217,14 @@
         <v>13.026258</v>
       </c>
       <c r="I12" s="22"/>
-      <c r="J12" s="45">
+      <c r="J12" s="46">
         <v>-0.32667400000000002</v>
       </c>
-      <c r="K12" s="47">
+      <c r="K12" s="52">
         <v>-0.13261100000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="54"/>
       <c r="B13" s="33" t="s">
         <v>17</v>
@@ -7246,10 +7246,10 @@
         <v>1.1520512141393715</v>
       </c>
       <c r="I13" s="22"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="47"/>
-    </row>
-    <row r="14" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="46"/>
+      <c r="K13" s="52"/>
+    </row>
+    <row r="14" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="55"/>
       <c r="B14" s="35" t="s">
         <v>34</v>
@@ -7276,10 +7276,10 @@
         <v>8.8440687581911204E-2</v>
       </c>
       <c r="I14" s="22"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="47"/>
-    </row>
-    <row r="15" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="46"/>
+      <c r="K14" s="52"/>
+    </row>
+    <row r="15" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="54" t="s">
         <v>27</v>
       </c>
@@ -7303,14 +7303,14 @@
         <v>290.23841599999997</v>
       </c>
       <c r="I15" s="25"/>
-      <c r="J15" s="50">
+      <c r="J15" s="45">
         <v>0.51528499999999999</v>
       </c>
-      <c r="K15" s="48">
+      <c r="K15" s="51">
         <v>1.5509E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="54"/>
       <c r="B16" s="33" t="s">
         <v>17</v>
@@ -7332,10 +7332,10 @@
         <v>33.816063239235881</v>
       </c>
       <c r="I16" s="22"/>
-      <c r="J16" s="45"/>
-      <c r="K16" s="47"/>
-    </row>
-    <row r="17" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="46"/>
+      <c r="K16" s="52"/>
+    </row>
+    <row r="17" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="54"/>
       <c r="B17" s="33" t="s">
         <v>34</v>
@@ -7362,10 +7362,10 @@
         <v>0.11651132784309257</v>
       </c>
       <c r="I17" s="24"/>
-      <c r="J17" s="46"/>
-      <c r="K17" s="49"/>
-    </row>
-    <row r="18" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J17" s="47"/>
+      <c r="K17" s="53"/>
+    </row>
+    <row r="18" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="56" t="s">
         <v>30</v>
       </c>
@@ -7389,14 +7389,14 @@
         <v>1328.2708680000001</v>
       </c>
       <c r="I18" s="22"/>
-      <c r="J18" s="45">
+      <c r="J18" s="46">
         <v>0.212811</v>
       </c>
-      <c r="K18" s="47">
+      <c r="K18" s="52">
         <v>0.184026</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="54"/>
       <c r="B19" s="33" t="s">
         <v>17</v>
@@ -7418,10 +7418,10 @@
         <v>185.2619838175118</v>
       </c>
       <c r="I19" s="22"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="47"/>
-    </row>
-    <row r="20" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J19" s="46"/>
+      <c r="K19" s="52"/>
+    </row>
+    <row r="20" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="55"/>
       <c r="B20" s="35" t="s">
         <v>34</v>
@@ -7448,10 +7448,10 @@
         <v>0.13947605739216723</v>
       </c>
       <c r="I20" s="22"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="47"/>
-    </row>
-    <row r="21" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J20" s="46"/>
+      <c r="K20" s="52"/>
+    </row>
+    <row r="21" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="54" t="s">
         <v>31</v>
       </c>
@@ -7475,14 +7475,14 @@
         <v>436.16804999999999</v>
       </c>
       <c r="I21" s="25"/>
-      <c r="J21" s="50">
+      <c r="J21" s="45">
         <v>0.42631999999999998</v>
       </c>
-      <c r="K21" s="48">
+      <c r="K21" s="51">
         <v>3.6583999999999998E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="54"/>
       <c r="B22" s="33" t="s">
         <v>17</v>
@@ -7504,10 +7504,10 @@
         <v>26.527001828325794</v>
       </c>
       <c r="I22" s="22"/>
-      <c r="J22" s="45"/>
-      <c r="K22" s="47"/>
-    </row>
-    <row r="23" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J22" s="46"/>
+      <c r="K22" s="52"/>
+    </row>
+    <row r="23" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="54"/>
       <c r="B23" s="33" t="s">
         <v>34</v>
@@ -7534,10 +7534,10 @@
         <v>6.0818305761565515E-2</v>
       </c>
       <c r="I23" s="24"/>
-      <c r="J23" s="46"/>
-      <c r="K23" s="49"/>
-    </row>
-    <row r="24" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J23" s="47"/>
+      <c r="K23" s="53"/>
+    </row>
+    <row r="24" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="56" t="s">
         <v>28</v>
       </c>
@@ -7561,14 +7561,14 @@
         <v>149.374664</v>
       </c>
       <c r="I24" s="22"/>
-      <c r="J24" s="45">
+      <c r="J24" s="46">
         <v>0.17419599999999999</v>
       </c>
-      <c r="K24" s="47">
+      <c r="K24" s="52">
         <v>0.53308299999999997</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="54"/>
       <c r="B25" s="33" t="s">
         <v>17</v>
@@ -7590,10 +7590,10 @@
         <v>25.510562851493496</v>
       </c>
       <c r="I25" s="22"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="47"/>
-    </row>
-    <row r="26" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="46"/>
+      <c r="K25" s="52"/>
+    </row>
+    <row r="26" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="55"/>
       <c r="B26" s="35" t="s">
         <v>34</v>
@@ -7620,11 +7620,11 @@
         <v>0.17078239487449826</v>
       </c>
       <c r="I26" s="22"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="47"/>
-    </row>
-    <row r="27" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="51" t="s">
+      <c r="J26" s="46"/>
+      <c r="K26" s="52"/>
+    </row>
+    <row r="27" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="48" t="s">
         <v>29</v>
       </c>
       <c r="B27" s="32" t="s">
@@ -7647,15 +7647,15 @@
         <v>0.95097100000000001</v>
       </c>
       <c r="I27" s="25"/>
-      <c r="J27" s="50">
+      <c r="J27" s="45">
         <v>-0.18006</v>
       </c>
-      <c r="K27" s="48">
+      <c r="K27" s="51">
         <v>-0.26681700000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="52"/>
+    <row r="28" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="49"/>
       <c r="B28" s="33" t="s">
         <v>17</v>
       </c>
@@ -7676,11 +7676,11 @@
         <v>1.0488088481701515E-2</v>
       </c>
       <c r="I28" s="22"/>
-      <c r="J28" s="45"/>
-      <c r="K28" s="47"/>
-    </row>
-    <row r="29" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="53"/>
+      <c r="J28" s="46"/>
+      <c r="K28" s="52"/>
+    </row>
+    <row r="29" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="50"/>
       <c r="B29" s="35" t="s">
         <v>34</v>
       </c>
@@ -7706,14 +7706,14 @@
         <v>1.1028820523130058E-2</v>
       </c>
       <c r="I29" s="24"/>
-      <c r="J29" s="46"/>
-      <c r="K29" s="49"/>
-    </row>
-    <row r="30" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="46" t="s">
+      <c r="J29" s="47"/>
+      <c r="K29" s="53"/>
+    </row>
+    <row r="30" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="46"/>
+      <c r="B30" s="47"/>
       <c r="C30" s="37">
         <v>0.45</v>
       </c>
@@ -7734,7 +7734,7 @@
       <c r="J30" s="22"/>
       <c r="K30" s="22"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -7744,7 +7744,7 @@
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B32" s="3"/>
       <c r="C32" s="26"/>
       <c r="E32" s="3"/>
@@ -7755,7 +7755,7 @@
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B33" s="3"/>
       <c r="C33" s="26"/>
       <c r="E33" s="3"/>
@@ -7766,7 +7766,7 @@
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B34" s="3"/>
       <c r="C34" s="26"/>
       <c r="E34" s="3"/>
@@ -7777,24 +7777,41 @@
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B35" s="3"/>
       <c r="C35" s="26"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B36" s="3"/>
       <c r="C36" s="26"/>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B38" s="3"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="K3:K5"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="K24:K26"/>
+    <mergeCell ref="K21:K23"/>
+    <mergeCell ref="K18:K20"/>
+    <mergeCell ref="K12:K14"/>
     <mergeCell ref="J21:J23"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A27:A29"/>
@@ -7811,23 +7828,6 @@
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="A21:A23"/>
-    <mergeCell ref="J18:J20"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="K3:K5"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="K15:K17"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="J9:J11"/>
-    <mergeCell ref="J12:J14"/>
-    <mergeCell ref="K24:K26"/>
-    <mergeCell ref="K21:K23"/>
-    <mergeCell ref="K18:K20"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="K9:K11"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="C32:C36">
@@ -7842,16 +7842,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3 I3">
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E6">
     <cfRule type="colorScale" priority="36">
       <colorScale>
@@ -7862,8 +7852,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E18 I18">
-    <cfRule type="colorScale" priority="33">
+  <conditionalFormatting sqref="E9 I9">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -7872,8 +7862,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21 I21">
-    <cfRule type="colorScale" priority="34">
+  <conditionalFormatting sqref="E12 I12">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -7882,8 +7872,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E24 I24">
-    <cfRule type="colorScale" priority="35">
+  <conditionalFormatting sqref="E15 I15">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -8012,8 +8002,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9 E9">
-    <cfRule type="colorScale" priority="30">
+  <conditionalFormatting sqref="I3 E3">
+    <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -8022,8 +8012,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I12 E12">
-    <cfRule type="colorScale" priority="31">
+  <conditionalFormatting sqref="I18 E18">
+    <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -8032,8 +8022,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I15 E15">
-    <cfRule type="colorScale" priority="32">
+  <conditionalFormatting sqref="I21 E21">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24 E24">
+    <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -8091,30 +8091,30 @@
       <selection pane="topRight" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.375" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="10" style="3" customWidth="1"/>
-    <col min="5" max="5" width="3.5703125" customWidth="1"/>
+    <col min="5" max="5" width="3.625" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="3.5703125" customWidth="1"/>
+    <col min="9" max="9" width="3.625" customWidth="1"/>
     <col min="10" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="3.5703125" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="3.625" customWidth="1"/>
+    <col min="15" max="15" width="9.125" customWidth="1"/>
+    <col min="17" max="17" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46">
         <v>2</v>
       </c>
-      <c r="D1" s="45"/>
+      <c r="D1" s="46"/>
       <c r="E1" s="22"/>
       <c r="F1" s="57">
         <v>3</v>
@@ -8122,23 +8122,23 @@
       <c r="G1" s="57"/>
       <c r="H1" s="57"/>
       <c r="I1" s="22"/>
-      <c r="J1" s="45">
+      <c r="J1" s="46">
         <v>4</v>
       </c>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
       <c r="N1" s="22"/>
-      <c r="O1" s="45" t="s">
+      <c r="O1" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="45"/>
-    </row>
-    <row r="2" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="P1" s="46"/>
+    </row>
+    <row r="2" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="46"/>
+      <c r="B2" s="47"/>
       <c r="C2" s="27">
         <v>1</v>
       </c>
@@ -8176,7 +8176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="54" t="s">
         <v>23</v>
       </c>
@@ -8213,10 +8213,10 @@
         <v>170.75</v>
       </c>
       <c r="N3" s="25"/>
-      <c r="O3" s="50">
+      <c r="O3" s="45">
         <v>0.19814899999999999</v>
       </c>
-      <c r="P3" s="48">
+      <c r="P3" s="51">
         <v>0.554253</v>
       </c>
       <c r="R3" s="20"/>
@@ -8229,7 +8229,7 @@
       <c r="Y3" s="20"/>
       <c r="Z3" s="20"/>
     </row>
-    <row r="4" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="54"/>
       <c r="B4" s="33" t="s">
         <v>17</v>
@@ -8264,8 +8264,8 @@
         <v>18.304956405301816</v>
       </c>
       <c r="N4" s="22"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="47"/>
+      <c r="O4" s="46"/>
+      <c r="P4" s="52"/>
       <c r="R4" s="20"/>
       <c r="S4" s="20"/>
       <c r="T4" s="20"/>
@@ -8276,7 +8276,7 @@
       <c r="Y4" s="20"/>
       <c r="Z4" s="20"/>
     </row>
-    <row r="5" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="55"/>
       <c r="B5" s="35" t="s">
         <v>37</v>
@@ -8320,10 +8320,10 @@
         <v>0.1072032585962039</v>
       </c>
       <c r="N5" s="24"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="49"/>
-    </row>
-    <row r="6" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O5" s="47"/>
+      <c r="P5" s="53"/>
+    </row>
+    <row r="6" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="56" t="s">
         <v>24</v>
       </c>
@@ -8360,14 +8360,14 @@
         <v>1066.667138</v>
       </c>
       <c r="N6" s="22"/>
-      <c r="O6" s="45">
+      <c r="O6" s="46">
         <v>0.38675100000000001</v>
       </c>
-      <c r="P6" s="47">
+      <c r="P6" s="52">
         <v>-0.30294199999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="54"/>
       <c r="B7" s="33" t="s">
         <v>17</v>
@@ -8402,10 +8402,10 @@
         <v>154.17636012048021</v>
       </c>
       <c r="N7" s="22"/>
-      <c r="O7" s="45"/>
-      <c r="P7" s="47"/>
-    </row>
-    <row r="8" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O7" s="46"/>
+      <c r="P7" s="52"/>
+    </row>
+    <row r="8" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="55"/>
       <c r="B8" s="35" t="s">
         <v>34</v>
@@ -8449,10 +8449,10 @@
         <v>0.14454027374421674</v>
       </c>
       <c r="N8" s="22"/>
-      <c r="O8" s="45"/>
-      <c r="P8" s="47"/>
-    </row>
-    <row r="9" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O8" s="46"/>
+      <c r="P8" s="52"/>
+    </row>
+    <row r="9" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="56" t="s">
         <v>25</v>
       </c>
@@ -8489,14 +8489,14 @@
         <v>613.25</v>
       </c>
       <c r="N9" s="25"/>
-      <c r="O9" s="50">
+      <c r="O9" s="45">
         <v>0.173847</v>
       </c>
-      <c r="P9" s="48">
+      <c r="P9" s="51">
         <v>0.57918999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="54"/>
       <c r="B10" s="33" t="s">
         <v>17</v>
@@ -8531,10 +8531,10 @@
         <v>50.024993753123049</v>
       </c>
       <c r="N10" s="22"/>
-      <c r="O10" s="45"/>
-      <c r="P10" s="47"/>
-    </row>
-    <row r="11" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O10" s="46"/>
+      <c r="P10" s="52"/>
+    </row>
+    <row r="11" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="55"/>
       <c r="B11" s="35" t="s">
         <v>34</v>
@@ -8578,10 +8578,10 @@
         <v>8.1573573180795833E-2</v>
       </c>
       <c r="N11" s="24"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="49"/>
-    </row>
-    <row r="12" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O11" s="47"/>
+      <c r="P11" s="53"/>
+    </row>
+    <row r="12" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="56" t="s">
         <v>26</v>
       </c>
@@ -8618,14 +8618,14 @@
         <v>12.416684999999999</v>
       </c>
       <c r="N12" s="22"/>
-      <c r="O12" s="45">
+      <c r="O12" s="46">
         <v>-0.25663200000000003</v>
       </c>
-      <c r="P12" s="47">
+      <c r="P12" s="52">
         <v>0.23480300000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="54"/>
       <c r="B13" s="33" t="s">
         <v>17</v>
@@ -8660,10 +8660,10 @@
         <v>0.62217280557735732</v>
       </c>
       <c r="N13" s="22"/>
-      <c r="O13" s="45"/>
-      <c r="P13" s="47"/>
-    </row>
-    <row r="14" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O13" s="46"/>
+      <c r="P13" s="52"/>
+    </row>
+    <row r="14" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="55"/>
       <c r="B14" s="35" t="s">
         <v>34</v>
@@ -8707,10 +8707,10 @@
         <v>5.0107802974574726E-2</v>
       </c>
       <c r="N14" s="22"/>
-      <c r="O14" s="45"/>
-      <c r="P14" s="47"/>
-    </row>
-    <row r="15" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O14" s="46"/>
+      <c r="P14" s="52"/>
+    </row>
+    <row r="15" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="54" t="s">
         <v>27</v>
       </c>
@@ -8747,14 +8747,14 @@
         <v>271.35037599999998</v>
       </c>
       <c r="N15" s="25"/>
-      <c r="O15" s="50">
+      <c r="O15" s="45">
         <v>0.423954</v>
       </c>
-      <c r="P15" s="48">
+      <c r="P15" s="51">
         <v>-0.33226099999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="54"/>
       <c r="B16" s="33" t="s">
         <v>36</v>
@@ -8789,10 +8789,10 @@
         <v>53.314599041913468</v>
       </c>
       <c r="N16" s="22"/>
-      <c r="O16" s="45"/>
-      <c r="P16" s="47"/>
-    </row>
-    <row r="17" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O16" s="46"/>
+      <c r="P16" s="52"/>
+    </row>
+    <row r="17" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="54"/>
       <c r="B17" s="33" t="s">
         <v>34</v>
@@ -8836,10 +8836,10 @@
         <v>0.19647881026674335</v>
       </c>
       <c r="N17" s="24"/>
-      <c r="O17" s="46"/>
-      <c r="P17" s="49"/>
-    </row>
-    <row r="18" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O17" s="47"/>
+      <c r="P17" s="53"/>
+    </row>
+    <row r="18" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="56" t="s">
         <v>30</v>
       </c>
@@ -8876,14 +8876,14 @@
         <v>1183.321686</v>
       </c>
       <c r="N18" s="22"/>
-      <c r="O18" s="45">
+      <c r="O18" s="46">
         <v>0.415715</v>
       </c>
-      <c r="P18" s="47">
+      <c r="P18" s="52">
         <v>-1.6017E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="54"/>
       <c r="B19" s="33" t="s">
         <v>17</v>
@@ -8918,10 +8918,10 @@
         <v>153.79639008117195</v>
       </c>
       <c r="N19" s="22"/>
-      <c r="O19" s="45"/>
-      <c r="P19" s="47"/>
-    </row>
-    <row r="20" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O19" s="46"/>
+      <c r="P19" s="52"/>
+    </row>
+    <row r="20" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="55"/>
       <c r="B20" s="35" t="s">
         <v>34</v>
@@ -8965,10 +8965,10 @@
         <v>0.12997005962178568</v>
       </c>
       <c r="N20" s="22"/>
-      <c r="O20" s="45"/>
-      <c r="P20" s="47"/>
-    </row>
-    <row r="21" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O20" s="46"/>
+      <c r="P20" s="52"/>
+    </row>
+    <row r="21" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="54" t="s">
         <v>31</v>
       </c>
@@ -9005,14 +9005,14 @@
         <v>505.92089199999998</v>
       </c>
       <c r="N21" s="25"/>
-      <c r="O21" s="50">
+      <c r="O21" s="45">
         <v>0.425207</v>
       </c>
-      <c r="P21" s="48">
+      <c r="P21" s="51">
         <v>-3.3320000000000002E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="54"/>
       <c r="B22" s="33" t="s">
         <v>17</v>
@@ -9047,10 +9047,10 @@
         <v>32.017303868377176</v>
       </c>
       <c r="N22" s="22"/>
-      <c r="O22" s="45"/>
-      <c r="P22" s="47"/>
-    </row>
-    <row r="23" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O22" s="46"/>
+      <c r="P22" s="52"/>
+    </row>
+    <row r="23" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="54"/>
       <c r="B23" s="33" t="s">
         <v>34</v>
@@ -9094,10 +9094,10 @@
         <v>6.3285198090568623E-2</v>
       </c>
       <c r="N23" s="24"/>
-      <c r="O23" s="46"/>
-      <c r="P23" s="49"/>
-    </row>
-    <row r="24" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O23" s="47"/>
+      <c r="P23" s="53"/>
+    </row>
+    <row r="24" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="56" t="s">
         <v>28</v>
       </c>
@@ -9134,14 +9134,14 @@
         <v>86.171711999999999</v>
       </c>
       <c r="N24" s="22"/>
-      <c r="O24" s="45">
+      <c r="O24" s="46">
         <v>0.424012</v>
       </c>
-      <c r="P24" s="47">
+      <c r="P24" s="52">
         <v>0.291018</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="54"/>
       <c r="B25" s="33" t="s">
         <v>17</v>
@@ -9176,10 +9176,10 @@
         <v>8.076926890841591</v>
       </c>
       <c r="N25" s="22"/>
-      <c r="O25" s="45"/>
-      <c r="P25" s="47"/>
-    </row>
-    <row r="26" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O25" s="46"/>
+      <c r="P25" s="52"/>
+    </row>
+    <row r="26" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="55"/>
       <c r="B26" s="35" t="s">
         <v>34</v>
@@ -9223,11 +9223,11 @@
         <v>9.3730607218777212E-2</v>
       </c>
       <c r="N26" s="22"/>
-      <c r="O26" s="45"/>
-      <c r="P26" s="47"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="51" t="s">
+      <c r="O26" s="46"/>
+      <c r="P26" s="52"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A27" s="48" t="s">
         <v>29</v>
       </c>
       <c r="B27" s="40" t="s">
@@ -9263,15 +9263,15 @@
         <v>0.96520300000000003</v>
       </c>
       <c r="N27" s="25"/>
-      <c r="O27" s="50">
+      <c r="O27" s="45">
         <v>-4.3986999999999998E-2</v>
       </c>
-      <c r="P27" s="48">
+      <c r="P27" s="51">
         <v>-0.118243</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="52"/>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A28" s="49"/>
       <c r="B28" s="33" t="s">
         <v>17</v>
       </c>
@@ -9305,11 +9305,11 @@
         <v>1.5132745950421557E-2</v>
       </c>
       <c r="N28" s="22"/>
-      <c r="O28" s="45"/>
-      <c r="P28" s="47"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="53"/>
+      <c r="O28" s="46"/>
+      <c r="P28" s="52"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A29" s="50"/>
       <c r="B29" s="35" t="s">
         <v>34</v>
       </c>
@@ -9352,14 +9352,14 @@
         <v>1.5678303890913681E-2</v>
       </c>
       <c r="N29" s="24"/>
-      <c r="O29" s="46"/>
-      <c r="P29" s="49"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="46" t="s">
+      <c r="O29" s="47"/>
+      <c r="P29" s="53"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A30" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="46"/>
+      <c r="B30" s="47"/>
       <c r="C30" s="37">
         <v>0.87</v>
       </c>
@@ -9393,7 +9393,7 @@
       <c r="O30" s="22"/>
       <c r="P30" s="22"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="E31" s="3"/>
@@ -9409,7 +9409,7 @@
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="E32" s="3"/>
@@ -9425,7 +9425,7 @@
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="E33" s="3"/>
@@ -9441,7 +9441,7 @@
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="E34" s="3"/>
@@ -9457,7 +9457,7 @@
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="E35" s="3"/>
@@ -9473,21 +9473,39 @@
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="O3:O5"/>
+    <mergeCell ref="P3:P5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="O6:O8"/>
+    <mergeCell ref="P6:P8"/>
+    <mergeCell ref="P18:P20"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="O9:O11"/>
+    <mergeCell ref="P9:P11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="O12:O14"/>
+    <mergeCell ref="P12:P14"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="O27:O29"/>
     <mergeCell ref="P27:P29"/>
@@ -9504,28 +9522,10 @@
     <mergeCell ref="P15:P17"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="O18:O20"/>
-    <mergeCell ref="P18:P20"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="O9:O11"/>
-    <mergeCell ref="P9:P11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="O12:O14"/>
-    <mergeCell ref="P12:P14"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="O3:O5"/>
-    <mergeCell ref="P3:P5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="O6:O8"/>
-    <mergeCell ref="P6:P8"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="E3 N3">
-    <cfRule type="colorScale" priority="34">
+  <conditionalFormatting sqref="E3 I3">
+    <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -9536,6 +9536,16 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
     <cfRule type="colorScale" priority="48">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6 I6">
+    <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -9562,8 +9572,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E9 I9">
-    <cfRule type="colorScale" priority="54">
+  <conditionalFormatting sqref="E9">
+    <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -9572,8 +9582,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E9 N9">
-    <cfRule type="colorScale" priority="35">
+  <conditionalFormatting sqref="E12 I12">
+    <cfRule type="colorScale" priority="59">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -9582,8 +9592,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E9">
-    <cfRule type="colorScale" priority="56">
+  <conditionalFormatting sqref="E12 N12">
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -9602,6 +9612,56 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E15 N15">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18 I18">
+    <cfRule type="colorScale" priority="69">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18 N18">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21 I21">
+    <cfRule type="colorScale" priority="74">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21 N21">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E21">
     <cfRule type="colorScale" priority="76">
       <colorScale>
@@ -9612,8 +9672,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E24 I24">
-    <cfRule type="colorScale" priority="79">
+  <conditionalFormatting sqref="E24 N24">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -9624,6 +9684,16 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
     <cfRule type="colorScale" priority="81">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27 I27">
+    <cfRule type="colorScale" priority="82">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -9742,28 +9812,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3 E3">
-    <cfRule type="colorScale" priority="46">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I6 E6">
-    <cfRule type="colorScale" priority="49">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12 E12">
-    <cfRule type="colorScale" priority="59">
+  <conditionalFormatting sqref="I9 E9">
+    <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -9773,14 +9823,6 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15 E15">
-    <cfRule type="colorScale" priority="64">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
     <cfRule type="colorScale" priority="66">
       <colorScale>
         <cfvo type="min"/>
@@ -9789,9 +9831,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18 E18">
-    <cfRule type="colorScale" priority="69">
+    <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -9810,18 +9850,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21 E21">
-    <cfRule type="colorScale" priority="74">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I27 E27">
-    <cfRule type="colorScale" priority="82">
+  <conditionalFormatting sqref="I24 E24">
+    <cfRule type="colorScale" priority="79">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -9840,8 +9870,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N12 E12">
-    <cfRule type="colorScale" priority="36">
+  <conditionalFormatting sqref="N3 E3">
+    <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -9850,38 +9880,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N15 E15">
-    <cfRule type="colorScale" priority="37">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N18 E18">
-    <cfRule type="colorScale" priority="38">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N21 E21">
-    <cfRule type="colorScale" priority="39">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N24 E24">
-    <cfRule type="colorScale" priority="40">
+  <conditionalFormatting sqref="N9 E9">
+    <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -9934,43 +9934,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F49CEF5C-F3E1-4A78-9556-E0BCACEDD567}">
   <dimension ref="A1:AF38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="W30" sqref="W30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.375" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="10" style="3" customWidth="1"/>
-    <col min="5" max="5" width="3.5703125" customWidth="1"/>
+    <col min="5" max="5" width="3.625" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="3.5703125" customWidth="1"/>
+    <col min="9" max="9" width="3.625" customWidth="1"/>
     <col min="10" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="3.5703125" customWidth="1"/>
+    <col min="14" max="14" width="3.625" customWidth="1"/>
     <col min="15" max="19" width="10" customWidth="1"/>
-    <col min="20" max="20" width="3.5703125" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" customWidth="1"/>
-    <col min="23" max="23" width="9.140625" customWidth="1"/>
+    <col min="20" max="20" width="3.625" customWidth="1"/>
+    <col min="21" max="21" width="9.125" customWidth="1"/>
+    <col min="23" max="23" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46">
         <v>2</v>
       </c>
-      <c r="D1" s="45"/>
+      <c r="D1" s="46"/>
       <c r="E1" s="22"/>
-      <c r="F1" s="45">
+      <c r="F1" s="46">
         <v>3</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
       <c r="I1" s="22"/>
       <c r="J1" s="57">
         <v>4</v>
@@ -9979,24 +9979,24 @@
       <c r="L1" s="57"/>
       <c r="M1" s="57"/>
       <c r="N1" s="22"/>
-      <c r="O1" s="45">
+      <c r="O1" s="46">
         <v>5</v>
       </c>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
       <c r="T1" s="22"/>
-      <c r="U1" s="45" t="s">
+      <c r="U1" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="45"/>
-    </row>
-    <row r="2" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="V1" s="46"/>
+    </row>
+    <row r="2" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="46"/>
+      <c r="B2" s="47"/>
       <c r="C2" s="27">
         <v>1</v>
       </c>
@@ -10050,7 +10050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="54" t="s">
         <v>23</v>
       </c>
@@ -10103,10 +10103,10 @@
         <v>300.2</v>
       </c>
       <c r="T3" s="25"/>
-      <c r="U3" s="50">
+      <c r="U3" s="45">
         <v>-0.33963700000000002</v>
       </c>
-      <c r="V3" s="48">
+      <c r="V3" s="51">
         <v>0.42593500000000001</v>
       </c>
       <c r="X3" s="20"/>
@@ -10119,7 +10119,7 @@
       <c r="AE3" s="20"/>
       <c r="AF3" s="20"/>
     </row>
-    <row r="4" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="54"/>
       <c r="B4" s="33" t="s">
         <v>17</v>
@@ -10170,8 +10170,8 @@
         <v>48.41435737464662</v>
       </c>
       <c r="T4" s="22"/>
-      <c r="U4" s="45"/>
-      <c r="V4" s="47"/>
+      <c r="U4" s="46"/>
+      <c r="V4" s="52"/>
       <c r="X4" s="20"/>
       <c r="Y4" s="20"/>
       <c r="Z4" s="20"/>
@@ -10182,7 +10182,7 @@
       <c r="AE4" s="20"/>
       <c r="AF4" s="20"/>
     </row>
-    <row r="5" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="55"/>
       <c r="B5" s="23" t="s">
         <v>37</v>
@@ -10247,10 +10247,10 @@
         <v>0.16127367546517862</v>
       </c>
       <c r="T5" s="24"/>
-      <c r="U5" s="46"/>
-      <c r="V5" s="49"/>
-    </row>
-    <row r="6" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U5" s="47"/>
+      <c r="V5" s="53"/>
+    </row>
+    <row r="6" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="56" t="s">
         <v>24</v>
       </c>
@@ -10303,14 +10303,14 @@
         <v>963.53767200000004</v>
       </c>
       <c r="T6" s="22"/>
-      <c r="U6" s="45">
+      <c r="U6" s="46">
         <v>0.461256</v>
       </c>
-      <c r="V6" s="47">
+      <c r="V6" s="52">
         <v>0.161083</v>
       </c>
     </row>
-    <row r="7" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="54"/>
       <c r="B7" s="33" t="s">
         <v>17</v>
@@ -10361,10 +10361,10 @@
         <v>68.108429918769971</v>
       </c>
       <c r="T7" s="22"/>
-      <c r="U7" s="45"/>
-      <c r="V7" s="47"/>
-    </row>
-    <row r="8" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U7" s="46"/>
+      <c r="V7" s="52"/>
+    </row>
+    <row r="8" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="55"/>
       <c r="B8" s="23" t="s">
         <v>34</v>
@@ -10429,10 +10429,10 @@
         <v>7.0685798695756613E-2</v>
       </c>
       <c r="T8" s="22"/>
-      <c r="U8" s="45"/>
-      <c r="V8" s="47"/>
-    </row>
-    <row r="9" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U8" s="46"/>
+      <c r="V8" s="52"/>
+    </row>
+    <row r="9" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="56" t="s">
         <v>25</v>
       </c>
@@ -10485,14 +10485,14 @@
         <v>1046.5999999999999</v>
       </c>
       <c r="T9" s="25"/>
-      <c r="U9" s="50">
+      <c r="U9" s="45">
         <v>-0.36423</v>
       </c>
-      <c r="V9" s="48">
+      <c r="V9" s="51">
         <v>0.41688399999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="54"/>
       <c r="B10" s="33" t="s">
         <v>17</v>
@@ -10543,10 +10543,10 @@
         <v>103.40901798199226</v>
       </c>
       <c r="T10" s="22"/>
-      <c r="U10" s="45"/>
-      <c r="V10" s="47"/>
-    </row>
-    <row r="11" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U10" s="46"/>
+      <c r="V10" s="52"/>
+    </row>
+    <row r="11" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="55"/>
       <c r="B11" s="35" t="s">
         <v>34</v>
@@ -10611,10 +10611,10 @@
         <v>9.8804718117707122E-2</v>
       </c>
       <c r="T11" s="24"/>
-      <c r="U11" s="46"/>
-      <c r="V11" s="49"/>
-    </row>
-    <row r="12" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U11" s="47"/>
+      <c r="V11" s="53"/>
+    </row>
+    <row r="12" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="56" t="s">
         <v>26</v>
       </c>
@@ -10667,14 +10667,14 @@
         <v>12.494548</v>
       </c>
       <c r="T12" s="22"/>
-      <c r="U12" s="45">
+      <c r="U12" s="46">
         <v>-0.28797299999999998</v>
       </c>
-      <c r="V12" s="47">
+      <c r="V12" s="52">
         <v>-0.17630399999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="54"/>
       <c r="B13" s="33" t="s">
         <v>17</v>
@@ -10725,10 +10725,10 @@
         <v>0.30815255961941967</v>
       </c>
       <c r="T13" s="22"/>
-      <c r="U13" s="45"/>
-      <c r="V13" s="47"/>
-    </row>
-    <row r="14" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U13" s="46"/>
+      <c r="V13" s="52"/>
+    </row>
+    <row r="14" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="55"/>
       <c r="B14" s="35" t="s">
         <v>34</v>
@@ -10793,10 +10793,10 @@
         <v>2.4662961766957852E-2</v>
       </c>
       <c r="T14" s="22"/>
-      <c r="U14" s="45"/>
-      <c r="V14" s="47"/>
-    </row>
-    <row r="15" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U14" s="46"/>
+      <c r="V14" s="52"/>
+    </row>
+    <row r="15" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="54" t="s">
         <v>27</v>
       </c>
@@ -10849,14 +10849,14 @@
         <v>255.87422000000001</v>
       </c>
       <c r="T15" s="25"/>
-      <c r="U15" s="50">
+      <c r="U15" s="45">
         <v>0.47454000000000002</v>
       </c>
-      <c r="V15" s="48">
+      <c r="V15" s="51">
         <v>0.22032199999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="54"/>
       <c r="B16" s="33" t="s">
         <v>17</v>
@@ -10907,10 +10907,10 @@
         <v>21.723481534965799</v>
       </c>
       <c r="T16" s="22"/>
-      <c r="U16" s="45"/>
-      <c r="V16" s="47"/>
-    </row>
-    <row r="17" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U16" s="46"/>
+      <c r="V16" s="52"/>
+    </row>
+    <row r="17" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="54"/>
       <c r="B17" s="33" t="s">
         <v>34</v>
@@ -10975,10 +10975,10 @@
         <v>8.4899063043419529E-2</v>
       </c>
       <c r="T17" s="24"/>
-      <c r="U17" s="46"/>
-      <c r="V17" s="49"/>
-    </row>
-    <row r="18" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U17" s="47"/>
+      <c r="V17" s="53"/>
+    </row>
+    <row r="18" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="56" t="s">
         <v>30</v>
       </c>
@@ -11031,14 +11031,14 @@
         <v>1194.846669</v>
       </c>
       <c r="T18" s="22"/>
-      <c r="U18" s="45">
+      <c r="U18" s="46">
         <v>0.21635299999999999</v>
       </c>
-      <c r="V18" s="47">
+      <c r="V18" s="52">
         <v>0.36393399999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="54"/>
       <c r="B19" s="33" t="s">
         <v>17</v>
@@ -11089,10 +11089,10 @@
         <v>261.5197644557673</v>
       </c>
       <c r="T19" s="22"/>
-      <c r="U19" s="45"/>
-      <c r="V19" s="47"/>
-    </row>
-    <row r="20" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U19" s="46"/>
+      <c r="V19" s="52"/>
+    </row>
+    <row r="20" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="55"/>
       <c r="B20" s="35" t="s">
         <v>34</v>
@@ -11157,10 +11157,10 @@
         <v>0.21887307488134888</v>
       </c>
       <c r="T20" s="22"/>
-      <c r="U20" s="45"/>
-      <c r="V20" s="47"/>
-    </row>
-    <row r="21" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U20" s="46"/>
+      <c r="V20" s="52"/>
+    </row>
+    <row r="21" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="54" t="s">
         <v>31</v>
       </c>
@@ -11213,14 +11213,14 @@
         <v>451.04004400000002</v>
       </c>
       <c r="T21" s="25"/>
-      <c r="U21" s="50">
+      <c r="U21" s="45">
         <v>0.400617</v>
       </c>
-      <c r="V21" s="48">
+      <c r="V21" s="51">
         <v>0.17532900000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="54"/>
       <c r="B22" s="33" t="s">
         <v>17</v>
@@ -11271,10 +11271,10 @@
         <v>27.061307581120317</v>
       </c>
       <c r="T22" s="22"/>
-      <c r="U22" s="45"/>
-      <c r="V22" s="47"/>
-    </row>
-    <row r="23" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U22" s="46"/>
+      <c r="V22" s="52"/>
+    </row>
+    <row r="23" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="54"/>
       <c r="B23" s="33" t="s">
         <v>34</v>
@@ -11339,10 +11339,10 @@
         <v>5.9997572147098131E-2</v>
       </c>
       <c r="T23" s="24"/>
-      <c r="U23" s="46"/>
-      <c r="V23" s="49"/>
-    </row>
-    <row r="24" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U23" s="47"/>
+      <c r="V23" s="53"/>
+    </row>
+    <row r="24" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="56" t="s">
         <v>28</v>
       </c>
@@ -11395,14 +11395,14 @@
         <v>122.930104</v>
       </c>
       <c r="T24" s="22"/>
-      <c r="U24" s="45">
+      <c r="U24" s="46">
         <v>-8.9659000000000003E-2</v>
       </c>
-      <c r="V24" s="47">
+      <c r="V24" s="52">
         <v>0.55726699999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="54"/>
       <c r="B25" s="33" t="s">
         <v>17</v>
@@ -11453,10 +11453,10 @@
         <v>16.131675052517018</v>
       </c>
       <c r="T25" s="22"/>
-      <c r="U25" s="45"/>
-      <c r="V25" s="47"/>
-    </row>
-    <row r="26" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U25" s="46"/>
+      <c r="V25" s="52"/>
+    </row>
+    <row r="26" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="55"/>
       <c r="B26" s="35" t="s">
         <v>34</v>
@@ -11521,11 +11521,11 @@
         <v>0.1312264004309068</v>
       </c>
       <c r="T26" s="22"/>
-      <c r="U26" s="45"/>
-      <c r="V26" s="47"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="51" t="s">
+      <c r="U26" s="46"/>
+      <c r="V26" s="52"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A27" s="48" t="s">
         <v>29</v>
       </c>
       <c r="B27" s="32" t="s">
@@ -11577,15 +11577,15 @@
         <v>0.96814999999999996</v>
       </c>
       <c r="T27" s="25"/>
-      <c r="U27" s="50">
+      <c r="U27" s="45">
         <v>0.12556899999999999</v>
       </c>
-      <c r="V27" s="48">
+      <c r="V27" s="51">
         <v>-0.25589000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="52"/>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A28" s="49"/>
       <c r="B28" s="33" t="s">
         <v>17</v>
       </c>
@@ -11635,11 +11635,11 @@
         <v>6.2449979983983982E-3</v>
       </c>
       <c r="T28" s="22"/>
-      <c r="U28" s="45"/>
-      <c r="V28" s="47"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="53"/>
+      <c r="U28" s="46"/>
+      <c r="V28" s="52"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A29" s="50"/>
       <c r="B29" s="35" t="s">
         <v>34</v>
       </c>
@@ -11703,14 +11703,14 @@
         <v>6.4504446608463547E-3</v>
       </c>
       <c r="T29" s="24"/>
-      <c r="U29" s="46"/>
-      <c r="V29" s="49"/>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" s="46" t="s">
+      <c r="U29" s="47"/>
+      <c r="V29" s="53"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A30" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="46"/>
+      <c r="B30" s="47"/>
       <c r="C30" s="37">
         <v>0.78</v>
       </c>
@@ -11760,7 +11760,7 @@
       <c r="U30" s="22"/>
       <c r="V30" s="22"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.4">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="E31" s="3"/>
@@ -11782,7 +11782,7 @@
       <c r="U31" s="3"/>
       <c r="V31" s="3"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.4">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="E32" s="3"/>
@@ -11804,7 +11804,7 @@
       <c r="U32" s="3"/>
       <c r="V32" s="3"/>
     </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="E33" s="3"/>
@@ -11826,7 +11826,7 @@
       <c r="U33" s="3"/>
       <c r="V33" s="3"/>
     </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="E34" s="3"/>
@@ -11848,7 +11848,7 @@
       <c r="U34" s="3"/>
       <c r="V34" s="3"/>
     </row>
-    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="E35" s="3"/>
@@ -11870,20 +11870,39 @@
       <c r="U35" s="3"/>
       <c r="V35" s="3"/>
     </row>
-    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="U3:U5"/>
+    <mergeCell ref="V3:V5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="U6:U8"/>
+    <mergeCell ref="V6:V8"/>
+    <mergeCell ref="V18:V20"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="U9:U11"/>
+    <mergeCell ref="V9:V11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="U12:U14"/>
+    <mergeCell ref="V12:V14"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="U27:U29"/>
     <mergeCell ref="V27:V29"/>
@@ -11900,39 +11919,10 @@
     <mergeCell ref="V15:V17"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="U18:U20"/>
-    <mergeCell ref="V18:V20"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="U9:U11"/>
-    <mergeCell ref="V9:V11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="U12:U14"/>
-    <mergeCell ref="V12:V14"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="U3:U5"/>
-    <mergeCell ref="V3:V5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="U6:U8"/>
-    <mergeCell ref="V6:V8"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="U1:V1"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="E3 I3">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3 T3">
-    <cfRule type="colorScale" priority="25">
+    <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11952,7 +11942,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6 I6">
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11972,6 +11962,142 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9 I9">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9 T9">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12 T12">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15 T15">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18 I18">
+    <cfRule type="colorScale" priority="43">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18 T18">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21 I21">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="45">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21 T21">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24 I24">
+    <cfRule type="colorScale" priority="47">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24 T24">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3 E3">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6 E6">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9 E9">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -11981,7 +12107,35 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15 I15">
+  <conditionalFormatting sqref="I9">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12 E12">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15 E15">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -12007,7 +12161,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E18 I18">
+  <conditionalFormatting sqref="I18 E18">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -12017,122 +12171,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E24 I24">
+  <conditionalFormatting sqref="I24 E24">
     <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E30 I30">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3 E3">
-    <cfRule type="colorScale" priority="33">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I6 E6">
-    <cfRule type="colorScale" priority="35">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I9 E9">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I9">
-    <cfRule type="colorScale" priority="38">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12 E12">
-    <cfRule type="colorScale" priority="39">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18 E18">
-    <cfRule type="colorScale" priority="43">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I21 E21">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="45">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="46">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I24 E24">
-    <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -12161,6 +12201,16 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="I27">
     <cfRule type="colorScale" priority="50">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I30 E30">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -12279,58 +12329,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T9 E9">
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T12 E12">
-    <cfRule type="colorScale" priority="27">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T15 E15">
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T18 E18">
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T21 E21">
-    <cfRule type="colorScale" priority="30">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T24 E24">
-    <cfRule type="colorScale" priority="31">
+  <conditionalFormatting sqref="T3 E3">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -12383,24 +12383,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CCB7AF-21A6-41ED-886C-DD886AE34E4A}">
   <dimension ref="A1:AX40"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AZ10" sqref="AZ10"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AC9" sqref="AC9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10" style="3" customWidth="1"/>
-    <col min="2" max="6" width="4.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" style="13" customWidth="1"/>
-    <col min="8" max="27" width="4.42578125" style="2" customWidth="1"/>
-    <col min="28" max="28" width="4.140625" style="3" customWidth="1"/>
+    <col min="2" max="6" width="4.25" style="3" customWidth="1"/>
+    <col min="7" max="7" width="6.25" style="13" customWidth="1"/>
+    <col min="8" max="27" width="4.375" style="2" customWidth="1"/>
+    <col min="28" max="28" width="4.125" style="3" customWidth="1"/>
     <col min="29" max="29" width="10" style="3" customWidth="1"/>
-    <col min="30" max="32" width="4.28515625" style="3" customWidth="1"/>
-    <col min="33" max="33" width="6.140625" style="3" customWidth="1"/>
-    <col min="34" max="43" width="4.42578125" style="4" customWidth="1"/>
+    <col min="30" max="32" width="4.25" style="3" customWidth="1"/>
+    <col min="33" max="33" width="6.125" style="3" customWidth="1"/>
+    <col min="34" max="43" width="4.375" style="4" customWidth="1"/>
     <col min="45" max="45" width="10" style="3" customWidth="1"/>
-    <col min="46" max="49" width="4.28515625" style="3" customWidth="1"/>
-    <col min="50" max="50" width="6.140625" style="3" customWidth="1"/>
+    <col min="46" max="49" width="4.25" style="3" customWidth="1"/>
+    <col min="50" max="50" width="6.125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12605,7 +12605,7 @@
       <c r="AW2" s="5"/>
       <c r="AX2" s="5"/>
     </row>
-    <row r="3" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -12738,7 +12738,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="4" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.4">
       <c r="C4" s="3">
         <v>2</v>
       </c>
@@ -12793,7 +12793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.4">
       <c r="G5" s="12"/>
       <c r="H5" s="16">
         <f>(COUNTIF(H3:H4,"○"))/2</f>
@@ -12888,7 +12888,7 @@
       <c r="AQ5" s="1"/>
       <c r="AX5" s="12"/>
     </row>
-    <row r="6" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.4">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -13012,7 +13012,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="7" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.4">
       <c r="C7" s="3">
         <v>2</v>
       </c>
@@ -13127,7 +13127,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.4">
       <c r="C8" s="3">
         <v>3</v>
       </c>
@@ -13242,34 +13242,74 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.4">
       <c r="C9" s="3">
         <v>4</v>
       </c>
       <c r="G9" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="9"/>
-      <c r="X9" s="10"/>
-      <c r="Y9" s="10"/>
-      <c r="Z9" s="9"/>
-      <c r="AA9" s="10"/>
+        <v>0.75</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="P9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="X9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA9" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AE9" s="3">
         <v>4</v>
       </c>
@@ -13294,37 +13334,77 @@
       <c r="AW9"/>
       <c r="AX9" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:50" x14ac:dyDescent="0.4">
       <c r="C10" s="3">
         <v>5</v>
       </c>
       <c r="G10" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="10"/>
-      <c r="X10" s="10"/>
-      <c r="Y10" s="10"/>
-      <c r="Z10" s="10"/>
-      <c r="AA10" s="10"/>
+        <v>0.65</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="P10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="R10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="S10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="V10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="X10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA10" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="AE10" s="3">
         <v>5</v>
       </c>
@@ -13349,37 +13429,77 @@
       <c r="AW10"/>
       <c r="AX10" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:50" x14ac:dyDescent="0.4">
       <c r="C11" s="3">
         <v>6</v>
       </c>
       <c r="G11" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="10"/>
-      <c r="V11" s="10"/>
-      <c r="W11" s="10"/>
-      <c r="X11" s="10"/>
-      <c r="Y11" s="10"/>
-      <c r="Z11" s="10"/>
-      <c r="AA11" s="10"/>
+        <v>0.95</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="P11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="S11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="X11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA11" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AE11" s="3">
         <v>6</v>
       </c>
@@ -13404,37 +13524,77 @@
       <c r="AW11"/>
       <c r="AX11" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+        <v>0.47499999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:50" x14ac:dyDescent="0.4">
       <c r="C12" s="3">
         <v>7</v>
       </c>
       <c r="G12" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="10"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="10"/>
-      <c r="X12" s="10"/>
-      <c r="Y12" s="9"/>
-      <c r="Z12" s="10"/>
-      <c r="AA12" s="10"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="P12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="R12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="S12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="T12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="V12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="X12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA12" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="AE12" s="3">
         <v>7</v>
       </c>
@@ -13459,10 +13619,10 @@
       <c r="AW12"/>
       <c r="AX12" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+        <v>0.27500000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:50" x14ac:dyDescent="0.4">
       <c r="C13" s="3">
         <v>8</v>
       </c>
@@ -13577,7 +13737,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.4">
       <c r="C14" s="3">
         <v>9</v>
       </c>
@@ -13692,7 +13852,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.4">
       <c r="C15" s="3">
         <v>10</v>
       </c>
@@ -13747,87 +13907,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.4">
       <c r="G16" s="12"/>
       <c r="H16" s="16">
         <f>(COUNTIF(H6:H15,"○"))/10</f>
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="I16" s="16">
         <f t="shared" ref="I16:AA16" si="4">(COUNTIF(I6:I15,"○"))/10</f>
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="J16" s="16">
         <f t="shared" si="4"/>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="K16" s="16">
         <f t="shared" si="4"/>
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="L16" s="16">
         <f t="shared" si="4"/>
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="M16" s="16">
         <f t="shared" si="4"/>
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="N16" s="16">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="O16" s="16">
         <f t="shared" si="4"/>
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="P16" s="16">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="Q16" s="16">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="R16" s="16">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="S16" s="16">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="T16" s="16">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="U16" s="16">
         <f t="shared" si="4"/>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="V16" s="16">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="W16" s="16">
         <f t="shared" si="4"/>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="X16" s="16">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="Y16" s="16">
         <f t="shared" si="4"/>
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="Z16" s="16">
         <f t="shared" si="4"/>
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="AA16" s="16">
         <f t="shared" si="4"/>
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AG16" s="12"/>
       <c r="AH16" s="10"/>
@@ -13842,7 +14002,7 @@
       <c r="AQ16" s="1"/>
       <c r="AX16" s="12"/>
     </row>
-    <row r="17" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:50" x14ac:dyDescent="0.4">
       <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
@@ -13966,7 +14126,7 @@
         <v>0.92500000000000004</v>
       </c>
     </row>
-    <row r="18" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C18" s="3">
         <v>2</v>
       </c>
@@ -14081,7 +14241,7 @@
         <v>0.77500000000000002</v>
       </c>
     </row>
-    <row r="19" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C19" s="3">
         <v>3</v>
       </c>
@@ -14196,7 +14356,7 @@
         <v>0.85000000000000009</v>
       </c>
     </row>
-    <row r="20" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C20" s="3">
         <v>4</v>
       </c>
@@ -14251,7 +14411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C21" s="3">
         <v>5</v>
       </c>
@@ -14366,7 +14526,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="22" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C22" s="3">
         <v>6</v>
       </c>
@@ -14481,7 +14641,7 @@
         <v>0.85000000000000009</v>
       </c>
     </row>
-    <row r="23" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C23" s="3">
         <v>7</v>
       </c>
@@ -14536,7 +14696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C24" s="3">
         <v>8</v>
       </c>
@@ -14651,7 +14811,7 @@
         <v>0.92500000000000004</v>
       </c>
     </row>
-    <row r="25" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C25" s="3">
         <v>9</v>
       </c>
@@ -14766,7 +14926,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="26" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C26" s="3">
         <v>10</v>
       </c>
@@ -14881,7 +15041,7 @@
         <v>0.67500000000000004</v>
       </c>
     </row>
-    <row r="27" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C27" s="3">
         <v>11</v>
       </c>
@@ -14996,7 +15156,7 @@
         <v>0.72499999999999998</v>
       </c>
     </row>
-    <row r="28" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C28" s="3">
         <v>12</v>
       </c>
@@ -15111,34 +15271,74 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="29" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C29" s="3">
         <v>13</v>
       </c>
       <c r="G29" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
-      <c r="U29" s="9"/>
-      <c r="V29" s="9"/>
-      <c r="W29" s="10"/>
-      <c r="X29" s="9"/>
-      <c r="Y29" s="9"/>
-      <c r="Z29" s="10"/>
-      <c r="AA29" s="9"/>
+        <v>0.6</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="X29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA29" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AE29" s="3">
         <v>13</v>
       </c>
@@ -15163,10 +15363,10 @@
       <c r="AW29"/>
       <c r="AX29" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:50" x14ac:dyDescent="0.4">
       <c r="C30" s="3">
         <v>14</v>
       </c>
@@ -15281,15 +15481,15 @@
         <v>0.85000000000000009</v>
       </c>
     </row>
-    <row r="31" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:50" x14ac:dyDescent="0.4">
       <c r="G31" s="5"/>
       <c r="H31" s="15">
         <f>(COUNTIF(H17:H30,"○"))/14</f>
-        <v>0.5714285714285714</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="I31" s="15">
         <f t="shared" ref="I31:AA31" si="6">(COUNTIF(I17:I30,"○"))/14</f>
-        <v>0.7142857142857143</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="J31" s="15">
         <f t="shared" si="6"/>
@@ -15305,11 +15505,11 @@
       </c>
       <c r="M31" s="15">
         <f t="shared" si="6"/>
-        <v>0.7857142857142857</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="N31" s="15">
         <f t="shared" si="6"/>
-        <v>0.6428571428571429</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="O31" s="15">
         <f t="shared" si="6"/>
@@ -15321,7 +15521,7 @@
       </c>
       <c r="Q31" s="15">
         <f t="shared" si="6"/>
-        <v>0.7142857142857143</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="R31" s="15">
         <f t="shared" si="6"/>
@@ -15329,27 +15529,27 @@
       </c>
       <c r="S31" s="15">
         <f>(COUNTIF(S17:S30,"○"))/14</f>
-        <v>0.5</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="T31" s="15">
         <f t="shared" si="6"/>
-        <v>0.5714285714285714</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="U31" s="15">
         <f t="shared" si="6"/>
-        <v>0.6428571428571429</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="V31" s="15">
         <f t="shared" si="6"/>
-        <v>0.7142857142857143</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="W31" s="15">
         <f t="shared" si="6"/>
-        <v>0.7142857142857143</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="X31" s="15">
         <f t="shared" si="6"/>
-        <v>0.7857142857142857</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="Y31" s="15">
         <f t="shared" si="6"/>
@@ -15361,7 +15561,7 @@
       </c>
       <c r="AA31" s="15">
         <f t="shared" si="6"/>
-        <v>0.5714285714285714</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="AD31" s="3" t="s">
         <v>5</v>
@@ -15416,7 +15616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:50" x14ac:dyDescent="0.4">
       <c r="G32" s="12"/>
       <c r="AE32" s="3">
         <v>2</v>
@@ -15465,7 +15665,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="33" spans="30:50" x14ac:dyDescent="0.25">
+    <row r="33" spans="30:50" x14ac:dyDescent="0.4">
       <c r="AD33" s="3" t="s">
         <v>7</v>
       </c>
@@ -15499,7 +15699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="30:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="34" spans="30:50" x14ac:dyDescent="0.4">
       <c r="AE34" s="3">
         <v>2</v>
       </c>
@@ -15527,7 +15727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="30:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="30:50" x14ac:dyDescent="0.4">
       <c r="AE35" s="3">
         <v>3</v>
       </c>
@@ -15555,7 +15755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="30:50" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="30:50" x14ac:dyDescent="0.4">
       <c r="AE36" s="3">
         <v>4</v>
       </c>
@@ -15603,7 +15803,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="37" spans="30:50" x14ac:dyDescent="0.25">
+    <row r="37" spans="30:50" x14ac:dyDescent="0.4">
       <c r="AD37" s="3" t="s">
         <v>6</v>
       </c>
@@ -15637,7 +15837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="30:50" x14ac:dyDescent="0.25">
+    <row r="38" spans="30:50" x14ac:dyDescent="0.4">
       <c r="AH38" s="15">
         <f>(COUNTIF(AH3:AH37,"○")/32)</f>
         <v>0.625</v>
@@ -15681,12 +15881,12 @@
       <c r="AV38"/>
       <c r="AW38"/>
     </row>
-    <row r="39" spans="30:50" x14ac:dyDescent="0.25">
+    <row r="39" spans="30:50" x14ac:dyDescent="0.4">
       <c r="AV39"/>
       <c r="AW39"/>
       <c r="AX39" s="12"/>
     </row>
-    <row r="40" spans="30:50" x14ac:dyDescent="0.25">
+    <row r="40" spans="30:50" x14ac:dyDescent="0.4">
       <c r="AG40" s="12"/>
     </row>
   </sheetData>

</xml_diff>